<commit_message>
Regenerated PDF with bookmarks - editorial changes to registry
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="108" documentId="11_2D2EDAC1EA08F252476343E40134398ECC69A957" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{76049B2C-6D45-4276-9C04-6BE6375F585D}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="11_2D2EDAC1EA08F252476343E40134398ECC69A957" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{69D36759-5961-408D-8938-75440E22905A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12503" yWindow="-3533" windowWidth="24495" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATION" sheetId="6" r:id="rId1"/>
@@ -773,12 +773,6 @@
     <t>Information being transmitted</t>
   </si>
   <si>
-    <t>Interconnection: Ports &amp; Circuts (Port)</t>
-  </si>
-  <si>
-    <t>Interconnection: Ports &amp; Circuts (Circuit)</t>
-  </si>
-  <si>
     <t>Under Ports and Circuits. Use this for circuit numbers.</t>
   </si>
   <si>
@@ -825,9 +819,6 @@
   </si>
   <si>
     <t>Citation Document: Version Number</t>
-  </si>
-  <si>
-    <t>Citation Document: Publicaiton Date</t>
   </si>
   <si>
     <t>Citation Document: Type</t>
@@ -1536,9 +1527,6 @@
     <t>The job/position title of an Individual.</t>
   </si>
   <si>
-    <t>The FedRAMP authorizatioin type (JAB, Agency, or LI-SaaS) (See the Accepted Values tab)</t>
-  </si>
-  <si>
     <t>The current number of external users.</t>
   </si>
   <si>
@@ -2006,9 +1994,6 @@
     <t>Included in web server scans</t>
   </si>
   <si>
-    <t>Required for all scanable components. May list more than one to indicate multiple scan types.</t>
-  </si>
-  <si>
     <t>/*/metadata/prop[@name="marking"][@ns="https://fedramp.gov/ns/oscal"]</t>
   </si>
   <si>
@@ -2114,9 +2099,6 @@
     <t>/*/back-matter/resource[@id="att-____"]/prop[@name="version"][@ns="https://fedramp.gov/ns/oscal"]</t>
   </si>
   <si>
-    <t>Component's Authoirzation Date</t>
-  </si>
-  <si>
     <t>Required for hardware and software components. If open source (no vendor), enter "Open Source"</t>
   </si>
   <si>
@@ -2181,9 +2163,6 @@
   </si>
   <si>
     <t>ID-Ref</t>
-  </si>
-  <si>
-    <t>Links by component-id to a coponent that represents the FIPS 140-2 validation certificate.</t>
   </si>
   <si>
     <t>ID-ref</t>
@@ -2366,6 +2345,27 @@
   </si>
   <si>
     <t>Indicates citation is related to Personally Identifiable Information (PII).</t>
+  </si>
+  <si>
+    <t>The FedRAMP authorization type (JAB, Agency, or LI-SaaS) (See the Accepted Values tab)</t>
+  </si>
+  <si>
+    <t>Required for all scannable components. May list more than one to indicate multiple scan types.</t>
+  </si>
+  <si>
+    <t>Links by component-id to a component that represents the FIPS 140-2 validation certificate.</t>
+  </si>
+  <si>
+    <t>Interconnection: Ports &amp; Circuits (Port)</t>
+  </si>
+  <si>
+    <t>Interconnection: Ports &amp; Circuits (Circuit)</t>
+  </si>
+  <si>
+    <t>Component's Authorization Date</t>
+  </si>
+  <si>
+    <t>Citation Document: Publication Date</t>
   </si>
 </sst>
 </file>
@@ -2944,11 +2944,11 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3291,7 +3291,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57CEA3A-8DD1-44C9-85C0-D74433EA434F}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3307,12 +3307,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="71" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="B1" s="72"/>
       <c r="C1" s="66"/>
       <c r="H1" s="57" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3321,13 +3321,13 @@
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="60" t="s">
-        <v>491</v>
+        <v>484</v>
       </c>
       <c r="B3" s="59"/>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="B4" s="69"/>
       <c r="C4" s="61"/>
@@ -3335,14 +3335,14 @@
     </row>
     <row r="5" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="70" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="B5" s="70"/>
       <c r="C5" s="61"/>
     </row>
     <row r="6" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B6" s="63"/>
       <c r="C6" s="62"/>
@@ -3351,7 +3351,7 @@
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="70" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="B7" s="68"/>
       <c r="C7" s="64"/>
@@ -3360,13 +3360,13 @@
     </row>
     <row r="8" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="B8" s="68"/>
     </row>
     <row r="9" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="60" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="B9" s="63"/>
       <c r="C9" s="62"/>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="70" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="B10" s="68"/>
       <c r="C10" s="64"/>
@@ -3384,25 +3384,25 @@
     </row>
     <row r="11" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="67" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="B11" s="68"/>
     </row>
     <row r="12" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="70" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="B12" s="70"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="68" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B13" s="68"/>
     </row>
     <row r="14" spans="1:8" ht="43.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="67" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="B14" s="68"/>
     </row>
@@ -3435,7 +3435,7 @@
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight"/>
@@ -3455,25 +3455,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D2" s="73" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E2" s="73"/>
       <c r="F2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G2" s="74" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="H2" s="74" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3493,7 +3493,7 @@
         <v>25</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="G3" s="74"/>
       <c r="H3" s="74"/>
@@ -3503,7 +3503,7 @@
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>31</v>
@@ -3516,14 +3516,14 @@
         <v>26</v>
       </c>
       <c r="F4" s="56" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>26</v>
@@ -3531,7 +3531,7 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>31</v>
@@ -3543,13 +3543,13 @@
         <v>26</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>26</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>31</v>
@@ -3572,13 +3572,13 @@
         <v>26</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -3595,13 +3595,13 @@
         <v>26</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>305</v>
+        <v>503</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -3618,13 +3618,13 @@
         <v>26</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -3641,13 +3641,13 @@
         <v>26</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -3664,13 +3664,13 @@
         <v>26</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -3687,13 +3687,13 @@
         <v>26</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -3701,7 +3701,7 @@
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>31</v>
@@ -3713,18 +3713,18 @@
         <v>26</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>31</v>
@@ -3736,18 +3736,18 @@
         <v>26</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>31</v>
@@ -3759,18 +3759,18 @@
         <v>26</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>31</v>
@@ -3782,18 +3782,18 @@
         <v>26</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>31</v>
@@ -3805,13 +3805,13 @@
         <v>26</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3831,16 +3831,16 @@
         <v>26</v>
       </c>
       <c r="F20" s="56" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3854,16 +3854,16 @@
         <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="56" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3883,10 +3883,10 @@
         <v>26</v>
       </c>
       <c r="F24" s="56" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3897,16 +3897,16 @@
         <v>31</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F25" s="56" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3926,10 +3926,10 @@
         <v>26</v>
       </c>
       <c r="F27" s="56" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3940,16 +3940,16 @@
         <v>31</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F28" s="56" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3960,16 +3960,16 @@
         <v>31</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="56" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3980,19 +3980,19 @@
         <v>31</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F30" s="56" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4003,16 +4003,16 @@
         <v>31</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="56" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>104</v>
@@ -4020,7 +4020,7 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>506</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>31</v>
@@ -4032,18 +4032,18 @@
         <v>26</v>
       </c>
       <c r="F32" s="56" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>106</v>
+        <v>507</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>31</v>
@@ -4055,13 +4055,13 @@
         <v>26</v>
       </c>
       <c r="F33" s="56" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4072,16 +4072,16 @@
         <v>32</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F34" s="56" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4089,7 +4089,7 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A36" s="54" t="s">
-        <v>463</v>
+        <v>508</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>31</v>
@@ -4101,18 +4101,18 @@
         <v>26</v>
       </c>
       <c r="F36" s="56" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A37" s="54" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>31</v>
@@ -4124,18 +4124,18 @@
         <v>26</v>
       </c>
       <c r="F37" s="56" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A38" s="54" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>31</v>
@@ -4147,41 +4147,41 @@
         <v>26</v>
       </c>
       <c r="F38" s="56" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A39" s="54" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F39" s="56" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>427</v>
+        <v>504</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A40" s="54" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>31</v>
@@ -4193,13 +4193,13 @@
         <v>26</v>
       </c>
       <c r="F40" s="56" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>486</v>
+        <v>505</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4208,7 +4208,7 @@
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A42" s="54" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>31</v>
@@ -4220,41 +4220,41 @@
         <v>26</v>
       </c>
       <c r="F42" s="56" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A43" s="54" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F43" s="56" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>427</v>
+        <v>504</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A44" s="54" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>31</v>
@@ -4266,13 +4266,13 @@
         <v>26</v>
       </c>
       <c r="F44" s="56" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>486</v>
+        <v>505</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4280,7 +4280,7 @@
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>32</v>
@@ -4292,18 +4292,18 @@
         <v>26</v>
       </c>
       <c r="F46" s="56" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>32</v>
@@ -4315,18 +4315,18 @@
         <v>26</v>
       </c>
       <c r="F47" s="56" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>31</v>
@@ -4338,18 +4338,18 @@
         <v>26</v>
       </c>
       <c r="F48" s="56" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>31</v>
@@ -4361,13 +4361,13 @@
         <v>26</v>
       </c>
       <c r="F49" s="56" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>487</v>
+        <v>480</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4375,7 +4375,7 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>119</v>
+        <v>509</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>31</v>
@@ -4387,21 +4387,21 @@
         <v>26</v>
       </c>
       <c r="F51" s="56" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>31</v>
@@ -4413,21 +4413,21 @@
         <v>26</v>
       </c>
       <c r="F52" s="56" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>31</v>
@@ -4439,21 +4439,21 @@
         <v>26</v>
       </c>
       <c r="F53" s="56" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>31</v>
@@ -4465,16 +4465,16 @@
         <v>26</v>
       </c>
       <c r="F54" s="56" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4482,7 +4482,7 @@
     </row>
     <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>31</v>
@@ -4494,21 +4494,21 @@
         <v>26</v>
       </c>
       <c r="F56" s="56" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>26</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>31</v>
@@ -4520,10 +4520,10 @@
         <v>26</v>
       </c>
       <c r="F57" s="56" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>26</v>
@@ -4534,7 +4534,7 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>31</v>
@@ -4546,10 +4546,10 @@
         <v>26</v>
       </c>
       <c r="F58" s="56" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>26</v>
@@ -4560,7 +4560,7 @@
     </row>
     <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>31</v>
@@ -4572,10 +4572,10 @@
         <v>26</v>
       </c>
       <c r="F59" s="56" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>26</v>
@@ -4603,9 +4603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H71" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4619,7 +4619,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4630,11 +4630,11 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B2" s="73"/>
       <c r="C2" s="28" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="D2" s="73" t="s">
         <v>39</v>
@@ -4654,7 +4654,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>0</v>
@@ -4690,7 +4690,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -4705,7 +4705,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O5" s="1"/>
     </row>
@@ -4714,7 +4714,7 @@
         <v>26</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -4729,7 +4729,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="O6" s="1"/>
     </row>
@@ -4738,7 +4738,7 @@
         <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
@@ -4753,7 +4753,7 @@
         <v>7</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="O7" s="1"/>
     </row>
@@ -4762,7 +4762,7 @@
         <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
@@ -4777,7 +4777,7 @@
         <v>88</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="O8" s="1"/>
     </row>
@@ -4786,7 +4786,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
@@ -4801,7 +4801,7 @@
         <v>8</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="O9" s="1"/>
     </row>
@@ -4810,7 +4810,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
@@ -4825,7 +4825,7 @@
         <v>8</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="O10" s="1"/>
     </row>
@@ -4834,7 +4834,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>5</v>
@@ -4849,7 +4849,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="O11" s="1"/>
     </row>
@@ -4858,7 +4858,7 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>5</v>
@@ -4873,7 +4873,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="O12" s="1"/>
     </row>
@@ -4882,7 +4882,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>7</v>
@@ -4897,7 +4897,7 @@
         <v>7</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="O13" s="1"/>
     </row>
@@ -4906,7 +4906,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>5</v>
@@ -4921,7 +4921,7 @@
         <v>5</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="O14" s="1"/>
     </row>
@@ -4930,7 +4930,7 @@
         <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>5</v>
@@ -4945,7 +4945,7 @@
         <v>8</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O15" s="1"/>
     </row>
@@ -4954,7 +4954,7 @@
         <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
@@ -4969,7 +4969,7 @@
         <v>88</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="I16" s="5"/>
       <c r="O16" s="1"/>
@@ -4979,7 +4979,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
@@ -4994,7 +4994,7 @@
         <v>88</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="I17" s="5"/>
       <c r="O17" s="1"/>
@@ -5004,7 +5004,7 @@
         <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
@@ -5019,7 +5019,7 @@
         <v>88</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -5028,7 +5028,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>7</v>
@@ -5043,7 +5043,7 @@
         <v>88</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="I19" s="5"/>
     </row>
@@ -5052,7 +5052,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
@@ -5067,7 +5067,7 @@
         <v>88</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -5076,7 +5076,7 @@
         <v>26</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>7</v>
@@ -5091,7 +5091,7 @@
         <v>88</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I21" s="5"/>
     </row>
@@ -5100,7 +5100,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>7</v>
@@ -5115,7 +5115,7 @@
         <v>88</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="I22" s="5"/>
     </row>
@@ -5124,7 +5124,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
@@ -5139,7 +5139,7 @@
         <v>88</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -5148,7 +5148,7 @@
         <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>7</v>
@@ -5163,7 +5163,7 @@
         <v>88</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -5172,7 +5172,7 @@
         <v>26</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>7</v>
@@ -5187,7 +5187,7 @@
         <v>8</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="I25" s="5"/>
     </row>
@@ -5196,7 +5196,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>7</v>
@@ -5211,7 +5211,7 @@
         <v>8</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="I26" s="5"/>
     </row>
@@ -5220,7 +5220,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>7</v>
@@ -5235,7 +5235,7 @@
         <v>8</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="I27" s="5"/>
     </row>
@@ -5244,7 +5244,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>7</v>
@@ -5259,7 +5259,7 @@
         <v>8</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="I28" s="5"/>
     </row>
@@ -5268,7 +5268,7 @@
         <v>26</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>7</v>
@@ -5283,7 +5283,7 @@
         <v>88</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -5291,7 +5291,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>8</v>
@@ -5306,7 +5306,7 @@
         <v>8</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.75" x14ac:dyDescent="0.3">
@@ -5314,7 +5314,7 @@
         <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>5</v>
@@ -5350,7 +5350,7 @@
         <v>26</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>5</v>
@@ -5373,7 +5373,7 @@
         <v>26</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>5</v>
@@ -5419,7 +5419,7 @@
         <v>26</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>12</v>
@@ -5442,7 +5442,7 @@
         <v>26</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>5</v>
@@ -5502,10 +5502,10 @@
       </c>
       <c r="B42" s="42"/>
       <c r="C42" s="43" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D42" s="44" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E42" s="44" t="s">
         <v>8</v>
@@ -5517,7 +5517,7 @@
         <v>8</v>
       </c>
       <c r="H42" s="45" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="I42" s="45"/>
     </row>
@@ -5575,7 +5575,7 @@
         <v>26</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>6</v>
@@ -5598,7 +5598,7 @@
         <v>26</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>6</v>
@@ -5621,7 +5621,7 @@
         <v>26</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>6</v>
@@ -5641,7 +5641,7 @@
     </row>
     <row r="52" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="75" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B52" s="75"/>
       <c r="C52" s="75"/>
@@ -5657,7 +5657,7 @@
         <v>26</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>5</v>
@@ -5672,7 +5672,7 @@
         <v>88</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -5680,7 +5680,7 @@
         <v>26</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>12</v>
@@ -5695,7 +5695,7 @@
         <v>88</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -5703,10 +5703,10 @@
         <v>26</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>88</v>
@@ -5718,7 +5718,7 @@
         <v>88</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -5726,10 +5726,10 @@
         <v>26</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>88</v>
@@ -5741,7 +5741,7 @@
         <v>88</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -5762,7 +5762,7 @@
         <v>26</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>5</v>
@@ -5785,7 +5785,7 @@
         <v>26</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>5</v>
@@ -5800,7 +5800,7 @@
         <v>12</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -5808,7 +5808,7 @@
         <v>26</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>5</v>
@@ -5823,7 +5823,7 @@
         <v>12</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -5859,7 +5859,7 @@
         <v>12</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
@@ -5882,7 +5882,7 @@
         <v>12</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
@@ -5890,7 +5890,7 @@
         <v>26</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>12</v>
@@ -5905,7 +5905,7 @@
         <v>12</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
@@ -5913,7 +5913,7 @@
         <v>26</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>8</v>
@@ -5928,7 +5928,7 @@
         <v>12</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="2:8" ht="15.75" x14ac:dyDescent="0.3">
@@ -6250,7 +6250,7 @@
         <v>12</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
@@ -6273,7 +6273,7 @@
         <v>8</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="2:8" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.3"/>
@@ -6316,7 +6316,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="65" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -6328,11 +6328,11 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B2" s="73"/>
       <c r="C2" s="28" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F2" s="73" t="s">
         <v>3</v>
@@ -6349,7 +6349,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>9</v>
@@ -6368,12 +6368,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="76" t="s">
-        <v>405</v>
-      </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="A4" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="B4" s="77"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
       <c r="F4" s="30" t="s">
         <v>89</v>
       </c>
@@ -6388,12 +6388,12 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="76" t="s">
-        <v>404</v>
-      </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
+      <c r="A5" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
       <c r="F5" s="30" t="s">
         <v>89</v>
       </c>
@@ -6412,10 +6412,10 @@
         <v>26</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D6" s="50" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="52"/>
@@ -6427,10 +6427,10 @@
         <v>26</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="40"/>
@@ -6448,12 +6448,12 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="76" t="s">
-        <v>411</v>
-      </c>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
+      <c r="A9" s="77" t="s">
+        <v>407</v>
+      </c>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
       <c r="F9" s="30" t="s">
         <v>89</v>
       </c>
@@ -6468,12 +6468,12 @@
       </c>
     </row>
     <row r="10" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="76" t="s">
-        <v>410</v>
-      </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
+      <c r="A10" s="77" t="s">
+        <v>406</v>
+      </c>
+      <c r="B10" s="77"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
       <c r="F10" s="30" t="s">
         <v>89</v>
       </c>
@@ -6492,10 +6492,10 @@
         <v>26</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F11" s="51"/>
       <c r="G11" s="52"/>
@@ -6507,10 +6507,10 @@
         <v>26</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="40"/>
@@ -6522,10 +6522,10 @@
         <v>26</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="40"/>
@@ -6543,12 +6543,12 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="76" t="s">
-        <v>346</v>
-      </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
+      <c r="A15" s="77" t="s">
+        <v>342</v>
+      </c>
+      <c r="B15" s="77"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
       <c r="F15" s="30" t="s">
         <v>89</v>
       </c>
@@ -6582,10 +6582,10 @@
         <v>26</v>
       </c>
       <c r="C17" s="49" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="F17" s="51"/>
       <c r="G17" s="52"/>
@@ -6603,12 +6603,12 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="76" t="s">
-        <v>347</v>
-      </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
+      <c r="A19" s="77" t="s">
+        <v>343</v>
+      </c>
+      <c r="B19" s="77"/>
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
       <c r="F19" s="30" t="s">
         <v>89</v>
       </c>
@@ -6623,12 +6623,12 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="76" t="s">
-        <v>348</v>
-      </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
+      <c r="A20" s="77" t="s">
+        <v>344</v>
+      </c>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="77"/>
       <c r="F20" s="30" t="s">
         <v>89</v>
       </c>
@@ -6643,12 +6643,12 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="76" t="s">
-        <v>349</v>
-      </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
+      <c r="A21" s="77" t="s">
+        <v>345</v>
+      </c>
+      <c r="B21" s="77"/>
+      <c r="C21" s="77"/>
+      <c r="D21" s="77"/>
       <c r="F21" s="30" t="s">
         <v>89</v>
       </c>
@@ -6663,12 +6663,12 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="76" t="s">
-        <v>350</v>
-      </c>
-      <c r="B22" s="76"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
+      <c r="A22" s="77" t="s">
+        <v>346</v>
+      </c>
+      <c r="B22" s="77"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
       <c r="F22" s="30" t="s">
         <v>89</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F23" s="22"/>
       <c r="G23" s="15"/>
@@ -6705,7 +6705,7 @@
         <v>2</v>
       </c>
       <c r="D24" s="16" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F24" s="22"/>
       <c r="G24" s="15"/>
@@ -6720,7 +6720,7 @@
         <v>3</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F25" s="22"/>
       <c r="G25" s="15"/>
@@ -6738,12 +6738,12 @@
       <c r="I26" s="14"/>
     </row>
     <row r="27" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="76" t="s">
-        <v>351</v>
-      </c>
-      <c r="B27" s="76"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
+      <c r="A27" s="77" t="s">
+        <v>347</v>
+      </c>
+      <c r="B27" s="77"/>
+      <c r="C27" s="77"/>
+      <c r="D27" s="77"/>
       <c r="F27" s="30" t="s">
         <v>89</v>
       </c>
@@ -6766,7 +6766,7 @@
         <v>10</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F28" s="22"/>
       <c r="G28" s="22"/>
@@ -6782,7 +6782,7 @@
         <v>19</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F29" s="22"/>
       <c r="G29" s="22"/>
@@ -6798,7 +6798,7 @@
         <v>20</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
@@ -6816,12 +6816,12 @@
       <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="76" t="s">
-        <v>401</v>
-      </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="76"/>
+      <c r="A32" s="77" t="s">
+        <v>397</v>
+      </c>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
       <c r="F32" s="30" t="s">
         <v>89</v>
       </c>
@@ -6843,7 +6843,7 @@
         <v>21</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F33" s="22"/>
       <c r="G33" s="15"/>
@@ -6858,7 +6858,7 @@
         <v>22</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F34" s="22"/>
       <c r="G34" s="15"/>
@@ -6873,7 +6873,7 @@
         <v>23</v>
       </c>
       <c r="D35" s="16" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F35" s="22"/>
       <c r="G35" s="15"/>
@@ -6888,7 +6888,7 @@
         <v>24</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F36" s="22"/>
       <c r="G36" s="15"/>
@@ -6906,12 +6906,12 @@
       <c r="I37" s="14"/>
     </row>
     <row r="38" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="76" t="s">
-        <v>352</v>
-      </c>
-      <c r="B38" s="76"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="76"/>
+      <c r="A38" s="77" t="s">
+        <v>348</v>
+      </c>
+      <c r="B38" s="77"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
       <c r="F38" s="30" t="s">
         <v>89</v>
       </c>
@@ -6930,10 +6930,10 @@
         <v>26</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F39" s="22"/>
       <c r="G39" s="15"/>
@@ -6945,10 +6945,10 @@
         <v>26</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F40" s="22"/>
       <c r="G40" s="15"/>
@@ -6961,27 +6961,27 @@
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="29" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="D41" s="29" t="s">
-        <v>327</v>
-      </c>
-      <c r="F41" s="77" t="s">
-        <v>329</v>
-      </c>
-      <c r="G41" s="77"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="77"/>
+        <v>323</v>
+      </c>
+      <c r="F41" s="76" t="s">
+        <v>325</v>
+      </c>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
     </row>
     <row r="42" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F42" s="22"/>
       <c r="G42" s="15"/>
@@ -6993,10 +6993,10 @@
         <v>26</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F43" s="22"/>
       <c r="G43" s="15"/>
@@ -7012,7 +7012,7 @@
         <v>24</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F44" s="22"/>
       <c r="G44" s="15"/>
@@ -7030,172 +7030,172 @@
       <c r="I45" s="14"/>
     </row>
     <row r="46" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="76" t="s">
+      <c r="A46" s="77" t="s">
+        <v>349</v>
+      </c>
+      <c r="B46" s="77"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="77"/>
+      <c r="F46" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G46" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H46" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I46" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A47" s="77" t="s">
+        <v>350</v>
+      </c>
+      <c r="B47" s="77"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="77"/>
+      <c r="F47" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G47" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H47" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I47" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A48" s="77" t="s">
+        <v>351</v>
+      </c>
+      <c r="B48" s="77"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="77"/>
+      <c r="F48" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G48" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H48" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I48" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A49" s="77" t="s">
+        <v>352</v>
+      </c>
+      <c r="B49" s="77"/>
+      <c r="C49" s="77"/>
+      <c r="D49" s="77"/>
+      <c r="F49" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G49" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="H49" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="I49" s="31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A50" s="77" t="s">
         <v>353</v>
       </c>
-      <c r="B46" s="76"/>
-      <c r="C46" s="76"/>
-      <c r="D46" s="76"/>
-      <c r="F46" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G46" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H46" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="I46" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="76" t="s">
+      <c r="B50" s="77"/>
+      <c r="C50" s="77"/>
+      <c r="D50" s="77"/>
+      <c r="F50" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G50" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="H50" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="I50" s="31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A51" s="77" t="s">
         <v>354</v>
       </c>
-      <c r="B47" s="76"/>
-      <c r="C47" s="76"/>
-      <c r="D47" s="76"/>
-      <c r="F47" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G47" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H47" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="I47" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="76" t="s">
+      <c r="B51" s="77"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="77"/>
+      <c r="F51" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G51" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="H51" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="I51" s="31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A52" s="77" t="s">
         <v>355</v>
       </c>
-      <c r="B48" s="76"/>
-      <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
-      <c r="F48" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G48" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H48" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="I48" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="76" t="s">
+      <c r="B52" s="77"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="77"/>
+      <c r="F52" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G52" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H52" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I52" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A53" s="77" t="s">
         <v>356</v>
       </c>
-      <c r="B49" s="76"/>
-      <c r="C49" s="76"/>
-      <c r="D49" s="76"/>
-      <c r="F49" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G49" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="H49" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="I49" s="31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="76" t="s">
+      <c r="B53" s="77"/>
+      <c r="C53" s="77"/>
+      <c r="D53" s="77"/>
+      <c r="F53" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G53" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H53" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I53" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A54" s="77" t="s">
         <v>357</v>
       </c>
-      <c r="B50" s="76"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="76"/>
-      <c r="F50" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G50" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="H50" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="I50" s="31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="76" t="s">
-        <v>358</v>
-      </c>
-      <c r="B51" s="76"/>
-      <c r="C51" s="76"/>
-      <c r="D51" s="76"/>
-      <c r="F51" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G51" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="H51" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="I51" s="31" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="76" t="s">
-        <v>359</v>
-      </c>
-      <c r="B52" s="76"/>
-      <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
-      <c r="F52" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G52" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H52" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="I52" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="76" t="s">
-        <v>360</v>
-      </c>
-      <c r="B53" s="76"/>
-      <c r="C53" s="76"/>
-      <c r="D53" s="76"/>
-      <c r="F53" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G53" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H53" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="I53" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="76" t="s">
-        <v>361</v>
-      </c>
-      <c r="B54" s="76"/>
-      <c r="C54" s="76"/>
-      <c r="D54" s="76"/>
+      <c r="B54" s="77"/>
+      <c r="C54" s="77"/>
+      <c r="D54" s="77"/>
       <c r="F54" s="30" t="s">
         <v>89</v>
       </c>
@@ -7262,12 +7262,12 @@
       <c r="I58" s="14"/>
     </row>
     <row r="59" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="76" t="s">
-        <v>362</v>
-      </c>
-      <c r="B59" s="76"/>
-      <c r="C59" s="76"/>
-      <c r="D59" s="76"/>
+      <c r="A59" s="77" t="s">
+        <v>358</v>
+      </c>
+      <c r="B59" s="77"/>
+      <c r="C59" s="77"/>
+      <c r="D59" s="77"/>
       <c r="F59" s="30" t="s">
         <v>89</v>
       </c>
@@ -7286,10 +7286,10 @@
         <v>26</v>
       </c>
       <c r="C60" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="D60" s="16" t="s">
-        <v>208</v>
       </c>
       <c r="F60" s="22"/>
       <c r="G60" s="15"/>
@@ -7301,10 +7301,10 @@
         <v>26</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F61" s="22"/>
       <c r="G61" s="15"/>
@@ -7322,83 +7322,83 @@
       <c r="I62" s="14"/>
     </row>
     <row r="63" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="76" t="s">
-        <v>363</v>
-      </c>
-      <c r="B63" s="76"/>
-      <c r="C63" s="76"/>
-      <c r="D63" s="76"/>
+      <c r="A63" s="77" t="s">
+        <v>359</v>
+      </c>
+      <c r="B63" s="77"/>
+      <c r="C63" s="77"/>
+      <c r="D63" s="77"/>
       <c r="F63" s="30" t="s">
         <v>89</v>
       </c>
       <c r="G63" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H63" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I63" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="64" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="76" t="s">
-        <v>364</v>
-      </c>
-      <c r="B64" s="76"/>
-      <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
+      <c r="A64" s="77" t="s">
+        <v>360</v>
+      </c>
+      <c r="B64" s="77"/>
+      <c r="C64" s="77"/>
+      <c r="D64" s="77"/>
       <c r="F64" s="30" t="s">
         <v>89</v>
       </c>
       <c r="G64" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H64" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I64" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="76" t="s">
-        <v>365</v>
-      </c>
-      <c r="B65" s="76"/>
-      <c r="C65" s="76"/>
-      <c r="D65" s="76"/>
+      <c r="A65" s="77" t="s">
+        <v>361</v>
+      </c>
+      <c r="B65" s="77"/>
+      <c r="C65" s="77"/>
+      <c r="D65" s="77"/>
       <c r="F65" s="30" t="s">
         <v>89</v>
       </c>
       <c r="G65" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H65" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I65" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="76" t="s">
-        <v>366</v>
-      </c>
-      <c r="B66" s="76"/>
-      <c r="C66" s="76"/>
-      <c r="D66" s="76"/>
+      <c r="A66" s="77" t="s">
+        <v>362</v>
+      </c>
+      <c r="B66" s="77"/>
+      <c r="C66" s="77"/>
+      <c r="D66" s="77"/>
       <c r="F66" s="30" t="s">
         <v>89</v>
       </c>
       <c r="G66" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H66" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="I66" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -7406,7 +7406,7 @@
         <v>26</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D67" s="16"/>
       <c r="F67" s="22"/>
@@ -7419,7 +7419,7 @@
         <v>26</v>
       </c>
       <c r="C68" s="12" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D68" s="16"/>
       <c r="F68" s="22"/>
@@ -7438,12 +7438,12 @@
       <c r="I69" s="14"/>
     </row>
     <row r="70" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="76" t="s">
-        <v>367</v>
-      </c>
-      <c r="B70" s="76"/>
-      <c r="C70" s="76"/>
-      <c r="D70" s="76"/>
+      <c r="A70" s="77" t="s">
+        <v>363</v>
+      </c>
+      <c r="B70" s="77"/>
+      <c r="C70" s="77"/>
+      <c r="D70" s="77"/>
       <c r="F70" s="30" t="s">
         <v>89</v>
       </c>
@@ -7510,12 +7510,12 @@
       <c r="I74" s="14"/>
     </row>
     <row r="75" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="76" t="s">
-        <v>403</v>
-      </c>
-      <c r="B75" s="76"/>
-      <c r="C75" s="76"/>
-      <c r="D75" s="76"/>
+      <c r="A75" s="77" t="s">
+        <v>399</v>
+      </c>
+      <c r="B75" s="77"/>
+      <c r="C75" s="77"/>
+      <c r="D75" s="77"/>
       <c r="F75" s="30" t="s">
         <v>89</v>
       </c>
@@ -7534,10 +7534,10 @@
         <v>26</v>
       </c>
       <c r="C76" s="12" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="F76" s="22"/>
       <c r="G76" s="15"/>
@@ -7555,12 +7555,12 @@
       <c r="I77" s="14"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A78" s="76" t="s">
-        <v>368</v>
-      </c>
-      <c r="B78" s="76"/>
-      <c r="C78" s="76"/>
-      <c r="D78" s="76"/>
+      <c r="A78" s="77" t="s">
+        <v>364</v>
+      </c>
+      <c r="B78" s="77"/>
+      <c r="C78" s="77"/>
+      <c r="D78" s="77"/>
       <c r="F78" s="30" t="s">
         <v>89</v>
       </c>
@@ -7575,12 +7575,12 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="76" t="s">
-        <v>369</v>
-      </c>
-      <c r="B79" s="76"/>
-      <c r="C79" s="76"/>
-      <c r="D79" s="76"/>
+      <c r="A79" s="77" t="s">
+        <v>365</v>
+      </c>
+      <c r="B79" s="77"/>
+      <c r="C79" s="77"/>
+      <c r="D79" s="77"/>
       <c r="F79" s="30" t="s">
         <v>89</v>
       </c>
@@ -7614,14 +7614,14 @@
         <v>36</v>
       </c>
       <c r="D81" s="36" t="s">
-        <v>343</v>
-      </c>
-      <c r="F81" s="77" t="s">
-        <v>329</v>
-      </c>
-      <c r="G81" s="77"/>
-      <c r="H81" s="77"/>
-      <c r="I81" s="77"/>
+        <v>339</v>
+      </c>
+      <c r="F81" s="76" t="s">
+        <v>325</v>
+      </c>
+      <c r="G81" s="76"/>
+      <c r="H81" s="76"/>
+      <c r="I81" s="76"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
@@ -7631,7 +7631,7 @@
         <v>37</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F82" s="22"/>
       <c r="G82" s="15"/>
@@ -7646,14 +7646,14 @@
         <v>38</v>
       </c>
       <c r="D83" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="F83" s="77" t="s">
-        <v>329</v>
-      </c>
-      <c r="G83" s="77"/>
-      <c r="H83" s="77"/>
-      <c r="I83" s="77"/>
+        <v>337</v>
+      </c>
+      <c r="F83" s="76" t="s">
+        <v>325</v>
+      </c>
+      <c r="G83" s="76"/>
+      <c r="H83" s="76"/>
+      <c r="I83" s="76"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
@@ -7663,7 +7663,7 @@
         <v>24</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F84" s="22"/>
       <c r="G84" s="15"/>
@@ -7671,12 +7671,12 @@
       <c r="I84" s="15"/>
     </row>
     <row r="86" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="76" t="s">
-        <v>370</v>
-      </c>
-      <c r="B86" s="76"/>
-      <c r="C86" s="76"/>
-      <c r="D86" s="76"/>
+      <c r="A86" s="77" t="s">
+        <v>366</v>
+      </c>
+      <c r="B86" s="77"/>
+      <c r="C86" s="77"/>
+      <c r="D86" s="77"/>
       <c r="F86" s="30" t="s">
         <v>89</v>
       </c>
@@ -7720,24 +7720,24 @@
       </c>
       <c r="B89" s="34"/>
       <c r="C89" s="35" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D89" s="36"/>
       <c r="E89" s="37"/>
-      <c r="F89" s="77" t="s">
-        <v>329</v>
-      </c>
-      <c r="G89" s="77"/>
-      <c r="H89" s="77"/>
-      <c r="I89" s="77"/>
+      <c r="F89" s="76" t="s">
+        <v>325</v>
+      </c>
+      <c r="G89" s="76"/>
+      <c r="H89" s="76"/>
+      <c r="I89" s="76"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A91" s="76" t="s">
-        <v>402</v>
-      </c>
-      <c r="B91" s="76"/>
-      <c r="C91" s="76"/>
-      <c r="D91" s="76"/>
+      <c r="A91" s="77" t="s">
+        <v>398</v>
+      </c>
+      <c r="B91" s="77"/>
+      <c r="C91" s="77"/>
+      <c r="D91" s="77"/>
       <c r="F91" s="30" t="s">
         <v>89</v>
       </c>
@@ -7756,7 +7756,7 @@
         <v>26</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F92" s="22"/>
       <c r="G92" s="15"/>
@@ -7768,7 +7768,7 @@
         <v>26</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F93" s="22"/>
       <c r="G93" s="15"/>
@@ -7780,7 +7780,7 @@
         <v>26</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F94" s="22"/>
       <c r="G94" s="15"/>
@@ -7788,12 +7788,12 @@
       <c r="I94" s="15"/>
     </row>
     <row r="96" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A96" s="76" t="s">
-        <v>371</v>
-      </c>
-      <c r="B96" s="76"/>
-      <c r="C96" s="76"/>
-      <c r="D96" s="76"/>
+      <c r="A96" s="77" t="s">
+        <v>367</v>
+      </c>
+      <c r="B96" s="77"/>
+      <c r="C96" s="77"/>
+      <c r="D96" s="77"/>
       <c r="F96" s="30" t="s">
         <v>89</v>
       </c>
@@ -7865,7 +7865,7 @@
         <v>26</v>
       </c>
       <c r="C101" s="18" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D101" s="16"/>
       <c r="F101" s="22"/>
@@ -7874,12 +7874,12 @@
       <c r="I101" s="15"/>
     </row>
     <row r="103" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A103" s="76" t="s">
-        <v>372</v>
-      </c>
-      <c r="B103" s="76"/>
-      <c r="C103" s="76"/>
-      <c r="D103" s="76"/>
+      <c r="A103" s="77" t="s">
+        <v>368</v>
+      </c>
+      <c r="B103" s="77"/>
+      <c r="C103" s="77"/>
+      <c r="D103" s="77"/>
       <c r="F103" s="30" t="s">
         <v>89</v>
       </c>
@@ -7899,7 +7899,7 @@
         <v>26</v>
       </c>
       <c r="C104" s="18" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F104" s="22"/>
       <c r="G104" s="15"/>
@@ -7912,7 +7912,7 @@
         <v>26</v>
       </c>
       <c r="C105" s="18" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F105" s="22"/>
       <c r="G105" s="15"/>
@@ -7925,7 +7925,7 @@
         <v>26</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F106" s="22"/>
       <c r="G106" s="15"/>
@@ -7942,12 +7942,12 @@
       <c r="I107" s="15"/>
     </row>
     <row r="108" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A108" s="76" t="s">
-        <v>373</v>
-      </c>
-      <c r="B108" s="76"/>
-      <c r="C108" s="76"/>
-      <c r="D108" s="76"/>
+      <c r="A108" s="77" t="s">
+        <v>369</v>
+      </c>
+      <c r="B108" s="77"/>
+      <c r="C108" s="77"/>
+      <c r="D108" s="77"/>
       <c r="F108" s="30" t="s">
         <v>89</v>
       </c>
@@ -7967,7 +7967,7 @@
         <v>26</v>
       </c>
       <c r="C109" s="18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F109" s="22"/>
       <c r="G109" s="15"/>
@@ -7980,7 +7980,7 @@
         <v>26</v>
       </c>
       <c r="C110" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F110" s="22"/>
       <c r="G110" s="15"/>
@@ -7992,7 +7992,7 @@
         <v>26</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F111" s="22"/>
       <c r="G111" s="15"/>
@@ -8004,7 +8004,7 @@
         <v>26</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F112" s="22"/>
       <c r="G112" s="15"/>
@@ -8016,7 +8016,7 @@
         <v>26</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F113" s="22"/>
       <c r="G113" s="15"/>
@@ -8031,7 +8031,7 @@
         <v>24</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F114" s="22"/>
       <c r="G114" s="15"/>
@@ -8042,12 +8042,12 @@
       <c r="B115" s="13"/>
     </row>
     <row r="116" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A116" s="76" t="s">
-        <v>374</v>
-      </c>
-      <c r="B116" s="76"/>
-      <c r="C116" s="76"/>
-      <c r="D116" s="76"/>
+      <c r="A116" s="77" t="s">
+        <v>370</v>
+      </c>
+      <c r="B116" s="77"/>
+      <c r="C116" s="77"/>
+      <c r="D116" s="77"/>
       <c r="F116" s="30" t="s">
         <v>89</v>
       </c>
@@ -8066,10 +8066,10 @@
         <v>26</v>
       </c>
       <c r="C117" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F117" s="22"/>
       <c r="G117" s="15"/>
@@ -8081,10 +8081,10 @@
         <v>26</v>
       </c>
       <c r="C118" s="18" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="F118" s="22"/>
       <c r="G118" s="15"/>
@@ -8096,10 +8096,10 @@
         <v>26</v>
       </c>
       <c r="C119" s="18" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="F119" s="22"/>
       <c r="G119" s="15"/>
@@ -8111,7 +8111,7 @@
         <v>26</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="F120" s="22"/>
       <c r="G120" s="15"/>
@@ -8123,7 +8123,7 @@
         <v>26</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F121" s="22"/>
       <c r="G121" s="15"/>
@@ -8135,7 +8135,7 @@
         <v>26</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F122" s="22"/>
       <c r="G122" s="15"/>
@@ -8147,7 +8147,7 @@
         <v>26</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F123" s="22"/>
       <c r="G123" s="15"/>
@@ -8159,7 +8159,7 @@
         <v>26</v>
       </c>
       <c r="C124" s="18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F124" s="22"/>
       <c r="G124" s="15"/>
@@ -8171,7 +8171,7 @@
         <v>26</v>
       </c>
       <c r="C125" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F125" s="22"/>
       <c r="G125" s="15"/>
@@ -8183,7 +8183,7 @@
         <v>26</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F126" s="22"/>
       <c r="G126" s="15"/>
@@ -8195,10 +8195,10 @@
         <v>26</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F127" s="22"/>
       <c r="G127" s="15"/>
@@ -8210,10 +8210,10 @@
         <v>26</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F128" s="22"/>
       <c r="G128" s="15"/>
@@ -8225,10 +8225,10 @@
         <v>26</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="F129" s="22"/>
       <c r="G129" s="15"/>
@@ -8243,12 +8243,12 @@
       <c r="I130" s="15"/>
     </row>
     <row r="131" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A131" s="76" t="s">
-        <v>419</v>
-      </c>
-      <c r="B131" s="76"/>
-      <c r="C131" s="76"/>
-      <c r="D131" s="76"/>
+      <c r="A131" s="77" t="s">
+        <v>415</v>
+      </c>
+      <c r="B131" s="77"/>
+      <c r="C131" s="77"/>
+      <c r="D131" s="77"/>
       <c r="F131" s="30" t="s">
         <v>89</v>
       </c>
@@ -8263,12 +8263,12 @@
       </c>
     </row>
     <row r="132" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A132" s="76" t="s">
-        <v>470</v>
-      </c>
-      <c r="B132" s="76"/>
-      <c r="C132" s="76"/>
-      <c r="D132" s="76"/>
+      <c r="A132" s="77" t="s">
+        <v>464</v>
+      </c>
+      <c r="B132" s="77"/>
+      <c r="C132" s="77"/>
+      <c r="D132" s="77"/>
       <c r="F132" s="30" t="s">
         <v>89</v>
       </c>
@@ -8287,10 +8287,10 @@
         <v>26</v>
       </c>
       <c r="C133" s="26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F133" s="22"/>
       <c r="G133" s="15"/>
@@ -8302,7 +8302,7 @@
         <v>26</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F134" s="22"/>
       <c r="G134" s="15"/>
@@ -8314,7 +8314,7 @@
         <v>26</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F135" s="22"/>
       <c r="G135" s="15"/>
@@ -8326,7 +8326,7 @@
         <v>26</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="F136" s="22"/>
       <c r="G136" s="15"/>
@@ -8338,7 +8338,7 @@
         <v>26</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="F137" s="22"/>
       <c r="G137" s="15"/>
@@ -8350,7 +8350,7 @@
         <v>26</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F138" s="22"/>
       <c r="G138" s="15"/>
@@ -8362,7 +8362,7 @@
         <v>26</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F139" s="22"/>
       <c r="G139" s="15"/>
@@ -8374,7 +8374,7 @@
         <v>26</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="F140" s="22"/>
       <c r="G140" s="15"/>
@@ -8386,7 +8386,7 @@
         <v>26</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F141" s="22"/>
       <c r="G141" s="15"/>
@@ -8398,7 +8398,7 @@
         <v>26</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="F142" s="22"/>
       <c r="G142" s="15"/>
@@ -8410,7 +8410,7 @@
         <v>26</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F143" s="22"/>
       <c r="G143" s="15"/>
@@ -8422,7 +8422,7 @@
         <v>26</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F144" s="22"/>
       <c r="G144" s="15"/>
@@ -8437,12 +8437,12 @@
       <c r="I145" s="41"/>
     </row>
     <row r="146" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A146" s="76" t="s">
-        <v>438</v>
-      </c>
-      <c r="B146" s="76"/>
-      <c r="C146" s="76"/>
-      <c r="D146" s="76"/>
+      <c r="A146" s="77" t="s">
+        <v>433</v>
+      </c>
+      <c r="B146" s="77"/>
+      <c r="C146" s="77"/>
+      <c r="D146" s="77"/>
       <c r="F146" s="30" t="s">
         <v>89</v>
       </c>
@@ -8457,12 +8457,12 @@
       </c>
     </row>
     <row r="147" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A147" s="76" t="s">
-        <v>439</v>
-      </c>
-      <c r="B147" s="76"/>
-      <c r="C147" s="76"/>
-      <c r="D147" s="76"/>
+      <c r="A147" s="77" t="s">
+        <v>434</v>
+      </c>
+      <c r="B147" s="77"/>
+      <c r="C147" s="77"/>
+      <c r="D147" s="77"/>
       <c r="F147" s="30" t="s">
         <v>89</v>
       </c>
@@ -8481,7 +8481,7 @@
         <v>26</v>
       </c>
       <c r="C148" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F148" s="22"/>
       <c r="G148" s="41"/>
@@ -8493,7 +8493,7 @@
         <v>26</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F149" s="22"/>
       <c r="G149" s="41"/>
@@ -8504,12 +8504,12 @@
       <c r="B150" s="13"/>
     </row>
     <row r="151" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A151" s="76" t="s">
-        <v>422</v>
-      </c>
-      <c r="B151" s="76"/>
-      <c r="C151" s="76"/>
-      <c r="D151" s="76"/>
+      <c r="A151" s="77" t="s">
+        <v>418</v>
+      </c>
+      <c r="B151" s="77"/>
+      <c r="C151" s="77"/>
+      <c r="D151" s="77"/>
       <c r="F151" s="30" t="s">
         <v>89</v>
       </c>
@@ -8528,10 +8528,10 @@
         <v>26</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F152" s="22"/>
       <c r="G152" s="41"/>
@@ -8543,10 +8543,10 @@
         <v>26</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F153" s="22"/>
       <c r="G153" s="41"/>
@@ -8558,10 +8558,10 @@
         <v>26</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F154" s="22"/>
       <c r="G154" s="41"/>
@@ -8576,12 +8576,12 @@
       <c r="I155" s="41"/>
     </row>
     <row r="156" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A156" s="76" t="s">
-        <v>369</v>
-      </c>
-      <c r="B156" s="76"/>
-      <c r="C156" s="76"/>
-      <c r="D156" s="76"/>
+      <c r="A156" s="77" t="s">
+        <v>365</v>
+      </c>
+      <c r="B156" s="77"/>
+      <c r="C156" s="77"/>
+      <c r="D156" s="77"/>
       <c r="F156" s="30" t="s">
         <v>89</v>
       </c>
@@ -8603,7 +8603,7 @@
         <v>36</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="F157" s="22"/>
       <c r="G157" s="39"/>
@@ -8615,10 +8615,10 @@
         <v>26</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F158" s="22"/>
       <c r="G158" s="39"/>
@@ -8633,7 +8633,7 @@
         <v>38</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F159" s="22"/>
       <c r="G159" s="39"/>
@@ -8656,12 +8656,12 @@
       <c r="B161" s="13"/>
     </row>
     <row r="162" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A162" s="76" t="s">
-        <v>416</v>
-      </c>
-      <c r="B162" s="76"/>
-      <c r="C162" s="76"/>
-      <c r="D162" s="76"/>
+      <c r="A162" s="77" t="s">
+        <v>412</v>
+      </c>
+      <c r="B162" s="77"/>
+      <c r="C162" s="77"/>
+      <c r="D162" s="77"/>
       <c r="F162" s="30" t="s">
         <v>89</v>
       </c>
@@ -8681,7 +8681,7 @@
       </c>
       <c r="B163" s="13"/>
       <c r="C163" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F163" s="22"/>
       <c r="G163" s="41"/>
@@ -8694,7 +8694,7 @@
       </c>
       <c r="B164" s="13"/>
       <c r="C164" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F164" s="22"/>
       <c r="G164" s="41"/>
@@ -8709,12 +8709,12 @@
       <c r="I165" s="15"/>
     </row>
     <row r="166" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A166" s="76" t="s">
-        <v>449</v>
-      </c>
-      <c r="B166" s="76"/>
-      <c r="C166" s="76"/>
-      <c r="D166" s="76"/>
+      <c r="A166" s="77" t="s">
+        <v>444</v>
+      </c>
+      <c r="B166" s="77"/>
+      <c r="C166" s="77"/>
+      <c r="D166" s="77"/>
       <c r="F166" s="30" t="s">
         <v>89</v>
       </c>
@@ -8729,12 +8729,12 @@
       </c>
     </row>
     <row r="167" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A167" s="76" t="s">
-        <v>450</v>
-      </c>
-      <c r="B167" s="76"/>
-      <c r="C167" s="76"/>
-      <c r="D167" s="76"/>
+      <c r="A167" s="77" t="s">
+        <v>445</v>
+      </c>
+      <c r="B167" s="77"/>
+      <c r="C167" s="77"/>
+      <c r="D167" s="77"/>
       <c r="F167" s="30" t="s">
         <v>89</v>
       </c>
@@ -8749,12 +8749,12 @@
       </c>
     </row>
     <row r="168" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A168" s="76" t="s">
-        <v>466</v>
-      </c>
-      <c r="B168" s="76"/>
-      <c r="C168" s="76"/>
-      <c r="D168" s="76"/>
+      <c r="A168" s="77" t="s">
+        <v>460</v>
+      </c>
+      <c r="B168" s="77"/>
+      <c r="C168" s="77"/>
+      <c r="D168" s="77"/>
       <c r="F168" s="30" t="s">
         <v>89</v>
       </c>
@@ -8769,12 +8769,12 @@
       </c>
     </row>
     <row r="169" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A169" s="76" t="s">
-        <v>465</v>
-      </c>
-      <c r="B169" s="76"/>
-      <c r="C169" s="76"/>
-      <c r="D169" s="76"/>
+      <c r="A169" s="77" t="s">
+        <v>459</v>
+      </c>
+      <c r="B169" s="77"/>
+      <c r="C169" s="77"/>
+      <c r="D169" s="77"/>
       <c r="F169" s="30" t="s">
         <v>89</v>
       </c>
@@ -8793,7 +8793,7 @@
         <v>26</v>
       </c>
       <c r="C170" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F170" s="22"/>
       <c r="G170" s="15"/>
@@ -8805,7 +8805,7 @@
         <v>26</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="F171" s="22"/>
       <c r="G171" s="15"/>
@@ -8816,12 +8816,12 @@
       <c r="B172" s="13"/>
     </row>
     <row r="173" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A173" s="76" t="s">
-        <v>375</v>
-      </c>
-      <c r="B173" s="76"/>
-      <c r="C173" s="76"/>
-      <c r="D173" s="76"/>
+      <c r="A173" s="77" t="s">
+        <v>371</v>
+      </c>
+      <c r="B173" s="77"/>
+      <c r="C173" s="77"/>
+      <c r="D173" s="77"/>
       <c r="F173" s="30" t="s">
         <v>89</v>
       </c>
@@ -8840,10 +8840,10 @@
         <v>26</v>
       </c>
       <c r="C174" s="18" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F174" s="22"/>
       <c r="G174" s="15"/>
@@ -8855,10 +8855,10 @@
         <v>26</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="F175" s="22"/>
       <c r="G175" s="15"/>
@@ -8870,10 +8870,10 @@
         <v>26</v>
       </c>
       <c r="C176" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D176" s="4" t="s">
         <v>136</v>
-      </c>
-      <c r="D176" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="F176" s="22"/>
       <c r="G176" s="15"/>
@@ -8885,10 +8885,10 @@
         <v>26</v>
       </c>
       <c r="C177" s="18" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F177" s="22"/>
       <c r="G177" s="15"/>
@@ -8900,10 +8900,10 @@
         <v>26</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F178" s="22"/>
       <c r="G178" s="15"/>
@@ -8911,12 +8911,12 @@
       <c r="I178" s="15"/>
     </row>
     <row r="180" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A180" s="76" t="s">
-        <v>376</v>
-      </c>
-      <c r="B180" s="76"/>
-      <c r="C180" s="76"/>
-      <c r="D180" s="76"/>
+      <c r="A180" s="77" t="s">
+        <v>372</v>
+      </c>
+      <c r="B180" s="77"/>
+      <c r="C180" s="77"/>
+      <c r="D180" s="77"/>
       <c r="F180" s="30" t="s">
         <v>89</v>
       </c>
@@ -8935,10 +8935,10 @@
         <v>26</v>
       </c>
       <c r="C181" s="18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F181" s="22"/>
       <c r="G181" s="15"/>
@@ -8950,10 +8950,10 @@
         <v>26</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F182" s="22"/>
       <c r="G182" s="15"/>
@@ -8965,10 +8965,10 @@
         <v>26</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F183" s="22"/>
       <c r="G183" s="15"/>
@@ -8980,10 +8980,10 @@
         <v>26</v>
       </c>
       <c r="C184" s="18" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F184" s="22"/>
       <c r="G184" s="15"/>
@@ -8995,10 +8995,10 @@
         <v>26</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="F185" s="22"/>
       <c r="G185" s="15"/>
@@ -9007,22 +9007,22 @@
     </row>
     <row r="186" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="C186" s="21" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B187" s="13"/>
     </row>
     <row r="188" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A188" s="76" t="s">
-        <v>377</v>
-      </c>
-      <c r="B188" s="76"/>
-      <c r="C188" s="76"/>
-      <c r="D188" s="76"/>
+      <c r="A188" s="77" t="s">
+        <v>373</v>
+      </c>
+      <c r="B188" s="77"/>
+      <c r="C188" s="77"/>
+      <c r="D188" s="77"/>
       <c r="F188" s="30" t="s">
         <v>89</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>88</v>
       </c>
       <c r="I188" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -9042,10 +9042,10 @@
         <v>26</v>
       </c>
       <c r="C189" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F189" s="22"/>
       <c r="G189" s="15"/>
@@ -9058,10 +9058,10 @@
         <v>26</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F190" s="22"/>
       <c r="G190" s="15"/>
@@ -9073,10 +9073,10 @@
         <v>26</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F191" s="22"/>
       <c r="G191" s="15"/>
@@ -9088,10 +9088,10 @@
         <v>26</v>
       </c>
       <c r="C192" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F192" s="22"/>
       <c r="G192" s="15"/>
@@ -9103,10 +9103,10 @@
         <v>26</v>
       </c>
       <c r="C193" s="18" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="F193" s="22"/>
       <c r="G193" s="15"/>
@@ -9114,12 +9114,12 @@
       <c r="I193" s="25"/>
     </row>
     <row r="195" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A195" s="76" t="s">
-        <v>378</v>
-      </c>
-      <c r="B195" s="76"/>
-      <c r="C195" s="76"/>
-      <c r="D195" s="76"/>
+      <c r="A195" s="77" t="s">
+        <v>374</v>
+      </c>
+      <c r="B195" s="77"/>
+      <c r="C195" s="77"/>
+      <c r="D195" s="77"/>
       <c r="F195" s="30" t="s">
         <v>89</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>88</v>
       </c>
       <c r="I195" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -9139,10 +9139,10 @@
         <v>26</v>
       </c>
       <c r="C196" s="18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D196" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F196" s="22"/>
       <c r="G196" s="15"/>
@@ -9155,10 +9155,10 @@
         <v>26</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D197" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F197" s="22"/>
       <c r="G197" s="15"/>
@@ -9170,10 +9170,10 @@
         <v>26</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F198" s="22"/>
       <c r="G198" s="15"/>
@@ -9185,10 +9185,10 @@
         <v>26</v>
       </c>
       <c r="C199" s="18" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F199" s="22"/>
       <c r="G199" s="15"/>
@@ -9200,10 +9200,10 @@
         <v>26</v>
       </c>
       <c r="C200" s="18" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F200" s="22"/>
       <c r="G200" s="15"/>
@@ -9215,10 +9215,10 @@
         <v>26</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F201" s="22"/>
       <c r="G201" s="15"/>
@@ -9226,12 +9226,12 @@
       <c r="I201" s="25"/>
     </row>
     <row r="203" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A203" s="76" t="s">
-        <v>379</v>
-      </c>
-      <c r="B203" s="76"/>
-      <c r="C203" s="76"/>
-      <c r="D203" s="76"/>
+      <c r="A203" s="77" t="s">
+        <v>375</v>
+      </c>
+      <c r="B203" s="77"/>
+      <c r="C203" s="77"/>
+      <c r="D203" s="77"/>
       <c r="F203" s="30" t="s">
         <v>89</v>
       </c>
@@ -9251,7 +9251,7 @@
         <v>26</v>
       </c>
       <c r="C204" s="18" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="F204" s="22"/>
       <c r="G204" s="22"/>
@@ -9264,7 +9264,7 @@
         <v>26</v>
       </c>
       <c r="C205" s="18" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="F205" s="22"/>
       <c r="G205" s="22"/>
@@ -9276,7 +9276,7 @@
         <v>26</v>
       </c>
       <c r="C206" s="18" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F206" s="22"/>
       <c r="G206" s="22"/>
@@ -9288,7 +9288,7 @@
         <v>26</v>
       </c>
       <c r="C207" s="18" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F207" s="22"/>
       <c r="G207" s="22"/>
@@ -9300,7 +9300,7 @@
         <v>26</v>
       </c>
       <c r="C208" s="18" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="F208" s="22"/>
       <c r="G208" s="22"/>
@@ -9313,26 +9313,28 @@
     <row r="210" spans="3:3" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A203:D203"/>
+    <mergeCell ref="A156:D156"/>
+    <mergeCell ref="A169:D169"/>
+    <mergeCell ref="A173:D173"/>
+    <mergeCell ref="A180:D180"/>
+    <mergeCell ref="A188:D188"/>
+    <mergeCell ref="A195:D195"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A131:D131"/>
+    <mergeCell ref="A166:D166"/>
+    <mergeCell ref="A167:D167"/>
+    <mergeCell ref="A168:D168"/>
+    <mergeCell ref="A162:D162"/>
+    <mergeCell ref="A151:D151"/>
+    <mergeCell ref="A146:D146"/>
+    <mergeCell ref="A147:D147"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A108:D108"/>
     <mergeCell ref="F89:I89"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A19:D19"/>
@@ -9349,28 +9351,26 @@
     <mergeCell ref="A50:D50"/>
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A52:D52"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="A166:D166"/>
-    <mergeCell ref="A167:D167"/>
-    <mergeCell ref="A168:D168"/>
-    <mergeCell ref="A162:D162"/>
-    <mergeCell ref="A151:D151"/>
-    <mergeCell ref="A146:D146"/>
-    <mergeCell ref="A147:D147"/>
-    <mergeCell ref="A132:D132"/>
-    <mergeCell ref="A203:D203"/>
-    <mergeCell ref="A156:D156"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="A180:D180"/>
-    <mergeCell ref="A188:D188"/>
-    <mergeCell ref="A195:D195"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed redundant entry on Accepted Values tab
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_2D2EDAC1EA08F252476343E40134398ECC69A957" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{69D36759-5961-408D-8938-75440E22905A}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="12503" yWindow="-3533" windowWidth="24495" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12510" yWindow="-3540" windowWidth="24495" windowHeight="15795"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATION" sheetId="6" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1364" uniqueCount="506">
   <si>
     <t>SSP</t>
   </si>
@@ -1802,18 +1801,6 @@
   </si>
   <si>
     <t>/*/back-matter/resource/resource/hash/@algorithm</t>
-  </si>
-  <si>
-    <t>operational</t>
-  </si>
-  <si>
-    <t>Component is being designed, implemented, or tested, or is pending CM approval, but is not yet operational</t>
-  </si>
-  <si>
-    <t>Component is operational or approved for operations</t>
-  </si>
-  <si>
-    <t>Component has been retired and is no longer available for operation</t>
   </si>
   <si>
     <t>All identifiers are case sensitive.</t>
@@ -2371,7 +2358,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2747,7 +2734,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -2853,9 +2840,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2944,17 +2928,17 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{AEF66C42-1564-4344-9750-5A2353322C32}"/>
+    <cellStyle name="Normal 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3288,123 +3272,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57CEA3A-8DD1-44C9-85C0-D74433EA434F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="43.7" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" style="57" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" style="57" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="57" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="57" customWidth="1"/>
-    <col min="5" max="5" width="19" style="57" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="57"/>
+    <col min="1" max="1" width="58.42578125" style="56" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" style="56" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" style="56" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="56" customWidth="1"/>
+    <col min="5" max="5" width="19" style="56" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="56"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="78.599999999999994" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="70" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="65"/>
+      <c r="H1" s="56" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3" s="58"/>
+    </row>
+    <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="68" t="s">
+        <v>493</v>
+      </c>
+      <c r="B4" s="68"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+    </row>
+    <row r="5" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="69" t="s">
+        <v>482</v>
+      </c>
+      <c r="B5" s="69"/>
+      <c r="C5" s="60"/>
+    </row>
+    <row r="6" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>483</v>
+      </c>
+      <c r="B6" s="62"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+    </row>
+    <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="69" t="s">
         <v>485</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="66"/>
-      <c r="H1" s="57" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="58"/>
-      <c r="B2" s="59"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="60" t="s">
+      <c r="B7" s="67"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+    </row>
+    <row r="8" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
         <v>484</v>
       </c>
-      <c r="B3" s="59"/>
-    </row>
-    <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69" t="s">
-        <v>497</v>
-      </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-    </row>
-    <row r="5" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+      <c r="B8" s="67"/>
+    </row>
+    <row r="9" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="59" t="s">
         <v>486</v>
       </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="61"/>
-    </row>
-    <row r="6" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="60" t="s">
+      <c r="B9" s="62"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+    </row>
+    <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="69" t="s">
         <v>487</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="62"/>
-      <c r="E6" s="62"/>
-    </row>
-    <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="63"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="63"/>
+    </row>
+    <row r="11" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="66" t="s">
+        <v>492</v>
+      </c>
+      <c r="B11" s="67"/>
+    </row>
+    <row r="12" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="69" t="s">
+        <v>488</v>
+      </c>
+      <c r="B12" s="69"/>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
+        <v>490</v>
+      </c>
+      <c r="B13" s="67"/>
+    </row>
+    <row r="14" spans="1:8" ht="43.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="66" t="s">
         <v>489</v>
       </c>
-      <c r="B7" s="68"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-    </row>
-    <row r="8" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
-        <v>488</v>
-      </c>
-      <c r="B8" s="68"/>
-    </row>
-    <row r="9" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="60" t="s">
-        <v>490</v>
-      </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-    </row>
-    <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="70" t="s">
-        <v>491</v>
-      </c>
-      <c r="B10" s="68"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-    </row>
-    <row r="11" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="67" t="s">
-        <v>496</v>
-      </c>
-      <c r="B11" s="68"/>
-    </row>
-    <row r="12" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="70" t="s">
-        <v>492</v>
-      </c>
-      <c r="B12" s="70"/>
-    </row>
-    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="68" t="s">
-        <v>494</v>
-      </c>
-      <c r="B13" s="68"/>
-    </row>
-    <row r="14" spans="1:8" ht="43.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="67" t="s">
-        <v>493</v>
-      </c>
-      <c r="B14" s="68"/>
+      <c r="B14" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3420,9 +3404,9 @@
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" xr:uid="{73808668-E3ED-4444-9D02-1E1FBF599EB8}"/>
-    <hyperlink ref="A14" r:id="rId2" xr:uid="{F0EF1C87-C506-4135-A240-2AFDA3195746}"/>
-    <hyperlink ref="A11" r:id="rId3" xr:uid="{8AF31DB5-1A97-44B6-AF6C-4C5ED8A8A8B4}"/>
+    <hyperlink ref="A8" r:id="rId1"/>
+    <hyperlink ref="A14" r:id="rId2"/>
+    <hyperlink ref="A11" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -3431,7 +3415,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629A29D9-5EDF-496E-9388-11A8CD056300}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3454,26 +3438,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
-        <v>495</v>
+      <c r="A1" s="64" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="72" t="s">
         <v>308</v>
       </c>
-      <c r="E2" s="73"/>
+      <c r="E2" s="72"/>
       <c r="F2" t="s">
         <v>329</v>
       </c>
-      <c r="G2" s="74" t="s">
-        <v>474</v>
-      </c>
-      <c r="H2" s="74" t="s">
-        <v>395</v>
+      <c r="G2" s="73" t="s">
+        <v>470</v>
+      </c>
+      <c r="H2" s="73" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3493,11 +3477,11 @@
         <v>25</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>382</v>
-      </c>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="53" t="s">
+        <v>378</v>
+      </c>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="52" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3515,11 +3499,11 @@
       <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="56" t="s">
-        <v>423</v>
+      <c r="F4" s="55" t="s">
+        <v>419</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="4" t="s">
@@ -3542,11 +3526,11 @@
       <c r="E5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="56" t="s">
-        <v>424</v>
+      <c r="F5" s="55" t="s">
+        <v>420</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>301</v>
@@ -3556,7 +3540,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F6" s="56"/>
+      <c r="F6" s="55"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -3571,11 +3555,11 @@
       <c r="E7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="56" t="s">
+      <c r="F7" s="55" t="s">
         <v>343</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I7" s="4" t="s">
         <v>300</v>
@@ -3594,14 +3578,14 @@
       <c r="E8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="56" t="s">
+      <c r="F8" s="55" t="s">
         <v>347</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -3617,8 +3601,8 @@
       <c r="E9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="56" t="s">
-        <v>425</v>
+      <c r="F9" s="55" t="s">
+        <v>421</v>
       </c>
       <c r="G9" s="6" t="s">
         <v>330</v>
@@ -3640,8 +3624,8 @@
       <c r="E10" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="56" t="s">
-        <v>426</v>
+      <c r="F10" s="55" t="s">
+        <v>422</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>330</v>
@@ -3663,8 +3647,8 @@
       <c r="E11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="56" t="s">
-        <v>427</v>
+      <c r="F11" s="55" t="s">
+        <v>423</v>
       </c>
       <c r="G11" s="6" t="s">
         <v>330</v>
@@ -3686,8 +3670,8 @@
       <c r="E12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="56" t="s">
-        <v>428</v>
+      <c r="F12" s="55" t="s">
+        <v>424</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>330</v>
@@ -3697,7 +3681,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F13" s="56"/>
+      <c r="F13" s="55"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -3712,11 +3696,11 @@
       <c r="E14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="56" t="s">
+      <c r="F14" s="55" t="s">
         <v>359</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>208</v>
@@ -3735,11 +3719,11 @@
       <c r="E15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="56" t="s">
+      <c r="F15" s="55" t="s">
         <v>360</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>209</v>
@@ -3758,11 +3742,11 @@
       <c r="E16" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="56" t="s">
+      <c r="F16" s="55" t="s">
         <v>361</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>210</v>
@@ -3781,11 +3765,11 @@
       <c r="E17" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="F17" s="55" t="s">
         <v>362</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>211</v>
@@ -3804,18 +3788,18 @@
       <c r="E18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="56" t="s">
-        <v>429</v>
+      <c r="F18" s="55" t="s">
+        <v>425</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I18" s="4" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F19" s="56"/>
+      <c r="F19" s="55"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
@@ -3830,11 +3814,11 @@
       <c r="E20" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="56" t="s">
-        <v>430</v>
+      <c r="F20" s="55" t="s">
+        <v>426</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>26</v>
@@ -3844,7 +3828,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F21" s="56"/>
+      <c r="F21" s="55"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -3859,15 +3843,15 @@
       <c r="E22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="56" t="s">
+      <c r="F22" s="55" t="s">
         <v>367</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F23" s="56"/>
+      <c r="F23" s="55"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
@@ -3882,11 +3866,11 @@
       <c r="E24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="56" t="s">
-        <v>435</v>
+      <c r="F24" s="55" t="s">
+        <v>431</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3902,15 +3886,15 @@
       <c r="E25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="56" t="s">
-        <v>436</v>
+      <c r="F25" s="55" t="s">
+        <v>432</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F26" s="56"/>
+      <c r="F26" s="55"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -3925,11 +3909,11 @@
       <c r="E27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="56" t="s">
-        <v>437</v>
+      <c r="F27" s="55" t="s">
+        <v>433</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3945,11 +3929,11 @@
       <c r="E28" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="56" t="s">
-        <v>438</v>
+      <c r="F28" s="55" t="s">
+        <v>434</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3965,11 +3949,11 @@
       <c r="E29" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="56" t="s">
-        <v>439</v>
+      <c r="F29" s="55" t="s">
+        <v>435</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -3985,11 +3969,11 @@
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="56" t="s">
+      <c r="F30" s="55" t="s">
         <v>368</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>106</v>
@@ -4008,11 +3992,11 @@
       <c r="E31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="56" t="s">
-        <v>440</v>
+      <c r="F31" s="55" t="s">
+        <v>436</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>104</v>
@@ -4020,7 +4004,7 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>31</v>
@@ -4031,19 +4015,19 @@
       <c r="E32" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="56" t="s">
-        <v>441</v>
+      <c r="F32" s="55" t="s">
+        <v>437</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>31</v>
@@ -4054,11 +4038,11 @@
       <c r="E33" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F33" s="56" t="s">
-        <v>442</v>
+      <c r="F33" s="55" t="s">
+        <v>438</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I33" s="4" t="s">
         <v>105</v>
@@ -4077,19 +4061,19 @@
       <c r="E34" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="56" t="s">
-        <v>443</v>
+      <c r="F34" s="55" t="s">
+        <v>439</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F35" s="56"/>
+      <c r="F35" s="55"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="54" t="s">
-        <v>508</v>
+      <c r="A36" s="53" t="s">
+        <v>504</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>31</v>
@@ -4100,18 +4084,18 @@
       <c r="E36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F36" s="56" t="s">
-        <v>431</v>
+      <c r="F36" s="55" t="s">
+        <v>427</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="54" t="s">
+      <c r="A37" s="53" t="s">
         <v>231</v>
       </c>
       <c r="B37" s="6" t="s">
@@ -4123,19 +4107,19 @@
       <c r="E37" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F37" s="56" t="s">
-        <v>432</v>
+      <c r="F37" s="55" t="s">
+        <v>428</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I37" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A38" s="53" t="s">
         <v>458</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="54" t="s">
-        <v>462</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>31</v>
@@ -4146,18 +4130,18 @@
       <c r="E38" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="56" t="s">
-        <v>463</v>
+      <c r="F38" s="55" t="s">
+        <v>459</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="53" t="s">
         <v>232</v>
       </c>
       <c r="B39" s="6" t="s">
@@ -4169,18 +4153,18 @@
       <c r="E39" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F39" s="56" t="s">
-        <v>418</v>
+      <c r="F39" s="55" t="s">
+        <v>414</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="54" t="s">
+      <c r="A40" s="53" t="s">
         <v>233</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -4192,23 +4176,23 @@
       <c r="E40" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="56" t="s">
-        <v>469</v>
+      <c r="F40" s="55" t="s">
+        <v>465</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="54"/>
-      <c r="F41" s="56"/>
+      <c r="A41" s="53"/>
+      <c r="F41" s="55"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A42" s="54" t="s">
-        <v>467</v>
+      <c r="A42" s="53" t="s">
+        <v>463</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>31</v>
@@ -4219,19 +4203,19 @@
       <c r="E42" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F42" s="56" t="s">
+      <c r="F42" s="55" t="s">
+        <v>464</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A43" s="53" t="s">
         <v>468</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A43" s="54" t="s">
-        <v>472</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>31</v>
@@ -4242,19 +4226,19 @@
       <c r="E43" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F43" s="56" t="s">
-        <v>470</v>
+      <c r="F43" s="55" t="s">
+        <v>466</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="54" t="s">
-        <v>473</v>
+      <c r="A44" s="53" t="s">
+        <v>469</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>31</v>
@@ -4265,18 +4249,18 @@
       <c r="E44" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F44" s="56" t="s">
-        <v>471</v>
+      <c r="F44" s="55" t="s">
+        <v>467</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F45" s="56"/>
+      <c r="F45" s="55"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
@@ -4291,14 +4275,14 @@
       <c r="E46" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F46" s="56" t="s">
-        <v>446</v>
+      <c r="F46" s="55" t="s">
+        <v>442</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4314,14 +4298,14 @@
       <c r="E47" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F47" s="56" t="s">
-        <v>447</v>
+      <c r="F47" s="55" t="s">
+        <v>443</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -4337,11 +4321,11 @@
       <c r="E48" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="56" t="s">
-        <v>448</v>
+      <c r="F48" s="55" t="s">
+        <v>444</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="I48" s="4" t="s">
         <v>159</v>
@@ -4349,7 +4333,7 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>31</v>
@@ -4360,22 +4344,22 @@
       <c r="E49" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F49" s="56" t="s">
-        <v>449</v>
+      <c r="F49" s="55" t="s">
+        <v>445</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="I49" s="4" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F50" s="56"/>
+      <c r="F50" s="55"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>31</v>
@@ -4386,11 +4370,11 @@
       <c r="E51" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F51" s="56" t="s">
-        <v>450</v>
+      <c r="F51" s="55" t="s">
+        <v>446</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>26</v>
@@ -4412,11 +4396,11 @@
       <c r="E52" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F52" s="56" t="s">
-        <v>451</v>
+      <c r="F52" s="55" t="s">
+        <v>447</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>26</v>
@@ -4438,11 +4422,11 @@
       <c r="E53" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F53" s="56" t="s">
-        <v>452</v>
+      <c r="F53" s="55" t="s">
+        <v>448</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>26</v>
@@ -4464,11 +4448,11 @@
       <c r="E54" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F54" s="56" t="s">
-        <v>453</v>
+      <c r="F54" s="55" t="s">
+        <v>449</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>26</v>
@@ -4478,7 +4462,7 @@
       </c>
     </row>
     <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F55" s="56"/>
+      <c r="F55" s="55"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -4493,11 +4477,11 @@
       <c r="E56" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="56" t="s">
-        <v>454</v>
+      <c r="F56" s="55" t="s">
+        <v>450</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>26</v>
@@ -4519,11 +4503,11 @@
       <c r="E57" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F57" s="56" t="s">
-        <v>455</v>
+      <c r="F57" s="55" t="s">
+        <v>451</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>26</v>
@@ -4545,11 +4529,11 @@
       <c r="E58" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F58" s="56" t="s">
-        <v>456</v>
+      <c r="F58" s="55" t="s">
+        <v>452</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>26</v>
@@ -4571,11 +4555,11 @@
       <c r="E59" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F59" s="56" t="s">
-        <v>457</v>
+      <c r="F59" s="55" t="s">
+        <v>453</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>26</v>
@@ -4585,9 +4569,9 @@
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="F60" s="56"/>
-    </row>
-    <row r="61" spans="1:9" s="56" customFormat="1" ht="15.75" x14ac:dyDescent="0.3"/>
+      <c r="F60" s="55"/>
+    </row>
+    <row r="61" spans="1:9" s="55" customFormat="1" ht="15.75" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="D2:E2"/>
@@ -4600,12 +4584,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H71" sqref="H1:H1048576"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4618,8 +4602,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
-        <v>495</v>
+      <c r="A1" s="64" t="s">
+        <v>491</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4629,19 +4613,19 @@
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="72" t="s">
         <v>153</v>
       </c>
-      <c r="B2" s="73"/>
+      <c r="B2" s="72"/>
       <c r="C2" s="28" t="s">
-        <v>380</v>
-      </c>
-      <c r="D2" s="73" t="s">
+        <v>376</v>
+      </c>
+      <c r="D2" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="23" t="s">
         <v>92</v>
       </c>
@@ -4654,7 +4638,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>0</v>
@@ -4673,16 +4657,16 @@
       </c>
     </row>
     <row r="4" spans="1:15" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="74" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="74"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
       <c r="I4" s="27"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -5052,7 +5036,7 @@
         <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
@@ -5067,7 +5051,7 @@
         <v>88</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="I20" s="5"/>
     </row>
@@ -5100,7 +5084,7 @@
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>7</v>
@@ -5115,7 +5099,7 @@
         <v>88</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="I22" s="5"/>
     </row>
@@ -5124,7 +5108,7 @@
         <v>26</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>7</v>
@@ -5139,7 +5123,7 @@
         <v>88</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -5148,7 +5132,7 @@
         <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>7</v>
@@ -5163,7 +5147,7 @@
         <v>88</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -5333,16 +5317,16 @@
       </c>
     </row>
     <row r="33" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="75"/>
-      <c r="C33" s="75"/>
-      <c r="D33" s="75"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
+      <c r="B33" s="74"/>
+      <c r="C33" s="74"/>
+      <c r="D33" s="74"/>
+      <c r="E33" s="74"/>
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="74"/>
       <c r="I33" s="27"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -5461,16 +5445,16 @@
       </c>
     </row>
     <row r="40" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="75"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="75"/>
+      <c r="B40" s="74"/>
+      <c r="C40" s="74"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="74"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
       <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -5496,42 +5480,42 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="43" t="s">
+    <row r="42" spans="1:9" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="B42" s="41"/>
+      <c r="C42" s="42" t="s">
         <v>288</v>
       </c>
-      <c r="D42" s="44" t="s">
-        <v>393</v>
-      </c>
-      <c r="E42" s="44" t="s">
+      <c r="D42" s="43" t="s">
+        <v>389</v>
+      </c>
+      <c r="E42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="F42" s="44" t="s">
+      <c r="F42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="G42" s="44" t="s">
+      <c r="G42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H42" s="45" t="s">
-        <v>394</v>
-      </c>
-      <c r="I42" s="45"/>
+      <c r="H42" s="44" t="s">
+        <v>390</v>
+      </c>
+      <c r="I42" s="44"/>
     </row>
     <row r="44" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="75" t="s">
+      <c r="A44" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="75"/>
-      <c r="C44" s="75"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="75"/>
+      <c r="B44" s="74"/>
+      <c r="C44" s="74"/>
+      <c r="D44" s="74"/>
+      <c r="E44" s="74"/>
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="74"/>
       <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -5558,16 +5542,16 @@
       </c>
     </row>
     <row r="47" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="75" t="s">
+      <c r="A47" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
+      <c r="B47" s="74"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="74"/>
+      <c r="E47" s="74"/>
+      <c r="F47" s="74"/>
+      <c r="G47" s="74"/>
+      <c r="H47" s="74"/>
       <c r="I47" s="27"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -5640,16 +5624,16 @@
       </c>
     </row>
     <row r="52" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="75" t="s">
+      <c r="A52" s="74" t="s">
         <v>149</v>
       </c>
-      <c r="B52" s="75"/>
-      <c r="C52" s="75"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
+      <c r="B52" s="74"/>
+      <c r="C52" s="74"/>
+      <c r="D52" s="74"/>
+      <c r="E52" s="74"/>
+      <c r="F52" s="74"/>
+      <c r="G52" s="74"/>
+      <c r="H52" s="74"/>
       <c r="I52" s="27"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -5745,16 +5729,16 @@
       </c>
     </row>
     <row r="58" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="75" t="s">
+      <c r="A58" s="74" t="s">
         <v>87</v>
       </c>
-      <c r="B58" s="75"/>
-      <c r="C58" s="75"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
+      <c r="B58" s="74"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
+      <c r="E58" s="74"/>
+      <c r="F58" s="74"/>
+      <c r="G58" s="74"/>
+      <c r="H58" s="74"/>
       <c r="I58" s="27"/>
     </row>
     <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
@@ -5823,20 +5807,20 @@
         <v>12</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="75" t="s">
+      <c r="A63" s="74" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="75"/>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
+      <c r="B63" s="74"/>
+      <c r="C63" s="74"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="74"/>
+      <c r="F63" s="74"/>
+      <c r="G63" s="74"/>
+      <c r="H63" s="74"/>
       <c r="I63" s="27"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -6296,8 +6280,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I210"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I204"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
@@ -6315,8 +6299,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
-        <v>495</v>
+      <c r="A1" s="64" t="s">
+        <v>491</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -6327,19 +6311,19 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="72" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="73"/>
+      <c r="B2" s="72"/>
       <c r="C2" s="28" t="s">
         <v>306</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -6368,12 +6352,12 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
-        <v>401</v>
-      </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="77"/>
-      <c r="D4" s="77"/>
+      <c r="A4" s="75" t="s">
+        <v>397</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
       <c r="F4" s="30" t="s">
         <v>89</v>
       </c>
@@ -6388,54 +6372,54 @@
       </c>
     </row>
     <row r="5" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="75" t="s">
+        <v>396</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
+      <c r="F5" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>399</v>
+      </c>
+      <c r="D6" s="49" t="s">
         <v>400</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="F5" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G5" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>403</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>404</v>
-      </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F7" s="22"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
     </row>
     <row r="8" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13"/>
@@ -6448,89 +6432,89 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="75" t="s">
+        <v>403</v>
+      </c>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="F9" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G9" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I9" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="75" t="s">
+        <v>402</v>
+      </c>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="F10" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>399</v>
+      </c>
+      <c r="D11" s="49" t="s">
         <v>407</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="F9" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I9" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="77" t="s">
-        <v>406</v>
-      </c>
-      <c r="B10" s="77"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="F10" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>403</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>411</v>
-      </c>
-      <c r="F11" s="51"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="52"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
     </row>
     <row r="12" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F12" s="22"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
     </row>
     <row r="13" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F13" s="22"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
     </row>
     <row r="14" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
@@ -6543,12 +6527,12 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="75" t="s">
         <v>342</v>
       </c>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
       <c r="F15" s="30" t="s">
         <v>89</v>
       </c>
@@ -6577,20 +6561,20 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
     </row>
-    <row r="17" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="49" t="s">
+    <row r="17" spans="1:9" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="48" t="s">
         <v>288</v>
       </c>
-      <c r="D17" s="50" t="s">
+      <c r="D17" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
     </row>
     <row r="18" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
@@ -6603,12 +6587,12 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="75" t="s">
         <v>343</v>
       </c>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="75"/>
       <c r="F19" s="30" t="s">
         <v>89</v>
       </c>
@@ -6623,12 +6607,12 @@
       </c>
     </row>
     <row r="20" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="75" t="s">
         <v>344</v>
       </c>
-      <c r="B20" s="77"/>
-      <c r="C20" s="77"/>
-      <c r="D20" s="77"/>
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
       <c r="F20" s="30" t="s">
         <v>89</v>
       </c>
@@ -6643,12 +6627,12 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="75" t="s">
         <v>345</v>
       </c>
-      <c r="B21" s="77"/>
-      <c r="C21" s="77"/>
-      <c r="D21" s="77"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="75"/>
+      <c r="D21" s="75"/>
       <c r="F21" s="30" t="s">
         <v>89</v>
       </c>
@@ -6663,12 +6647,12 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="75" t="s">
         <v>346</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
-      <c r="D22" s="77"/>
+      <c r="B22" s="75"/>
+      <c r="C22" s="75"/>
+      <c r="D22" s="75"/>
       <c r="F22" s="30" t="s">
         <v>89</v>
       </c>
@@ -6738,12 +6722,12 @@
       <c r="I26" s="14"/>
     </row>
     <row r="27" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="75" t="s">
         <v>347</v>
       </c>
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="77"/>
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
       <c r="F27" s="30" t="s">
         <v>89</v>
       </c>
@@ -6816,12 +6800,12 @@
       <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="77" t="s">
-        <v>397</v>
-      </c>
-      <c r="B32" s="77"/>
-      <c r="C32" s="77"/>
-      <c r="D32" s="77"/>
+      <c r="A32" s="75" t="s">
+        <v>393</v>
+      </c>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
       <c r="F32" s="30" t="s">
         <v>89</v>
       </c>
@@ -6906,12 +6890,12 @@
       <c r="I37" s="14"/>
     </row>
     <row r="38" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="75" t="s">
         <v>348</v>
       </c>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
+      <c r="B38" s="75"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
       <c r="F38" s="30" t="s">
         <v>89</v>
       </c>
@@ -7030,12 +7014,12 @@
       <c r="I45" s="14"/>
     </row>
     <row r="46" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="77" t="s">
+      <c r="A46" s="75" t="s">
         <v>349</v>
       </c>
-      <c r="B46" s="77"/>
-      <c r="C46" s="77"/>
-      <c r="D46" s="77"/>
+      <c r="B46" s="75"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="75"/>
       <c r="F46" s="30" t="s">
         <v>89</v>
       </c>
@@ -7050,12 +7034,12 @@
       </c>
     </row>
     <row r="47" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A47" s="77" t="s">
+      <c r="A47" s="75" t="s">
         <v>350</v>
       </c>
-      <c r="B47" s="77"/>
-      <c r="C47" s="77"/>
-      <c r="D47" s="77"/>
+      <c r="B47" s="75"/>
+      <c r="C47" s="75"/>
+      <c r="D47" s="75"/>
       <c r="F47" s="30" t="s">
         <v>89</v>
       </c>
@@ -7070,12 +7054,12 @@
       </c>
     </row>
     <row r="48" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A48" s="77" t="s">
+      <c r="A48" s="75" t="s">
         <v>351</v>
       </c>
-      <c r="B48" s="77"/>
-      <c r="C48" s="77"/>
-      <c r="D48" s="77"/>
+      <c r="B48" s="75"/>
+      <c r="C48" s="75"/>
+      <c r="D48" s="75"/>
       <c r="F48" s="30" t="s">
         <v>89</v>
       </c>
@@ -7090,12 +7074,12 @@
       </c>
     </row>
     <row r="49" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A49" s="77" t="s">
+      <c r="A49" s="75" t="s">
         <v>352</v>
       </c>
-      <c r="B49" s="77"/>
-      <c r="C49" s="77"/>
-      <c r="D49" s="77"/>
+      <c r="B49" s="75"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="75"/>
       <c r="F49" s="30" t="s">
         <v>89</v>
       </c>
@@ -7110,12 +7094,12 @@
       </c>
     </row>
     <row r="50" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A50" s="77" t="s">
+      <c r="A50" s="75" t="s">
         <v>353</v>
       </c>
-      <c r="B50" s="77"/>
-      <c r="C50" s="77"/>
-      <c r="D50" s="77"/>
+      <c r="B50" s="75"/>
+      <c r="C50" s="75"/>
+      <c r="D50" s="75"/>
       <c r="F50" s="30" t="s">
         <v>89</v>
       </c>
@@ -7130,12 +7114,12 @@
       </c>
     </row>
     <row r="51" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="77" t="s">
+      <c r="A51" s="75" t="s">
         <v>354</v>
       </c>
-      <c r="B51" s="77"/>
-      <c r="C51" s="77"/>
-      <c r="D51" s="77"/>
+      <c r="B51" s="75"/>
+      <c r="C51" s="75"/>
+      <c r="D51" s="75"/>
       <c r="F51" s="30" t="s">
         <v>89</v>
       </c>
@@ -7150,12 +7134,12 @@
       </c>
     </row>
     <row r="52" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A52" s="77" t="s">
+      <c r="A52" s="75" t="s">
         <v>355</v>
       </c>
-      <c r="B52" s="77"/>
-      <c r="C52" s="77"/>
-      <c r="D52" s="77"/>
+      <c r="B52" s="75"/>
+      <c r="C52" s="75"/>
+      <c r="D52" s="75"/>
       <c r="F52" s="30" t="s">
         <v>89</v>
       </c>
@@ -7170,12 +7154,12 @@
       </c>
     </row>
     <row r="53" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A53" s="77" t="s">
+      <c r="A53" s="75" t="s">
         <v>356</v>
       </c>
-      <c r="B53" s="77"/>
-      <c r="C53" s="77"/>
-      <c r="D53" s="77"/>
+      <c r="B53" s="75"/>
+      <c r="C53" s="75"/>
+      <c r="D53" s="75"/>
       <c r="F53" s="30" t="s">
         <v>89</v>
       </c>
@@ -7190,12 +7174,12 @@
       </c>
     </row>
     <row r="54" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="77" t="s">
+      <c r="A54" s="75" t="s">
         <v>357</v>
       </c>
-      <c r="B54" s="77"/>
-      <c r="C54" s="77"/>
-      <c r="D54" s="77"/>
+      <c r="B54" s="75"/>
+      <c r="C54" s="75"/>
+      <c r="D54" s="75"/>
       <c r="F54" s="30" t="s">
         <v>89</v>
       </c>
@@ -7262,12 +7246,12 @@
       <c r="I58" s="14"/>
     </row>
     <row r="59" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A59" s="77" t="s">
+      <c r="A59" s="75" t="s">
         <v>358</v>
       </c>
-      <c r="B59" s="77"/>
-      <c r="C59" s="77"/>
-      <c r="D59" s="77"/>
+      <c r="B59" s="75"/>
+      <c r="C59" s="75"/>
+      <c r="D59" s="75"/>
       <c r="F59" s="30" t="s">
         <v>89</v>
       </c>
@@ -7322,12 +7306,12 @@
       <c r="I62" s="14"/>
     </row>
     <row r="63" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A63" s="77" t="s">
+      <c r="A63" s="75" t="s">
         <v>359</v>
       </c>
-      <c r="B63" s="77"/>
-      <c r="C63" s="77"/>
-      <c r="D63" s="77"/>
+      <c r="B63" s="75"/>
+      <c r="C63" s="75"/>
+      <c r="D63" s="75"/>
       <c r="F63" s="30" t="s">
         <v>89</v>
       </c>
@@ -7342,12 +7326,12 @@
       </c>
     </row>
     <row r="64" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A64" s="77" t="s">
+      <c r="A64" s="75" t="s">
         <v>360</v>
       </c>
-      <c r="B64" s="77"/>
-      <c r="C64" s="77"/>
-      <c r="D64" s="77"/>
+      <c r="B64" s="75"/>
+      <c r="C64" s="75"/>
+      <c r="D64" s="75"/>
       <c r="F64" s="30" t="s">
         <v>89</v>
       </c>
@@ -7362,12 +7346,12 @@
       </c>
     </row>
     <row r="65" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A65" s="77" t="s">
+      <c r="A65" s="75" t="s">
         <v>361</v>
       </c>
-      <c r="B65" s="77"/>
-      <c r="C65" s="77"/>
-      <c r="D65" s="77"/>
+      <c r="B65" s="75"/>
+      <c r="C65" s="75"/>
+      <c r="D65" s="75"/>
       <c r="F65" s="30" t="s">
         <v>89</v>
       </c>
@@ -7382,12 +7366,12 @@
       </c>
     </row>
     <row r="66" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A66" s="77" t="s">
+      <c r="A66" s="75" t="s">
         <v>362</v>
       </c>
-      <c r="B66" s="77"/>
-      <c r="C66" s="77"/>
-      <c r="D66" s="77"/>
+      <c r="B66" s="75"/>
+      <c r="C66" s="75"/>
+      <c r="D66" s="75"/>
       <c r="F66" s="30" t="s">
         <v>89</v>
       </c>
@@ -7438,12 +7422,12 @@
       <c r="I69" s="14"/>
     </row>
     <row r="70" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="77" t="s">
+      <c r="A70" s="75" t="s">
         <v>363</v>
       </c>
-      <c r="B70" s="77"/>
-      <c r="C70" s="77"/>
-      <c r="D70" s="77"/>
+      <c r="B70" s="75"/>
+      <c r="C70" s="75"/>
+      <c r="D70" s="75"/>
       <c r="F70" s="30" t="s">
         <v>89</v>
       </c>
@@ -7510,12 +7494,12 @@
       <c r="I74" s="14"/>
     </row>
     <row r="75" spans="1:9" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A75" s="77" t="s">
-        <v>399</v>
-      </c>
-      <c r="B75" s="77"/>
-      <c r="C75" s="77"/>
-      <c r="D75" s="77"/>
+      <c r="A75" s="75" t="s">
+        <v>395</v>
+      </c>
+      <c r="B75" s="75"/>
+      <c r="C75" s="75"/>
+      <c r="D75" s="75"/>
       <c r="F75" s="30" t="s">
         <v>89</v>
       </c>
@@ -7555,12 +7539,12 @@
       <c r="I77" s="14"/>
     </row>
     <row r="78" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A78" s="77" t="s">
+      <c r="A78" s="75" t="s">
         <v>364</v>
       </c>
-      <c r="B78" s="77"/>
-      <c r="C78" s="77"/>
-      <c r="D78" s="77"/>
+      <c r="B78" s="75"/>
+      <c r="C78" s="75"/>
+      <c r="D78" s="75"/>
       <c r="F78" s="30" t="s">
         <v>89</v>
       </c>
@@ -7575,12 +7559,12 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="77" t="s">
+      <c r="A79" s="75" t="s">
         <v>365</v>
       </c>
-      <c r="B79" s="77"/>
-      <c r="C79" s="77"/>
-      <c r="D79" s="77"/>
+      <c r="B79" s="75"/>
+      <c r="C79" s="75"/>
+      <c r="D79" s="75"/>
       <c r="F79" s="30" t="s">
         <v>89</v>
       </c>
@@ -7671,12 +7655,12 @@
       <c r="I84" s="15"/>
     </row>
     <row r="86" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A86" s="77" t="s">
+      <c r="A86" s="75" t="s">
         <v>366</v>
       </c>
-      <c r="B86" s="77"/>
-      <c r="C86" s="77"/>
-      <c r="D86" s="77"/>
+      <c r="B86" s="75"/>
+      <c r="C86" s="75"/>
+      <c r="D86" s="75"/>
       <c r="F86" s="30" t="s">
         <v>89</v>
       </c>
@@ -7732,12 +7716,12 @@
       <c r="I89" s="76"/>
     </row>
     <row r="91" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A91" s="77" t="s">
-        <v>398</v>
-      </c>
-      <c r="B91" s="77"/>
-      <c r="C91" s="77"/>
-      <c r="D91" s="77"/>
+      <c r="A91" s="75" t="s">
+        <v>394</v>
+      </c>
+      <c r="B91" s="75"/>
+      <c r="C91" s="75"/>
+      <c r="D91" s="75"/>
       <c r="F91" s="30" t="s">
         <v>89</v>
       </c>
@@ -7788,12 +7772,12 @@
       <c r="I94" s="15"/>
     </row>
     <row r="96" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A96" s="77" t="s">
+      <c r="A96" s="75" t="s">
         <v>367</v>
       </c>
-      <c r="B96" s="77"/>
-      <c r="C96" s="77"/>
-      <c r="D96" s="77"/>
+      <c r="B96" s="75"/>
+      <c r="C96" s="75"/>
+      <c r="D96" s="75"/>
       <c r="F96" s="30" t="s">
         <v>89</v>
       </c>
@@ -7874,12 +7858,12 @@
       <c r="I101" s="15"/>
     </row>
     <row r="103" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A103" s="77" t="s">
+      <c r="A103" s="75" t="s">
         <v>368</v>
       </c>
-      <c r="B103" s="77"/>
-      <c r="C103" s="77"/>
-      <c r="D103" s="77"/>
+      <c r="B103" s="75"/>
+      <c r="C103" s="75"/>
+      <c r="D103" s="75"/>
       <c r="F103" s="30" t="s">
         <v>89</v>
       </c>
@@ -7942,12 +7926,12 @@
       <c r="I107" s="15"/>
     </row>
     <row r="108" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A108" s="77" t="s">
+      <c r="A108" s="75" t="s">
         <v>369</v>
       </c>
-      <c r="B108" s="77"/>
-      <c r="C108" s="77"/>
-      <c r="D108" s="77"/>
+      <c r="B108" s="75"/>
+      <c r="C108" s="75"/>
+      <c r="D108" s="75"/>
       <c r="F108" s="30" t="s">
         <v>89</v>
       </c>
@@ -8042,12 +8026,12 @@
       <c r="B115" s="13"/>
     </row>
     <row r="116" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A116" s="77" t="s">
+      <c r="A116" s="75" t="s">
         <v>370</v>
       </c>
-      <c r="B116" s="77"/>
-      <c r="C116" s="77"/>
-      <c r="D116" s="77"/>
+      <c r="B116" s="75"/>
+      <c r="C116" s="75"/>
+      <c r="D116" s="75"/>
       <c r="F116" s="30" t="s">
         <v>89</v>
       </c>
@@ -8084,7 +8068,7 @@
         <v>161</v>
       </c>
       <c r="D118" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F118" s="22"/>
       <c r="G118" s="15"/>
@@ -8099,7 +8083,7 @@
         <v>162</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F119" s="22"/>
       <c r="G119" s="15"/>
@@ -8243,12 +8227,12 @@
       <c r="I130" s="15"/>
     </row>
     <row r="131" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A131" s="77" t="s">
-        <v>415</v>
-      </c>
-      <c r="B131" s="77"/>
-      <c r="C131" s="77"/>
-      <c r="D131" s="77"/>
+      <c r="A131" s="75" t="s">
+        <v>411</v>
+      </c>
+      <c r="B131" s="75"/>
+      <c r="C131" s="75"/>
+      <c r="D131" s="75"/>
       <c r="F131" s="30" t="s">
         <v>89</v>
       </c>
@@ -8263,12 +8247,12 @@
       </c>
     </row>
     <row r="132" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A132" s="77" t="s">
-        <v>464</v>
-      </c>
-      <c r="B132" s="77"/>
-      <c r="C132" s="77"/>
-      <c r="D132" s="77"/>
+      <c r="A132" s="75" t="s">
+        <v>460</v>
+      </c>
+      <c r="B132" s="75"/>
+      <c r="C132" s="75"/>
+      <c r="D132" s="75"/>
       <c r="F132" s="30" t="s">
         <v>89</v>
       </c>
@@ -8290,7 +8274,7 @@
         <v>212</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F133" s="22"/>
       <c r="G133" s="15"/>
@@ -8432,17 +8416,17 @@
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B145" s="13"/>
       <c r="F145" s="22"/>
-      <c r="G145" s="41"/>
-      <c r="H145" s="41"/>
-      <c r="I145" s="41"/>
+      <c r="G145" s="40"/>
+      <c r="H145" s="40"/>
+      <c r="I145" s="40"/>
     </row>
     <row r="146" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A146" s="77" t="s">
-        <v>433</v>
-      </c>
-      <c r="B146" s="77"/>
-      <c r="C146" s="77"/>
-      <c r="D146" s="77"/>
+      <c r="A146" s="75" t="s">
+        <v>429</v>
+      </c>
+      <c r="B146" s="75"/>
+      <c r="C146" s="75"/>
+      <c r="D146" s="75"/>
       <c r="F146" s="30" t="s">
         <v>89</v>
       </c>
@@ -8457,12 +8441,12 @@
       </c>
     </row>
     <row r="147" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A147" s="77" t="s">
-        <v>434</v>
-      </c>
-      <c r="B147" s="77"/>
-      <c r="C147" s="77"/>
-      <c r="D147" s="77"/>
+      <c r="A147" s="75" t="s">
+        <v>430</v>
+      </c>
+      <c r="B147" s="75"/>
+      <c r="C147" s="75"/>
+      <c r="D147" s="75"/>
       <c r="F147" s="30" t="s">
         <v>89</v>
       </c>
@@ -8484,9 +8468,9 @@
         <v>202</v>
       </c>
       <c r="F148" s="22"/>
-      <c r="G148" s="41"/>
+      <c r="G148" s="40"/>
       <c r="H148" s="22"/>
-      <c r="I148" s="41"/>
+      <c r="I148" s="40"/>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
@@ -8496,20 +8480,20 @@
         <v>203</v>
       </c>
       <c r="F149" s="22"/>
-      <c r="G149" s="41"/>
+      <c r="G149" s="40"/>
       <c r="H149" s="22"/>
-      <c r="I149" s="41"/>
+      <c r="I149" s="40"/>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B150" s="13"/>
     </row>
     <row r="151" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A151" s="77" t="s">
-        <v>418</v>
-      </c>
-      <c r="B151" s="77"/>
-      <c r="C151" s="77"/>
-      <c r="D151" s="77"/>
+      <c r="A151" s="75" t="s">
+        <v>414</v>
+      </c>
+      <c r="B151" s="75"/>
+      <c r="C151" s="75"/>
+      <c r="D151" s="75"/>
       <c r="F151" s="30" t="s">
         <v>89</v>
       </c>
@@ -8528,15 +8512,15 @@
         <v>26</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="D152" s="4" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F152" s="22"/>
-      <c r="G152" s="41"/>
-      <c r="H152" s="41"/>
-      <c r="I152" s="41"/>
+      <c r="G152" s="40"/>
+      <c r="H152" s="40"/>
+      <c r="I152" s="40"/>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B153" s="13" t="s">
@@ -8546,200 +8530,207 @@
         <v>215</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F153" s="22"/>
-      <c r="G153" s="41"/>
-      <c r="H153" s="41"/>
-      <c r="I153" s="41"/>
+      <c r="G153" s="40"/>
+      <c r="H153" s="40"/>
+      <c r="I153" s="40"/>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B154" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F154" s="22"/>
-      <c r="G154" s="41"/>
-      <c r="H154" s="41"/>
-      <c r="I154" s="41"/>
+      <c r="G154" s="40"/>
+      <c r="H154" s="40"/>
+      <c r="I154" s="40"/>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B155" s="13"/>
       <c r="F155" s="22"/>
-      <c r="G155" s="41"/>
-      <c r="H155" s="41"/>
-      <c r="I155" s="41"/>
+      <c r="G155" s="40"/>
+      <c r="H155" s="40"/>
+      <c r="I155" s="40"/>
     </row>
     <row r="156" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A156" s="77" t="s">
-        <v>365</v>
-      </c>
-      <c r="B156" s="77"/>
-      <c r="C156" s="77"/>
-      <c r="D156" s="77"/>
+      <c r="A156" s="75" t="s">
+        <v>408</v>
+      </c>
+      <c r="B156" s="75"/>
+      <c r="C156" s="75"/>
+      <c r="D156" s="75"/>
       <c r="F156" s="30" t="s">
         <v>89</v>
       </c>
       <c r="G156" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="H156" s="30" t="s">
-        <v>89</v>
+      <c r="H156" s="32" t="s">
+        <v>88</v>
       </c>
       <c r="I156" s="32" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A157" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C157" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="D157" s="4" t="s">
-        <v>377</v>
+      <c r="A157" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B157" s="13"/>
+      <c r="C157" s="1" t="s">
+        <v>409</v>
       </c>
       <c r="F157" s="22"/>
-      <c r="G157" s="39"/>
-      <c r="H157" s="22"/>
-      <c r="I157" s="39"/>
+      <c r="G157" s="40"/>
+      <c r="H157" s="40"/>
+      <c r="I157" s="40"/>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A158" s="13" t="s">
-        <v>26</v>
-      </c>
+      <c r="A158" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B158" s="13"/>
       <c r="C158" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="D158" s="4" t="s">
-        <v>378</v>
+        <v>410</v>
       </c>
       <c r="F158" s="22"/>
-      <c r="G158" s="39"/>
-      <c r="H158" s="22"/>
-      <c r="I158" s="39"/>
+      <c r="G158" s="40"/>
+      <c r="H158" s="40"/>
+      <c r="I158" s="40"/>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A159" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C159" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D159" s="4" t="s">
-        <v>379</v>
-      </c>
+      <c r="B159" s="13"/>
       <c r="F159" s="22"/>
-      <c r="G159" s="39"/>
-      <c r="H159" s="22"/>
-      <c r="I159" s="39"/>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A160" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F160" s="22"/>
-      <c r="G160" s="39"/>
-      <c r="H160" s="22"/>
-      <c r="I160" s="39"/>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B161" s="13"/>
+      <c r="G159" s="15"/>
+      <c r="H159" s="15"/>
+      <c r="I159" s="15"/>
+    </row>
+    <row r="160" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A160" s="75" t="s">
+        <v>440</v>
+      </c>
+      <c r="B160" s="75"/>
+      <c r="C160" s="75"/>
+      <c r="D160" s="75"/>
+      <c r="F160" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G160" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H160" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I160" s="32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A161" s="75" t="s">
+        <v>441</v>
+      </c>
+      <c r="B161" s="75"/>
+      <c r="C161" s="75"/>
+      <c r="D161" s="75"/>
+      <c r="F161" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G161" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H161" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I161" s="32" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="162" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A162" s="77" t="s">
-        <v>412</v>
-      </c>
-      <c r="B162" s="77"/>
-      <c r="C162" s="77"/>
-      <c r="D162" s="77"/>
+      <c r="A162" s="75" t="s">
+        <v>456</v>
+      </c>
+      <c r="B162" s="75"/>
+      <c r="C162" s="75"/>
+      <c r="D162" s="75"/>
       <c r="F162" s="30" t="s">
         <v>89</v>
       </c>
       <c r="G162" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="H162" s="32" t="s">
-        <v>88</v>
+      <c r="H162" s="30" t="s">
+        <v>89</v>
       </c>
       <c r="I162" s="32" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A163" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B163" s="13"/>
-      <c r="C163" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="F163" s="22"/>
-      <c r="G163" s="41"/>
-      <c r="H163" s="41"/>
-      <c r="I163" s="41"/>
+    <row r="163" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A163" s="75" t="s">
+        <v>455</v>
+      </c>
+      <c r="B163" s="75"/>
+      <c r="C163" s="75"/>
+      <c r="D163" s="75"/>
+      <c r="F163" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G163" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H163" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I163" s="32" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B164" s="13"/>
-      <c r="C164" s="1" t="s">
-        <v>414</v>
+      <c r="A164" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C164" s="18" t="s">
+        <v>202</v>
       </c>
       <c r="F164" s="22"/>
-      <c r="G164" s="41"/>
-      <c r="H164" s="41"/>
-      <c r="I164" s="41"/>
+      <c r="G164" s="15"/>
+      <c r="H164" s="22"/>
+      <c r="I164" s="15"/>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B165" s="13"/>
+      <c r="A165" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="F165" s="22"/>
       <c r="G165" s="15"/>
-      <c r="H165" s="15"/>
+      <c r="H165" s="22"/>
       <c r="I165" s="15"/>
     </row>
-    <row r="166" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A166" s="77" t="s">
-        <v>444</v>
-      </c>
-      <c r="B166" s="77"/>
-      <c r="C166" s="77"/>
-      <c r="D166" s="77"/>
-      <c r="F166" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G166" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H166" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I166" s="32" t="s">
-        <v>88</v>
-      </c>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B166" s="13"/>
     </row>
     <row r="167" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A167" s="77" t="s">
-        <v>445</v>
-      </c>
-      <c r="B167" s="77"/>
-      <c r="C167" s="77"/>
-      <c r="D167" s="77"/>
+      <c r="A167" s="75" t="s">
+        <v>371</v>
+      </c>
+      <c r="B167" s="75"/>
+      <c r="C167" s="75"/>
+      <c r="D167" s="75"/>
       <c r="F167" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="G167" s="32" t="s">
-        <v>88</v>
+      <c r="G167" s="30" t="s">
+        <v>89</v>
       </c>
       <c r="H167" s="30" t="s">
         <v>89</v>
@@ -8748,52 +8739,45 @@
         <v>88</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A168" s="77" t="s">
-        <v>460</v>
-      </c>
-      <c r="B168" s="77"/>
-      <c r="C168" s="77"/>
-      <c r="D168" s="77"/>
-      <c r="F168" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G168" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H168" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I168" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A169" s="77" t="s">
-        <v>459</v>
-      </c>
-      <c r="B169" s="77"/>
-      <c r="C169" s="77"/>
-      <c r="D169" s="77"/>
-      <c r="F169" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G169" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H169" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I169" s="32" t="s">
-        <v>88</v>
-      </c>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B168" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C168" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F168" s="22"/>
+      <c r="G168" s="15"/>
+      <c r="H168" s="22"/>
+      <c r="I168" s="15"/>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B169" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="F169" s="22"/>
+      <c r="G169" s="15"/>
+      <c r="H169" s="22"/>
+      <c r="I169" s="15"/>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A170" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C170" s="18" t="s">
-        <v>202</v>
+      <c r="B170" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="F170" s="22"/>
       <c r="G170" s="15"/>
@@ -8801,11 +8785,14 @@
       <c r="I170" s="15"/>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A171" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C171" s="1" t="s">
-        <v>203</v>
+      <c r="B171" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C171" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>135</v>
       </c>
       <c r="F171" s="22"/>
       <c r="G171" s="15"/>
@@ -8813,52 +8800,49 @@
       <c r="I171" s="15"/>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B172" s="13"/>
-    </row>
-    <row r="173" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A173" s="77" t="s">
-        <v>371</v>
-      </c>
-      <c r="B173" s="77"/>
-      <c r="C173" s="77"/>
-      <c r="D173" s="77"/>
-      <c r="F173" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G173" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H173" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I173" s="32" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B174" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C174" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="D174" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="F174" s="22"/>
-      <c r="G174" s="15"/>
-      <c r="H174" s="22"/>
-      <c r="I174" s="15"/>
+      <c r="B172" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F172" s="22"/>
+      <c r="G172" s="15"/>
+      <c r="H172" s="22"/>
+      <c r="I172" s="15"/>
+    </row>
+    <row r="174" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A174" s="75" t="s">
+        <v>372</v>
+      </c>
+      <c r="B174" s="75"/>
+      <c r="C174" s="75"/>
+      <c r="D174" s="75"/>
+      <c r="F174" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G174" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H174" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I174" s="32" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B175" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C175" s="1" t="s">
-        <v>132</v>
+      <c r="C175" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>499</v>
+        <v>144</v>
       </c>
       <c r="F175" s="22"/>
       <c r="G175" s="15"/>
@@ -8870,10 +8854,10 @@
         <v>26</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="F176" s="22"/>
       <c r="G176" s="15"/>
@@ -8884,11 +8868,11 @@
       <c r="B177" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C177" s="18" t="s">
-        <v>134</v>
+      <c r="C177" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="F177" s="22"/>
       <c r="G177" s="15"/>
@@ -8896,172 +8880,173 @@
       <c r="I177" s="15"/>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B178" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C178" s="1" t="s">
-        <v>336</v>
+      <c r="B178" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C178" s="18" t="s">
+        <v>142</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="F178" s="22"/>
       <c r="G178" s="15"/>
       <c r="H178" s="22"/>
       <c r="I178" s="15"/>
     </row>
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B179" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="F179" s="22"/>
+      <c r="G179" s="15"/>
+      <c r="H179" s="22"/>
+      <c r="I179" s="15"/>
+    </row>
     <row r="180" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A180" s="77" t="s">
-        <v>372</v>
-      </c>
-      <c r="B180" s="77"/>
-      <c r="C180" s="77"/>
-      <c r="D180" s="77"/>
-      <c r="F180" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G180" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H180" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I180" s="32" t="s">
-        <v>88</v>
+      <c r="C180" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D180" s="4" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B181" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C181" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D181" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F181" s="22"/>
-      <c r="G181" s="15"/>
-      <c r="H181" s="22"/>
-      <c r="I181" s="15"/>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B182" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C182" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D182" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="F182" s="22"/>
-      <c r="G182" s="15"/>
-      <c r="H182" s="22"/>
-      <c r="I182" s="15"/>
+      <c r="B181" s="13"/>
+    </row>
+    <row r="182" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A182" s="75" t="s">
+        <v>373</v>
+      </c>
+      <c r="B182" s="75"/>
+      <c r="C182" s="75"/>
+      <c r="D182" s="75"/>
+      <c r="F182" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G182" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H182" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I182" s="31" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A183" s="13"/>
       <c r="B183" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C183" s="1" t="s">
-        <v>141</v>
+      <c r="C183" s="18" t="s">
+        <v>122</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="F183" s="22"/>
       <c r="G183" s="15"/>
-      <c r="H183" s="22"/>
-      <c r="I183" s="15"/>
+      <c r="H183" s="15"/>
+      <c r="I183" s="25"/>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A184" s="13"/>
       <c r="B184" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C184" s="18" t="s">
-        <v>142</v>
+      <c r="C184" s="1" t="s">
+        <v>124</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>147</v>
+        <v>193</v>
       </c>
       <c r="F184" s="22"/>
       <c r="G184" s="15"/>
-      <c r="H184" s="22"/>
-      <c r="I184" s="15"/>
+      <c r="H184" s="15"/>
+      <c r="I184" s="25"/>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B185" s="6" t="s">
+      <c r="B185" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>500</v>
+        <v>194</v>
       </c>
       <c r="F185" s="22"/>
       <c r="G185" s="15"/>
-      <c r="H185" s="22"/>
-      <c r="I185" s="15"/>
-    </row>
-    <row r="186" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C186" s="21" t="s">
-        <v>148</v>
+      <c r="H185" s="15"/>
+      <c r="I185" s="25"/>
+    </row>
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B186" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C186" s="18" t="s">
+        <v>123</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>501</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="F186" s="22"/>
+      <c r="G186" s="15"/>
+      <c r="H186" s="15"/>
+      <c r="I186" s="25"/>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B187" s="13"/>
-    </row>
-    <row r="188" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A188" s="77" t="s">
-        <v>373</v>
-      </c>
-      <c r="B188" s="77"/>
-      <c r="C188" s="77"/>
-      <c r="D188" s="77"/>
-      <c r="F188" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G188" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H188" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="I188" s="31" t="s">
+      <c r="B187" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C187" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D187" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="F187" s="22"/>
+      <c r="G187" s="15"/>
+      <c r="H187" s="15"/>
+      <c r="I187" s="25"/>
+    </row>
+    <row r="189" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A189" s="75" t="s">
+        <v>374</v>
+      </c>
+      <c r="B189" s="75"/>
+      <c r="C189" s="75"/>
+      <c r="D189" s="75"/>
+      <c r="F189" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G189" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="H189" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="I189" s="31" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A189" s="13"/>
-      <c r="B189" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C189" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="D189" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F189" s="22"/>
-      <c r="G189" s="15"/>
-      <c r="H189" s="15"/>
-      <c r="I189" s="25"/>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="13"/>
       <c r="B190" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C190" s="1" t="s">
-        <v>124</v>
+      <c r="C190" s="18" t="s">
+        <v>164</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="F190" s="22"/>
       <c r="G190" s="15"/>
@@ -9069,14 +9054,15 @@
       <c r="I190" s="25"/>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A191" s="13"/>
       <c r="B191" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F191" s="22"/>
       <c r="G191" s="15"/>
@@ -9087,11 +9073,11 @@
       <c r="B192" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C192" s="18" t="s">
-        <v>123</v>
+      <c r="C192" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="D192" s="4" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F192" s="22"/>
       <c r="G192" s="15"/>
@@ -9103,238 +9089,154 @@
         <v>26</v>
       </c>
       <c r="C193" s="18" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D193" s="4" t="s">
-        <v>502</v>
+        <v>190</v>
       </c>
       <c r="F193" s="22"/>
       <c r="G193" s="15"/>
       <c r="H193" s="15"/>
       <c r="I193" s="25"/>
     </row>
-    <row r="195" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A195" s="77" t="s">
-        <v>374</v>
-      </c>
-      <c r="B195" s="77"/>
-      <c r="C195" s="77"/>
-      <c r="D195" s="77"/>
-      <c r="F195" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G195" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="H195" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="I195" s="31" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A196" s="13"/>
-      <c r="B196" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C196" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="D196" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="F196" s="22"/>
-      <c r="G196" s="15"/>
-      <c r="H196" s="15"/>
-      <c r="I196" s="25"/>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A197" s="13"/>
-      <c r="B197" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C197" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D197" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="F197" s="22"/>
-      <c r="G197" s="15"/>
-      <c r="H197" s="15"/>
-      <c r="I197" s="25"/>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B194" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C194" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F194" s="22"/>
+      <c r="G194" s="15"/>
+      <c r="H194" s="15"/>
+      <c r="I194" s="25"/>
+    </row>
+    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B195" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F195" s="22"/>
+      <c r="G195" s="15"/>
+      <c r="H195" s="15"/>
+      <c r="I195" s="25"/>
+    </row>
+    <row r="197" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A197" s="75" t="s">
+        <v>375</v>
+      </c>
+      <c r="B197" s="75"/>
+      <c r="C197" s="75"/>
+      <c r="D197" s="75"/>
+      <c r="F197" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G197" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H197" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="I197" s="30" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A198" s="13"/>
       <c r="B198" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C198" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D198" s="4" t="s">
-        <v>189</v>
+      <c r="C198" s="18" t="s">
+        <v>290</v>
       </c>
       <c r="F198" s="22"/>
-      <c r="G198" s="15"/>
-      <c r="H198" s="15"/>
-      <c r="I198" s="25"/>
+      <c r="G198" s="22"/>
+      <c r="H198" s="22"/>
+      <c r="I198" s="22"/>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A199" s="13"/>
       <c r="B199" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C199" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="D199" s="4" t="s">
-        <v>190</v>
+        <v>291</v>
       </c>
       <c r="F199" s="22"/>
-      <c r="G199" s="15"/>
-      <c r="H199" s="15"/>
-      <c r="I199" s="25"/>
+      <c r="G199" s="22"/>
+      <c r="H199" s="22"/>
+      <c r="I199" s="22"/>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B200" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C200" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="D200" s="4" t="s">
-        <v>191</v>
+        <v>292</v>
       </c>
       <c r="F200" s="22"/>
-      <c r="G200" s="15"/>
-      <c r="H200" s="15"/>
-      <c r="I200" s="25"/>
+      <c r="G200" s="22"/>
+      <c r="H200" s="22"/>
+      <c r="I200" s="22"/>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B201" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C201" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D201" s="4" t="s">
-        <v>186</v>
+      <c r="C201" s="18" t="s">
+        <v>293</v>
       </c>
       <c r="F201" s="22"/>
-      <c r="G201" s="15"/>
-      <c r="H201" s="15"/>
-      <c r="I201" s="25"/>
-    </row>
-    <row r="203" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A203" s="77" t="s">
-        <v>375</v>
-      </c>
-      <c r="B203" s="77"/>
-      <c r="C203" s="77"/>
-      <c r="D203" s="77"/>
-      <c r="F203" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G203" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="H203" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="I203" s="30" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A204" s="13"/>
-      <c r="B204" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C204" s="18" t="s">
-        <v>290</v>
-      </c>
-      <c r="F204" s="22"/>
-      <c r="G204" s="22"/>
-      <c r="H204" s="22"/>
-      <c r="I204" s="22"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A205" s="13"/>
-      <c r="B205" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C205" s="18" t="s">
-        <v>291</v>
-      </c>
-      <c r="F205" s="22"/>
-      <c r="G205" s="22"/>
-      <c r="H205" s="22"/>
-      <c r="I205" s="22"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B206" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C206" s="18" t="s">
-        <v>292</v>
-      </c>
-      <c r="F206" s="22"/>
-      <c r="G206" s="22"/>
-      <c r="H206" s="22"/>
-      <c r="I206" s="22"/>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B207" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C207" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="F207" s="22"/>
-      <c r="G207" s="22"/>
-      <c r="H207" s="22"/>
-      <c r="I207" s="22"/>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B208" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C208" s="18" t="s">
+      <c r="G201" s="22"/>
+      <c r="H201" s="22"/>
+      <c r="I201" s="22"/>
+    </row>
+    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B202" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C202" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="F208" s="22"/>
-      <c r="G208" s="22"/>
-      <c r="H208" s="22"/>
-      <c r="I208" s="22"/>
-    </row>
-    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C209" s="18"/>
-    </row>
-    <row r="210" spans="3:3" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.3"/>
+      <c r="F202" s="22"/>
+      <c r="G202" s="22"/>
+      <c r="H202" s="22"/>
+      <c r="I202" s="22"/>
+    </row>
+    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C203" s="18"/>
+    </row>
+    <row r="204" spans="1:9" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="A203:D203"/>
-    <mergeCell ref="A156:D156"/>
-    <mergeCell ref="A169:D169"/>
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="A180:D180"/>
-    <mergeCell ref="A188:D188"/>
-    <mergeCell ref="A195:D195"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="A166:D166"/>
-    <mergeCell ref="A167:D167"/>
-    <mergeCell ref="A168:D168"/>
-    <mergeCell ref="A162:D162"/>
-    <mergeCell ref="A151:D151"/>
-    <mergeCell ref="A146:D146"/>
-    <mergeCell ref="A147:D147"/>
-    <mergeCell ref="A132:D132"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A108:D108"/>
+  <mergeCells count="57">
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A70:D70"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A9:D9"/>
     <mergeCell ref="F89:I89"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A19:D19"/>
@@ -9351,26 +9253,27 @@
     <mergeCell ref="A50:D50"/>
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="A52:D52"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A65:D65"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A70:D70"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A131:D131"/>
+    <mergeCell ref="A160:D160"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="A162:D162"/>
+    <mergeCell ref="A156:D156"/>
+    <mergeCell ref="A151:D151"/>
+    <mergeCell ref="A146:D146"/>
+    <mergeCell ref="A147:D147"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A197:D197"/>
+    <mergeCell ref="A163:D163"/>
+    <mergeCell ref="A167:D167"/>
+    <mergeCell ref="A174:D174"/>
+    <mergeCell ref="A182:D182"/>
+    <mergeCell ref="A189:D189"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
SAP Guide - Pre Editorial Review
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="-3540" windowWidth="10065" windowHeight="12525" activeTab="4"/>
+    <workbookView xWindow="12510" yWindow="-3540" windowWidth="10065" windowHeight="12525" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATION" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2045" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="643">
   <si>
     <t>SSP</t>
   </si>
@@ -2282,6 +2282,30 @@
   </si>
   <si>
     <t>This identifies CSP points of contact who should receive the assessment results.</t>
+  </si>
+  <si>
+    <t>Signed SAP</t>
+  </si>
+  <si>
+    <t>Signed SAR</t>
+  </si>
+  <si>
+    <t>signed-sap</t>
+  </si>
+  <si>
+    <t>signed-sar</t>
+  </si>
+  <si>
+    <t>penetration-test-plan</t>
+  </si>
+  <si>
+    <t>Pentration Test Plan</t>
+  </si>
+  <si>
+    <t>Pentration Test Report</t>
+  </si>
+  <si>
+    <t>penetration-test-report</t>
   </si>
 </sst>
 </file>
@@ -2842,7 +2866,7 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -3073,6 +3097,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3112,12 +3139,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="AUTHOR-NOTE" xfId="5"/>
@@ -3478,12 +3506,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="100" t="s">
         <v>397</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
       <c r="H1" s="55" t="s">
         <v>395</v>
       </c>
@@ -3499,18 +3527,18 @@
       <c r="B3" s="57"/>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="103" t="s">
         <v>406</v>
       </c>
-      <c r="B4" s="102"/>
+      <c r="B4" s="103"/>
       <c r="C4" s="59"/>
       <c r="D4" s="59"/>
     </row>
     <row r="5" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="104" t="s">
         <v>420</v>
       </c>
-      <c r="B5" s="103"/>
+      <c r="B5" s="104"/>
       <c r="C5" s="59"/>
     </row>
     <row r="6" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -3523,19 +3551,19 @@
       <c r="E6" s="60"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="104" t="s">
         <v>418</v>
       </c>
-      <c r="B7" s="101"/>
+      <c r="B7" s="102"/>
       <c r="C7" s="62"/>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
     </row>
     <row r="8" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="100" t="s">
+      <c r="A8" s="101" t="s">
         <v>419</v>
       </c>
-      <c r="B8" s="101"/>
+      <c r="B8" s="102"/>
     </row>
     <row r="9" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
@@ -3547,45 +3575,45 @@
       <c r="E9" s="60"/>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="103" t="s">
+      <c r="A10" s="104" t="s">
         <v>400</v>
       </c>
-      <c r="B10" s="101"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="62"/>
       <c r="D10" s="62"/>
       <c r="E10" s="62"/>
     </row>
     <row r="11" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="100" t="s">
+      <c r="A11" s="101" t="s">
         <v>405</v>
       </c>
-      <c r="B11" s="101"/>
+      <c r="B11" s="102"/>
     </row>
     <row r="12" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="104" t="s">
         <v>401</v>
       </c>
-      <c r="B12" s="103"/>
+      <c r="B12" s="104"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="101" t="s">
+      <c r="A13" s="102" t="s">
         <v>403</v>
       </c>
-      <c r="B13" s="101"/>
+      <c r="B13" s="102"/>
     </row>
     <row r="14" spans="1:8" ht="43.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="A14" s="101" t="s">
         <v>402</v>
       </c>
-      <c r="B14" s="101"/>
+      <c r="B14" s="102"/>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="96" t="s">
+      <c r="A15" s="97" t="s">
         <v>421</v>
       </c>
-      <c r="B15" s="97"/>
-      <c r="C15" s="97"/>
-      <c r="D15" s="98"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="99"/>
     </row>
     <row r="16" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="75" t="s">
@@ -3729,35 +3757,35 @@
       <c r="C1" s="6"/>
       <c r="D1"/>
       <c r="E1" s="6"/>
-      <c r="H1" s="105"/>
-      <c r="I1" s="105"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
       <c r="J1" s="91" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
       <c r="G2" s="64" t="s">
         <v>430</v>
       </c>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="106"/>
       <c r="J2" t="s">
         <v>468</v>
       </c>
-      <c r="K2" s="104" t="s">
+      <c r="K2" s="105" t="s">
         <v>386</v>
       </c>
-      <c r="L2" s="104" t="s">
+      <c r="L2" s="105" t="s">
         <v>316</v>
       </c>
-      <c r="M2" s="104" t="s">
+      <c r="M2" s="105" t="s">
         <v>589</v>
       </c>
     </row>
@@ -3789,9 +3817,9 @@
       <c r="J3" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
+      <c r="M3" s="105"/>
       <c r="N3" s="53" t="s">
         <v>8</v>
       </c>
@@ -5749,27 +5777,27 @@
       <c r="I1" s="95"/>
     </row>
     <row r="2" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
       <c r="G2" s="64" t="s">
         <v>431</v>
       </c>
-      <c r="H2" s="107" t="s">
+      <c r="H2" s="108" t="s">
         <v>501</v>
       </c>
-      <c r="I2" s="107"/>
+      <c r="I2" s="108"/>
       <c r="J2" t="s">
         <v>468</v>
       </c>
-      <c r="K2" s="104" t="s">
+      <c r="K2" s="105" t="s">
         <v>386</v>
       </c>
-      <c r="L2" s="104" t="s">
+      <c r="L2" s="105" t="s">
         <v>316</v>
       </c>
     </row>
@@ -5801,8 +5829,8 @@
       <c r="J3" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
+      <c r="K3" s="105"/>
+      <c r="L3" s="105"/>
       <c r="M3" s="53" t="s">
         <v>8</v>
       </c>
@@ -7017,13 +7045,13 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H41" sqref="H41"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7046,7 +7074,7 @@
       <c r="D1"/>
       <c r="E1" s="6"/>
       <c r="H1" s="80"/>
-      <c r="I1" s="105" t="str">
+      <c r="I1" s="106" t="str">
         <f>CONCATENATE("All FedRAMP Compliance tags must use name='", tagname, "', as well as ns='https://fedramp.gov/ns/oscal'")</f>
         <v>All FedRAMP Compliance tags must use name='conformity', as well as ns='https://fedramp.gov/ns/oscal'</v>
       </c>
@@ -7055,18 +7083,18 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
       <c r="G2" s="64" t="s">
         <v>430</v>
       </c>
       <c r="H2" s="80"/>
-      <c r="I2" s="105"/>
+      <c r="I2" s="106"/>
       <c r="J2" t="s">
         <v>468</v>
       </c>
@@ -7185,7 +7213,7 @@
         <f>CONCATENATE(I7,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H7,"']/..")</f>
         <v>/*/metadata/location/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='primary-data-center']/..</v>
       </c>
-      <c r="K7" s="108" t="s">
+      <c r="K7" s="109" t="s">
         <v>566</v>
       </c>
       <c r="L7" s="83" t="str">
@@ -7222,7 +7250,7 @@
         <f>CONCATENATE(I8,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H8,"']/..")</f>
         <v>/*/metadata/location/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='alternate-data-center']/..</v>
       </c>
-      <c r="K8" s="108"/>
+      <c r="K8" s="109"/>
       <c r="L8" s="83" t="str">
         <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H8,"&lt;/prop&gt;")</f>
         <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;alternate-data-center&lt;/prop&gt;</v>
@@ -7897,130 +7925,266 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="H30" s="84"/>
-      <c r="I30" s="79"/>
-      <c r="J30" s="79"/>
-    </row>
-    <row r="31" spans="1:12" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="88"/>
-      <c r="F31" s="90"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="H32" s="86" t="s">
+      <c r="A30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="54" t="s">
+        <v>635</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="I30" s="79" t="s">
+        <v>550</v>
+      </c>
+      <c r="J30" s="96" t="str">
+        <f t="shared" ref="J30" si="3">CONCATENATE(I30,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H30,"']/..")</f>
+        <v>/*/back-matter/resource/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='signed-sap']/..</v>
+      </c>
+      <c r="L30" s="96" t="str">
+        <f t="shared" ref="L30" si="4">CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H30,"&lt;/prop&gt;")</f>
+        <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;signed-sap&lt;/prop&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="54" t="s">
+        <v>636</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="I31" s="79" t="s">
+        <v>550</v>
+      </c>
+      <c r="J31" s="96" t="str">
+        <f t="shared" ref="J31" si="5">CONCATENATE(I31,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H31,"']/..")</f>
+        <v>/*/back-matter/resource/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='signed-sar']/..</v>
+      </c>
+      <c r="L31" s="96" t="str">
+        <f t="shared" ref="L31" si="6">CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H31,"&lt;/prop&gt;")</f>
+        <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;signed-sar&lt;/prop&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="54" t="s">
+        <v>640</v>
+      </c>
+      <c r="H32" s="112" t="s">
+        <v>639</v>
+      </c>
+      <c r="I32" s="79" t="s">
+        <v>550</v>
+      </c>
+      <c r="J32" s="96" t="str">
+        <f t="shared" ref="J32" si="7">CONCATENATE(I32,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H32,"']/..")</f>
+        <v>/*/back-matter/resource/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='penetration-test-plan']/..</v>
+      </c>
+      <c r="L32" s="96" t="str">
+        <f t="shared" ref="L32" si="8">CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H32,"&lt;/prop&gt;")</f>
+        <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;penetration-test-plan&lt;/prop&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="54" t="s">
+        <v>641</v>
+      </c>
+      <c r="H33" s="112" t="s">
+        <v>642</v>
+      </c>
+      <c r="I33" s="79" t="s">
+        <v>550</v>
+      </c>
+      <c r="J33" s="96" t="str">
+        <f t="shared" ref="J33" si="9">CONCATENATE(I33,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H33,"']/..")</f>
+        <v>/*/back-matter/resource/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='penetration-test-report']/..</v>
+      </c>
+      <c r="L33" s="96" t="str">
+        <f t="shared" ref="L33" si="10">CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H33,"&lt;/prop&gt;")</f>
+        <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;penetration-test-report&lt;/prop&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="79"/>
+    </row>
+    <row r="35" spans="1:12" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A35" s="88"/>
+      <c r="F35" s="90"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="H36" s="86" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="6">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
         <v>1</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B40" s="6">
         <v>1</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E40" s="6">
         <v>1</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G40" t="s">
         <v>551</v>
       </c>
-      <c r="H36" s="84" t="s">
+      <c r="H40" s="84" t="s">
         <v>202</v>
       </c>
-      <c r="I36" s="79" t="s">
+      <c r="I40" s="79" t="s">
         <v>504</v>
       </c>
-      <c r="J36" s="66" t="str">
-        <f>CONCATENATE(I36,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H36,"']/..")</f>
+      <c r="J40" s="66" t="str">
+        <f>CONCATENATE(I40,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H40,"']/..")</f>
         <v>/*/metadata/party/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='csp']/..</v>
       </c>
-      <c r="L36" s="83" t="str">
-        <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H36,"&lt;/prop&gt;")</f>
+      <c r="L40" s="83" t="str">
+        <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H40,"&lt;/prop&gt;")</f>
         <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;csp&lt;/prop&gt;</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="6">
+    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A41" s="6">
         <v>1</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B41" s="6">
         <v>1</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C41" s="6">
         <v>1</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D41" s="6">
         <v>1</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E41" s="6">
         <v>1</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G41" t="s">
         <v>428</v>
       </c>
-      <c r="H37" s="84" t="s">
+      <c r="H41" s="84" t="s">
         <v>203</v>
       </c>
-      <c r="I37" s="79" t="s">
+      <c r="I41" s="79" t="s">
         <v>504</v>
       </c>
-      <c r="J37" s="83" t="str">
-        <f>CONCATENATE(I37,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H37,"']/..")</f>
+      <c r="J41" s="83" t="str">
+        <f>CONCATENATE(I41,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H41,"']/..")</f>
         <v>/*/metadata/party/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='fedramp-pmo']/..</v>
       </c>
-      <c r="L37" s="83" t="str">
-        <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H37,"&lt;/prop&gt;")</f>
+      <c r="L41" s="83" t="str">
+        <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H41,"&lt;/prop&gt;")</f>
         <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;fedramp-pmo&lt;/prop&gt;</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="6">
+    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
         <v>1</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B42" s="6">
         <v>1</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C42" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D42" s="6">
         <v>1</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E42" s="6">
         <v>1</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G42" t="s">
         <v>552</v>
       </c>
-      <c r="H38" s="84" t="s">
+      <c r="H42" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="I38" s="79" t="s">
+      <c r="I42" s="79" t="s">
         <v>504</v>
       </c>
-      <c r="J38" s="83" t="str">
-        <f>CONCATENATE(I38,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H38,"']/..")</f>
+      <c r="J42" s="83" t="str">
+        <f>CONCATENATE(I42,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H42,"']/..")</f>
         <v>/*/metadata/party/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='fedramp-jab']/..</v>
       </c>
-      <c r="L38" s="83" t="str">
-        <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H38,"&lt;/prop&gt;")</f>
+      <c r="L42" s="83" t="str">
+        <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H42,"&lt;/prop&gt;")</f>
         <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;fedramp-jab&lt;/prop&gt;</v>
       </c>
     </row>
@@ -8040,7 +8204,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
@@ -8067,17 +8231,17 @@
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="G2" s="106" t="s">
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="G2" s="107" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="106"/>
+      <c r="H2" s="107"/>
       <c r="I2" s="28" t="s">
         <v>301</v>
       </c>
@@ -9290,17 +9454,17 @@
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="G2" s="106" t="s">
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="G2" s="107" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="106"/>
+      <c r="H2" s="107"/>
       <c r="I2" s="28" t="s">
         <v>230</v>
       </c>
@@ -9350,12 +9514,12 @@
       <c r="E4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="109" t="s">
+      <c r="G4" s="111" t="s">
         <v>322</v>
       </c>
-      <c r="H4" s="109"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="109"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="111"/>
+      <c r="J4" s="111"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
@@ -9373,12 +9537,12 @@
       <c r="E5" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="109" t="s">
+      <c r="G5" s="111" t="s">
         <v>321</v>
       </c>
-      <c r="H5" s="109"/>
-      <c r="I5" s="109"/>
-      <c r="J5" s="109"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="111"/>
+      <c r="J5" s="111"/>
     </row>
     <row r="6" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
@@ -9439,12 +9603,12 @@
       <c r="E9" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="109" t="s">
+      <c r="G9" s="111" t="s">
         <v>328</v>
       </c>
-      <c r="H9" s="109"/>
-      <c r="I9" s="109"/>
-      <c r="J9" s="109"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
+      <c r="J9" s="111"/>
     </row>
     <row r="10" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
@@ -9462,12 +9626,12 @@
       <c r="E10" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="109" t="s">
+      <c r="G10" s="111" t="s">
         <v>327</v>
       </c>
-      <c r="H10" s="109"/>
-      <c r="I10" s="109"/>
-      <c r="J10" s="109"/>
+      <c r="H10" s="111"/>
+      <c r="I10" s="111"/>
+      <c r="J10" s="111"/>
     </row>
     <row r="11" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
@@ -9544,12 +9708,12 @@
       <c r="E15" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="109" t="s">
+      <c r="G15" s="111" t="s">
         <v>264</v>
       </c>
-      <c r="H15" s="109"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="109"/>
+      <c r="H15" s="111"/>
+      <c r="I15" s="111"/>
+      <c r="J15" s="111"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
@@ -9610,12 +9774,12 @@
       <c r="E19" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="109" t="s">
+      <c r="G19" s="111" t="s">
         <v>265</v>
       </c>
-      <c r="H19" s="109"/>
-      <c r="I19" s="109"/>
-      <c r="J19" s="109"/>
+      <c r="H19" s="111"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
     </row>
     <row r="20" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
@@ -9633,12 +9797,12 @@
       <c r="E20" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="109" t="s">
+      <c r="G20" s="111" t="s">
         <v>266</v>
       </c>
-      <c r="H20" s="109"/>
-      <c r="I20" s="109"/>
-      <c r="J20" s="109"/>
+      <c r="H20" s="111"/>
+      <c r="I20" s="111"/>
+      <c r="J20" s="111"/>
     </row>
     <row r="21" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
@@ -9656,12 +9820,12 @@
       <c r="E21" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="109" t="s">
+      <c r="G21" s="111" t="s">
         <v>267</v>
       </c>
-      <c r="H21" s="109"/>
-      <c r="I21" s="109"/>
-      <c r="J21" s="109"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
     </row>
     <row r="22" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
@@ -9679,12 +9843,12 @@
       <c r="E22" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="109" t="s">
+      <c r="G22" s="111" t="s">
         <v>268</v>
       </c>
-      <c r="H22" s="109"/>
-      <c r="I22" s="109"/>
-      <c r="J22" s="109"/>
+      <c r="H22" s="111"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="111"/>
     </row>
     <row r="23" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
@@ -9761,12 +9925,12 @@
       <c r="E27" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="109" t="s">
+      <c r="G27" s="111" t="s">
         <v>269</v>
       </c>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="109"/>
+      <c r="H27" s="111"/>
+      <c r="I27" s="111"/>
+      <c r="J27" s="111"/>
     </row>
     <row r="28" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
@@ -9846,12 +10010,12 @@
       <c r="E32" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G32" s="109" t="s">
+      <c r="G32" s="111" t="s">
         <v>318</v>
       </c>
-      <c r="H32" s="109"/>
-      <c r="I32" s="109"/>
-      <c r="J32" s="109"/>
+      <c r="H32" s="111"/>
+      <c r="I32" s="111"/>
+      <c r="J32" s="111"/>
     </row>
     <row r="33" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
@@ -9944,12 +10108,12 @@
       <c r="E38" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G38" s="109" t="s">
+      <c r="G38" s="111" t="s">
         <v>270</v>
       </c>
-      <c r="H38" s="109"/>
-      <c r="I38" s="109"/>
-      <c r="J38" s="109"/>
+      <c r="H38" s="111"/>
+      <c r="I38" s="111"/>
+      <c r="J38" s="111"/>
     </row>
     <row r="39" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -10077,12 +10241,12 @@
       <c r="E46" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G46" s="109" t="s">
+      <c r="G46" s="111" t="s">
         <v>271</v>
       </c>
-      <c r="H46" s="109"/>
-      <c r="I46" s="109"/>
-      <c r="J46" s="109"/>
+      <c r="H46" s="111"/>
+      <c r="I46" s="111"/>
+      <c r="J46" s="111"/>
     </row>
     <row r="47" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
@@ -10100,12 +10264,12 @@
       <c r="E47" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G47" s="109" t="s">
+      <c r="G47" s="111" t="s">
         <v>272</v>
       </c>
-      <c r="H47" s="109"/>
-      <c r="I47" s="109"/>
-      <c r="J47" s="109"/>
+      <c r="H47" s="111"/>
+      <c r="I47" s="111"/>
+      <c r="J47" s="111"/>
     </row>
     <row r="48" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
@@ -10123,12 +10287,12 @@
       <c r="E48" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="109" t="s">
+      <c r="G48" s="111" t="s">
         <v>273</v>
       </c>
-      <c r="H48" s="109"/>
-      <c r="I48" s="109"/>
-      <c r="J48" s="109"/>
+      <c r="H48" s="111"/>
+      <c r="I48" s="111"/>
+      <c r="J48" s="111"/>
     </row>
     <row r="49" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
@@ -10146,12 +10310,12 @@
       <c r="E49" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G49" s="109" t="s">
+      <c r="G49" s="111" t="s">
         <v>274</v>
       </c>
-      <c r="H49" s="109"/>
-      <c r="I49" s="109"/>
-      <c r="J49" s="109"/>
+      <c r="H49" s="111"/>
+      <c r="I49" s="111"/>
+      <c r="J49" s="111"/>
     </row>
     <row r="50" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
@@ -10169,12 +10333,12 @@
       <c r="E50" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G50" s="109" t="s">
+      <c r="G50" s="111" t="s">
         <v>275</v>
       </c>
-      <c r="H50" s="109"/>
-      <c r="I50" s="109"/>
-      <c r="J50" s="109"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="111"/>
+      <c r="J50" s="111"/>
     </row>
     <row r="51" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
@@ -10192,12 +10356,12 @@
       <c r="E51" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G51" s="109" t="s">
+      <c r="G51" s="111" t="s">
         <v>276</v>
       </c>
-      <c r="H51" s="109"/>
-      <c r="I51" s="109"/>
-      <c r="J51" s="109"/>
+      <c r="H51" s="111"/>
+      <c r="I51" s="111"/>
+      <c r="J51" s="111"/>
     </row>
     <row r="52" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
@@ -10215,12 +10379,12 @@
       <c r="E52" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G52" s="109" t="s">
+      <c r="G52" s="111" t="s">
         <v>277</v>
       </c>
-      <c r="H52" s="109"/>
-      <c r="I52" s="109"/>
-      <c r="J52" s="109"/>
+      <c r="H52" s="111"/>
+      <c r="I52" s="111"/>
+      <c r="J52" s="111"/>
     </row>
     <row r="53" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
@@ -10238,12 +10402,12 @@
       <c r="E53" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G53" s="109" t="s">
+      <c r="G53" s="111" t="s">
         <v>278</v>
       </c>
-      <c r="H53" s="109"/>
-      <c r="I53" s="109"/>
-      <c r="J53" s="109"/>
+      <c r="H53" s="111"/>
+      <c r="I53" s="111"/>
+      <c r="J53" s="111"/>
     </row>
     <row r="54" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
@@ -10261,12 +10425,12 @@
       <c r="E54" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G54" s="109" t="s">
+      <c r="G54" s="111" t="s">
         <v>279</v>
       </c>
-      <c r="H54" s="109"/>
-      <c r="I54" s="109"/>
-      <c r="J54" s="109"/>
+      <c r="H54" s="111"/>
+      <c r="I54" s="111"/>
+      <c r="J54" s="111"/>
     </row>
     <row r="55" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
@@ -10340,12 +10504,12 @@
       <c r="E59" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G59" s="109" t="s">
+      <c r="G59" s="111" t="s">
         <v>280</v>
       </c>
-      <c r="H59" s="109"/>
-      <c r="I59" s="109"/>
-      <c r="J59" s="109"/>
+      <c r="H59" s="111"/>
+      <c r="I59" s="111"/>
+      <c r="J59" s="111"/>
     </row>
     <row r="60" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
@@ -10406,12 +10570,12 @@
       <c r="E63" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G63" s="109" t="s">
+      <c r="G63" s="111" t="s">
         <v>281</v>
       </c>
-      <c r="H63" s="109"/>
-      <c r="I63" s="109"/>
-      <c r="J63" s="109"/>
+      <c r="H63" s="111"/>
+      <c r="I63" s="111"/>
+      <c r="J63" s="111"/>
     </row>
     <row r="64" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A64" s="31" t="s">
@@ -10429,12 +10593,12 @@
       <c r="E64" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G64" s="109" t="s">
+      <c r="G64" s="111" t="s">
         <v>282</v>
       </c>
-      <c r="H64" s="109"/>
-      <c r="I64" s="109"/>
-      <c r="J64" s="109"/>
+      <c r="H64" s="111"/>
+      <c r="I64" s="111"/>
+      <c r="J64" s="111"/>
     </row>
     <row r="65" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65" s="31" t="s">
@@ -10452,12 +10616,12 @@
       <c r="E65" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G65" s="109" t="s">
+      <c r="G65" s="111" t="s">
         <v>283</v>
       </c>
-      <c r="H65" s="109"/>
-      <c r="I65" s="109"/>
-      <c r="J65" s="109"/>
+      <c r="H65" s="111"/>
+      <c r="I65" s="111"/>
+      <c r="J65" s="111"/>
     </row>
     <row r="66" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A66" s="31" t="s">
@@ -10475,12 +10639,12 @@
       <c r="E66" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G66" s="109" t="s">
+      <c r="G66" s="111" t="s">
         <v>284</v>
       </c>
-      <c r="H66" s="109"/>
-      <c r="I66" s="109"/>
-      <c r="J66" s="109"/>
+      <c r="H66" s="111"/>
+      <c r="I66" s="111"/>
+      <c r="J66" s="111"/>
     </row>
     <row r="67" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="22"/>
@@ -10537,12 +10701,12 @@
       <c r="E70" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G70" s="109" t="s">
+      <c r="G70" s="111" t="s">
         <v>285</v>
       </c>
-      <c r="H70" s="109"/>
-      <c r="I70" s="109"/>
-      <c r="J70" s="109"/>
+      <c r="H70" s="111"/>
+      <c r="I70" s="111"/>
+      <c r="J70" s="111"/>
     </row>
     <row r="71" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22"/>
@@ -10616,12 +10780,12 @@
       <c r="E75" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G75" s="109" t="s">
+      <c r="G75" s="111" t="s">
         <v>320</v>
       </c>
-      <c r="H75" s="109"/>
-      <c r="I75" s="109"/>
-      <c r="J75" s="109"/>
+      <c r="H75" s="111"/>
+      <c r="I75" s="111"/>
+      <c r="J75" s="111"/>
     </row>
     <row r="76" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
@@ -10666,12 +10830,12 @@
       <c r="E78" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G78" s="109" t="s">
+      <c r="G78" s="111" t="s">
         <v>286</v>
       </c>
-      <c r="H78" s="109"/>
-      <c r="I78" s="109"/>
-      <c r="J78" s="109"/>
+      <c r="H78" s="111"/>
+      <c r="I78" s="111"/>
+      <c r="J78" s="111"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A79" s="30" t="s">
@@ -10689,12 +10853,12 @@
       <c r="E79" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G79" s="109" t="s">
+      <c r="G79" s="111" t="s">
         <v>287</v>
       </c>
-      <c r="H79" s="109"/>
-      <c r="I79" s="109"/>
-      <c r="J79" s="109"/>
+      <c r="H79" s="111"/>
+      <c r="I79" s="111"/>
+      <c r="J79" s="111"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
@@ -10791,12 +10955,12 @@
       <c r="E86" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G86" s="109" t="s">
+      <c r="G86" s="111" t="s">
         <v>288</v>
       </c>
-      <c r="H86" s="109"/>
-      <c r="I86" s="109"/>
-      <c r="J86" s="109"/>
+      <c r="H86" s="111"/>
+      <c r="I86" s="111"/>
+      <c r="J86" s="111"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
@@ -10858,12 +11022,12 @@
       <c r="E91" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G91" s="109" t="s">
+      <c r="G91" s="111" t="s">
         <v>319</v>
       </c>
-      <c r="H91" s="109"/>
-      <c r="I91" s="109"/>
-      <c r="J91" s="109"/>
+      <c r="H91" s="111"/>
+      <c r="I91" s="111"/>
+      <c r="J91" s="111"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="22"/>
@@ -10920,12 +11084,12 @@
       <c r="E96" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G96" s="109" t="s">
+      <c r="G96" s="111" t="s">
         <v>289</v>
       </c>
-      <c r="H96" s="109"/>
-      <c r="I96" s="109"/>
-      <c r="J96" s="109"/>
+      <c r="H96" s="111"/>
+      <c r="I96" s="111"/>
+      <c r="J96" s="111"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="22"/>
@@ -11014,12 +11178,12 @@
       <c r="E103" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G103" s="109" t="s">
+      <c r="G103" s="111" t="s">
         <v>290</v>
       </c>
-      <c r="H103" s="109"/>
-      <c r="I103" s="109"/>
-      <c r="J103" s="109"/>
+      <c r="H103" s="111"/>
+      <c r="I103" s="111"/>
+      <c r="J103" s="111"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="22"/>
@@ -11089,12 +11253,12 @@
       <c r="E108" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G108" s="109" t="s">
+      <c r="G108" s="111" t="s">
         <v>291</v>
       </c>
-      <c r="H108" s="109"/>
-      <c r="I108" s="109"/>
-      <c r="J108" s="109"/>
+      <c r="H108" s="111"/>
+      <c r="I108" s="111"/>
+      <c r="J108" s="111"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="22"/>
@@ -11198,12 +11362,12 @@
       <c r="E116" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G116" s="109" t="s">
+      <c r="G116" s="111" t="s">
         <v>292</v>
       </c>
-      <c r="H116" s="109"/>
-      <c r="I116" s="109"/>
-      <c r="J116" s="109"/>
+      <c r="H116" s="111"/>
+      <c r="I116" s="111"/>
+      <c r="J116" s="111"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="22"/>
@@ -11416,12 +11580,12 @@
       <c r="E131" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G131" s="109" t="s">
+      <c r="G131" s="111" t="s">
         <v>336</v>
       </c>
-      <c r="H131" s="109"/>
-      <c r="I131" s="109"/>
-      <c r="J131" s="109"/>
+      <c r="H131" s="111"/>
+      <c r="I131" s="111"/>
+      <c r="J131" s="111"/>
     </row>
     <row r="132" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A132" s="30" t="s">
@@ -11439,12 +11603,12 @@
       <c r="E132" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G132" s="109" t="s">
+      <c r="G132" s="111" t="s">
         <v>376</v>
       </c>
-      <c r="H132" s="109"/>
-      <c r="I132" s="109"/>
-      <c r="J132" s="109"/>
+      <c r="H132" s="111"/>
+      <c r="I132" s="111"/>
+      <c r="J132" s="111"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="22"/>
@@ -11629,12 +11793,12 @@
       <c r="E146" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G146" s="109" t="s">
+      <c r="G146" s="111" t="s">
         <v>353</v>
       </c>
-      <c r="H146" s="109"/>
-      <c r="I146" s="109"/>
-      <c r="J146" s="109"/>
+      <c r="H146" s="111"/>
+      <c r="I146" s="111"/>
+      <c r="J146" s="111"/>
     </row>
     <row r="147" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A147" s="30" t="s">
@@ -11652,12 +11816,12 @@
       <c r="E147" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G147" s="109" t="s">
+      <c r="G147" s="111" t="s">
         <v>354</v>
       </c>
-      <c r="H147" s="109"/>
-      <c r="I147" s="109"/>
-      <c r="J147" s="109"/>
+      <c r="H147" s="111"/>
+      <c r="I147" s="111"/>
+      <c r="J147" s="111"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="22"/>
@@ -11704,12 +11868,12 @@
       <c r="E151" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G151" s="109" t="s">
+      <c r="G151" s="111" t="s">
         <v>339</v>
       </c>
-      <c r="H151" s="109"/>
-      <c r="I151" s="109"/>
-      <c r="J151" s="109"/>
+      <c r="H151" s="111"/>
+      <c r="I151" s="111"/>
+      <c r="J151" s="111"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="22"/>
@@ -11783,12 +11947,12 @@
       <c r="E156" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G156" s="109" t="s">
+      <c r="G156" s="111" t="s">
         <v>287</v>
       </c>
-      <c r="H156" s="109"/>
-      <c r="I156" s="109"/>
-      <c r="J156" s="109"/>
+      <c r="H156" s="111"/>
+      <c r="I156" s="111"/>
+      <c r="J156" s="111"/>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="22"/>
@@ -11870,12 +12034,12 @@
       <c r="E162" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G162" s="109" t="s">
+      <c r="G162" s="111" t="s">
         <v>333</v>
       </c>
-      <c r="H162" s="109"/>
-      <c r="I162" s="109"/>
-      <c r="J162" s="109"/>
+      <c r="H162" s="111"/>
+      <c r="I162" s="111"/>
+      <c r="J162" s="111"/>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="22"/>
@@ -11929,12 +12093,12 @@
       <c r="E166" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G166" s="109" t="s">
+      <c r="G166" s="111" t="s">
         <v>364</v>
       </c>
-      <c r="H166" s="109"/>
-      <c r="I166" s="109"/>
-      <c r="J166" s="109"/>
+      <c r="H166" s="111"/>
+      <c r="I166" s="111"/>
+      <c r="J166" s="111"/>
     </row>
     <row r="167" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A167" s="30" t="s">
@@ -11952,12 +12116,12 @@
       <c r="E167" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G167" s="109" t="s">
+      <c r="G167" s="111" t="s">
         <v>365</v>
       </c>
-      <c r="H167" s="109"/>
-      <c r="I167" s="109"/>
-      <c r="J167" s="109"/>
+      <c r="H167" s="111"/>
+      <c r="I167" s="111"/>
+      <c r="J167" s="111"/>
     </row>
     <row r="168" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A168" s="30" t="s">
@@ -11975,12 +12139,12 @@
       <c r="E168" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G168" s="109" t="s">
+      <c r="G168" s="111" t="s">
         <v>372</v>
       </c>
-      <c r="H168" s="109"/>
-      <c r="I168" s="109"/>
-      <c r="J168" s="109"/>
+      <c r="H168" s="111"/>
+      <c r="I168" s="111"/>
+      <c r="J168" s="111"/>
     </row>
     <row r="169" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A169" s="30" t="s">
@@ -11998,12 +12162,12 @@
       <c r="E169" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G169" s="109" t="s">
+      <c r="G169" s="111" t="s">
         <v>371</v>
       </c>
-      <c r="H169" s="109"/>
-      <c r="I169" s="109"/>
-      <c r="J169" s="109"/>
+      <c r="H169" s="111"/>
+      <c r="I169" s="111"/>
+      <c r="J169" s="111"/>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="22"/>
@@ -12050,12 +12214,12 @@
       <c r="E173" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G173" s="109" t="s">
+      <c r="G173" s="111" t="s">
         <v>293</v>
       </c>
-      <c r="H173" s="109"/>
-      <c r="I173" s="109"/>
-      <c r="J173" s="109"/>
+      <c r="H173" s="111"/>
+      <c r="I173" s="111"/>
+      <c r="J173" s="111"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="22"/>
@@ -12153,12 +12317,12 @@
       <c r="E180" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G180" s="109" t="s">
+      <c r="G180" s="111" t="s">
         <v>294</v>
       </c>
-      <c r="H180" s="109"/>
-      <c r="I180" s="109"/>
-      <c r="J180" s="109"/>
+      <c r="H180" s="111"/>
+      <c r="I180" s="111"/>
+      <c r="J180" s="111"/>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="22"/>
@@ -12267,12 +12431,12 @@
       <c r="E188" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G188" s="109" t="s">
+      <c r="G188" s="111" t="s">
         <v>585</v>
       </c>
-      <c r="H188" s="109"/>
-      <c r="I188" s="109"/>
-      <c r="J188" s="109"/>
+      <c r="H188" s="111"/>
+      <c r="I188" s="111"/>
+      <c r="J188" s="111"/>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="22"/>
@@ -12346,12 +12510,12 @@
       <c r="E193" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G193" s="109" t="s">
+      <c r="G193" s="111" t="s">
         <v>602</v>
       </c>
-      <c r="H193" s="109"/>
-      <c r="I193" s="109"/>
-      <c r="J193" s="109"/>
+      <c r="H193" s="111"/>
+      <c r="I193" s="111"/>
+      <c r="J193" s="111"/>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="22"/>
@@ -12409,12 +12573,12 @@
       <c r="E197" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G197" s="109" t="s">
+      <c r="G197" s="111" t="s">
         <v>295</v>
       </c>
-      <c r="H197" s="109"/>
-      <c r="I197" s="109"/>
-      <c r="J197" s="109"/>
+      <c r="H197" s="111"/>
+      <c r="I197" s="111"/>
+      <c r="J197" s="111"/>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="22"/>
@@ -12612,12 +12776,12 @@
       <c r="E210" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G210" s="109" t="s">
+      <c r="G210" s="111" t="s">
         <v>296</v>
       </c>
-      <c r="H210" s="109"/>
-      <c r="I210" s="109"/>
-      <c r="J210" s="109"/>
+      <c r="H210" s="111"/>
+      <c r="I210" s="111"/>
+      <c r="J210" s="111"/>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="22"/>
@@ -12694,26 +12858,29 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="G63:J63"/>
-    <mergeCell ref="G64:J64"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="G66:J66"/>
-    <mergeCell ref="G70:J70"/>
-    <mergeCell ref="G75:J75"/>
-    <mergeCell ref="G78:J78"/>
-    <mergeCell ref="G79:J79"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G210:J210"/>
+    <mergeCell ref="G156:J156"/>
+    <mergeCell ref="G169:J169"/>
+    <mergeCell ref="G173:J173"/>
+    <mergeCell ref="G180:J180"/>
+    <mergeCell ref="G197:J197"/>
+    <mergeCell ref="G193:J193"/>
+    <mergeCell ref="G188:J188"/>
+    <mergeCell ref="G116:J116"/>
+    <mergeCell ref="G131:J131"/>
+    <mergeCell ref="G166:J166"/>
+    <mergeCell ref="G167:J167"/>
+    <mergeCell ref="G168:J168"/>
+    <mergeCell ref="G162:J162"/>
+    <mergeCell ref="G151:J151"/>
+    <mergeCell ref="G146:J146"/>
+    <mergeCell ref="G147:J147"/>
+    <mergeCell ref="G132:J132"/>
+    <mergeCell ref="G86:J86"/>
+    <mergeCell ref="G91:J91"/>
+    <mergeCell ref="G96:J96"/>
+    <mergeCell ref="G103:J103"/>
+    <mergeCell ref="G108:J108"/>
     <mergeCell ref="B89:E89"/>
     <mergeCell ref="G15:J15"/>
     <mergeCell ref="G19:J19"/>
@@ -12730,29 +12897,26 @@
     <mergeCell ref="G50:J50"/>
     <mergeCell ref="G51:J51"/>
     <mergeCell ref="G52:J52"/>
-    <mergeCell ref="G86:J86"/>
-    <mergeCell ref="G91:J91"/>
-    <mergeCell ref="G96:J96"/>
-    <mergeCell ref="G103:J103"/>
-    <mergeCell ref="G108:J108"/>
-    <mergeCell ref="G116:J116"/>
-    <mergeCell ref="G131:J131"/>
-    <mergeCell ref="G166:J166"/>
-    <mergeCell ref="G167:J167"/>
-    <mergeCell ref="G168:J168"/>
-    <mergeCell ref="G162:J162"/>
-    <mergeCell ref="G151:J151"/>
-    <mergeCell ref="G146:J146"/>
-    <mergeCell ref="G147:J147"/>
-    <mergeCell ref="G132:J132"/>
-    <mergeCell ref="G210:J210"/>
-    <mergeCell ref="G156:J156"/>
-    <mergeCell ref="G169:J169"/>
-    <mergeCell ref="G173:J173"/>
-    <mergeCell ref="G180:J180"/>
-    <mergeCell ref="G197:J197"/>
-    <mergeCell ref="G193:J193"/>
-    <mergeCell ref="G188:J188"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="G63:J63"/>
+    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="G66:J66"/>
+    <mergeCell ref="G70:J70"/>
+    <mergeCell ref="G75:J75"/>
+    <mergeCell ref="G78:J78"/>
+    <mergeCell ref="G79:J79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
SAR WIP, plus SAP Tweaks
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="-3540" windowWidth="10065" windowHeight="12525" activeTab="3"/>
+    <workbookView xWindow="12510" yWindow="-3540" windowWidth="10065" windowHeight="12525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATION" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2077" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="652">
   <si>
     <t>SSP</t>
   </si>
@@ -2306,6 +2306,33 @@
   </si>
   <si>
     <t>penetration-test-report</t>
+  </si>
+  <si>
+    <t>Authorization Date</t>
+  </si>
+  <si>
+    <t>authorized</t>
+  </si>
+  <si>
+    <t>System Purpose</t>
+  </si>
+  <si>
+    <t>System Description</t>
+  </si>
+  <si>
+    <t>purpose</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>/*/back-matter/resource/prop[@name="description"][@ns="https://fedramp.gov/ns/oscal"]</t>
+  </si>
+  <si>
+    <t>/*/back-matter/resource/prop[@name="authorized"][@ns="https://fedramp.gov/ns/oscal"]</t>
+  </si>
+  <si>
+    <t>/*/back-matter/resource/prop[@name="purpose"][@ns="https://fedramp.gov/ns/oscal"]</t>
   </si>
 </sst>
 </file>
@@ -2866,7 +2893,7 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="7" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -3100,6 +3127,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="29" fillId="6" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3139,13 +3170,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="AUTHOR-NOTE" xfId="5"/>
@@ -3506,12 +3536,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="102" t="s">
         <v>397</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
       <c r="H1" s="55" t="s">
         <v>395</v>
       </c>
@@ -3527,18 +3557,18 @@
       <c r="B3" s="57"/>
     </row>
     <row r="4" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="105" t="s">
         <v>406</v>
       </c>
-      <c r="B4" s="103"/>
+      <c r="B4" s="105"/>
       <c r="C4" s="59"/>
       <c r="D4" s="59"/>
     </row>
     <row r="5" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="106" t="s">
         <v>420</v>
       </c>
-      <c r="B5" s="104"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="59"/>
     </row>
     <row r="6" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
@@ -3551,19 +3581,19 @@
       <c r="E6" s="60"/>
     </row>
     <row r="7" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="106" t="s">
         <v>418</v>
       </c>
-      <c r="B7" s="102"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="62"/>
       <c r="D7" s="62"/>
       <c r="E7" s="62"/>
     </row>
     <row r="8" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="101" t="s">
+      <c r="A8" s="103" t="s">
         <v>419</v>
       </c>
-      <c r="B8" s="102"/>
+      <c r="B8" s="104"/>
     </row>
     <row r="9" spans="1:8" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
@@ -3575,45 +3605,45 @@
       <c r="E9" s="60"/>
     </row>
     <row r="10" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="104" t="s">
+      <c r="A10" s="106" t="s">
         <v>400</v>
       </c>
-      <c r="B10" s="102"/>
+      <c r="B10" s="104"/>
       <c r="C10" s="62"/>
       <c r="D10" s="62"/>
       <c r="E10" s="62"/>
     </row>
     <row r="11" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="103" t="s">
         <v>405</v>
       </c>
-      <c r="B11" s="102"/>
+      <c r="B11" s="104"/>
     </row>
     <row r="12" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="106" t="s">
         <v>401</v>
       </c>
-      <c r="B12" s="104"/>
+      <c r="B12" s="106"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="102" t="s">
+      <c r="A13" s="104" t="s">
         <v>403</v>
       </c>
-      <c r="B13" s="102"/>
+      <c r="B13" s="104"/>
     </row>
     <row r="14" spans="1:8" ht="43.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="101" t="s">
+      <c r="A14" s="103" t="s">
         <v>402</v>
       </c>
-      <c r="B14" s="102"/>
+      <c r="B14" s="104"/>
     </row>
     <row r="15" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="99" t="s">
         <v>421</v>
       </c>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="99"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="100"/>
+      <c r="D15" s="101"/>
     </row>
     <row r="16" spans="1:8" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="75" t="s">
@@ -3727,13 +3757,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:O84"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="7" ySplit="3" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3757,35 +3787,35 @@
       <c r="C1" s="6"/>
       <c r="D1"/>
       <c r="E1" s="6"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
+      <c r="H1" s="108"/>
+      <c r="I1" s="108"/>
       <c r="J1" s="91" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
       <c r="G2" s="64" t="s">
         <v>430</v>
       </c>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
       <c r="J2" t="s">
         <v>468</v>
       </c>
-      <c r="K2" s="105" t="s">
+      <c r="K2" s="107" t="s">
         <v>386</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="107" t="s">
         <v>316</v>
       </c>
-      <c r="M2" s="105" t="s">
+      <c r="M2" s="107" t="s">
         <v>589</v>
       </c>
     </row>
@@ -3817,9 +3847,9 @@
       <c r="J3" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
-      <c r="M3" s="105"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
+      <c r="M3" s="107"/>
       <c r="N3" s="53" t="s">
         <v>8</v>
       </c>
@@ -5584,14 +5614,39 @@
       </c>
     </row>
     <row r="67" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="H67" s="78"/>
-      <c r="I67" s="78"/>
-      <c r="J67" s="79"/>
+      <c r="A67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" t="s">
+        <v>643</v>
+      </c>
+      <c r="H67" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="I67" s="78" t="s">
+        <v>644</v>
+      </c>
+      <c r="J67" s="97" t="s">
+        <v>650</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="N67" s="4" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="68" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
@@ -5600,131 +5655,214 @@
       <c r="B68" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C68" s="6">
-        <v>1</v>
-      </c>
-      <c r="D68" s="6">
-        <v>1</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>7</v>
+      <c r="C68" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="G68" t="s">
-        <v>600</v>
+        <v>645</v>
       </c>
       <c r="H68" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I68" s="78" t="s">
-        <v>601</v>
-      </c>
-      <c r="J68" s="93" t="s">
-        <v>602</v>
+        <v>647</v>
+      </c>
+      <c r="J68" s="97" t="s">
+        <v>651</v>
       </c>
       <c r="K68" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="M68" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="N68" s="4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G69" t="s">
+        <v>646</v>
+      </c>
+      <c r="H69" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="I69" s="78" t="s">
+        <v>648</v>
+      </c>
+      <c r="J69" s="97" t="s">
+        <v>649</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="H70" s="78"/>
+      <c r="I70" s="78"/>
+      <c r="J70" s="79"/>
+    </row>
+    <row r="71" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="6">
+        <v>1</v>
+      </c>
+      <c r="D71" s="6">
+        <v>1</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" t="s">
+        <v>600</v>
+      </c>
+      <c r="H71" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="I71" s="78" t="s">
+        <v>601</v>
+      </c>
+      <c r="J71" s="93" t="s">
+        <v>602</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N71" s="4" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="H69" s="78"/>
-      <c r="I69" s="78"/>
-      <c r="J69" s="79"/>
-    </row>
-    <row r="70" spans="1:14" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="87"/>
-      <c r="F70" s="90"/>
-      <c r="L70" s="90"/>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G71" s="82" t="s">
+    <row r="72" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="H72" s="78"/>
+      <c r="I72" s="78"/>
+      <c r="J72" s="79"/>
+    </row>
+    <row r="73" spans="1:14" s="65" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A73" s="87"/>
+      <c r="F73" s="90"/>
+      <c r="L73" s="90"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G74" s="82" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G72" t="s">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
         <v>251</v>
       </c>
-      <c r="H72" s="78" t="s">
+      <c r="H75" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="I72" s="81" t="s">
+      <c r="I75" s="81" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G73" t="s">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
         <v>115</v>
       </c>
-      <c r="H73" s="78" t="s">
+      <c r="H76" s="78" t="s">
         <v>434</v>
       </c>
-      <c r="I73" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G74" t="s">
+      <c r="I76" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
         <v>73</v>
       </c>
-      <c r="H74" s="78" t="s">
+      <c r="H77" s="78" t="s">
         <v>503</v>
       </c>
-      <c r="I74" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G80" s="82" t="s">
+      <c r="I77" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G83" s="82" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="81" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G81" t="s">
+    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
         <v>417</v>
       </c>
-      <c r="H81" s="78" t="s">
+      <c r="H84" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="I81" s="78" t="s">
+      <c r="I84" s="78" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="82" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G82" t="s">
+    <row r="85" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
         <v>71</v>
       </c>
-      <c r="H82" s="78" t="s">
+      <c r="H85" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="I82" s="78" t="s">
+      <c r="I85" s="78" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="83" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G83" t="s">
+    <row r="86" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
         <v>72</v>
       </c>
-      <c r="H83" s="78" t="s">
+      <c r="H86" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="I83" s="78" t="s">
+      <c r="I86" s="78" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="84" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="H84" s="78"/>
-      <c r="I84" s="78"/>
+    <row r="87" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="H87" s="78"/>
+      <c r="I87" s="78"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5777,27 +5915,27 @@
       <c r="I1" s="95"/>
     </row>
     <row r="2" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
       <c r="G2" s="64" t="s">
         <v>431</v>
       </c>
-      <c r="H2" s="108" t="s">
+      <c r="H2" s="110" t="s">
         <v>501</v>
       </c>
-      <c r="I2" s="108"/>
+      <c r="I2" s="110"/>
       <c r="J2" t="s">
         <v>468</v>
       </c>
-      <c r="K2" s="105" t="s">
+      <c r="K2" s="107" t="s">
         <v>386</v>
       </c>
-      <c r="L2" s="105" t="s">
+      <c r="L2" s="107" t="s">
         <v>316</v>
       </c>
     </row>
@@ -5829,8 +5967,8 @@
       <c r="J3" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="K3" s="105"/>
-      <c r="L3" s="105"/>
+      <c r="K3" s="107"/>
+      <c r="L3" s="107"/>
       <c r="M3" s="53" t="s">
         <v>8</v>
       </c>
@@ -7047,7 +7185,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="7" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -7074,7 +7212,7 @@
       <c r="D1"/>
       <c r="E1" s="6"/>
       <c r="H1" s="80"/>
-      <c r="I1" s="106" t="str">
+      <c r="I1" s="108" t="str">
         <f>CONCATENATE("All FedRAMP Compliance tags must use name='", tagname, "', as well as ns='https://fedramp.gov/ns/oscal'")</f>
         <v>All FedRAMP Compliance tags must use name='conformity', as well as ns='https://fedramp.gov/ns/oscal'</v>
       </c>
@@ -7083,18 +7221,18 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
       <c r="G2" s="64" t="s">
         <v>430</v>
       </c>
       <c r="H2" s="80"/>
-      <c r="I2" s="106"/>
+      <c r="I2" s="108"/>
       <c r="J2" t="s">
         <v>468</v>
       </c>
@@ -7213,7 +7351,7 @@
         <f>CONCATENATE(I7,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H7,"']/..")</f>
         <v>/*/metadata/location/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='primary-data-center']/..</v>
       </c>
-      <c r="K7" s="109" t="s">
+      <c r="K7" s="111" t="s">
         <v>566</v>
       </c>
       <c r="L7" s="83" t="str">
@@ -7250,7 +7388,7 @@
         <f>CONCATENATE(I8,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H8,"']/..")</f>
         <v>/*/metadata/location/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='alternate-data-center']/..</v>
       </c>
-      <c r="K8" s="109"/>
+      <c r="K8" s="111"/>
       <c r="L8" s="83" t="str">
         <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H8,"&lt;/prop&gt;")</f>
         <v>&lt;prop name='conformity' ns='https://fedramp.gov/ns/oscal'&gt;alternate-data-center&lt;/prop&gt;</v>
@@ -8011,7 +8149,7 @@
       <c r="G32" s="54" t="s">
         <v>640</v>
       </c>
-      <c r="H32" s="112" t="s">
+      <c r="H32" s="98" t="s">
         <v>639</v>
       </c>
       <c r="I32" s="79" t="s">
@@ -8045,7 +8183,7 @@
       <c r="G33" s="54" t="s">
         <v>641</v>
       </c>
-      <c r="H33" s="112" t="s">
+      <c r="H33" s="98" t="s">
         <v>642</v>
       </c>
       <c r="I33" s="79" t="s">
@@ -8066,7 +8204,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="H34" s="112"/>
+      <c r="H34" s="98"/>
       <c r="I34" s="79"/>
       <c r="J34" s="79"/>
     </row>
@@ -8231,17 +8369,17 @@
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="109" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="G2" s="107" t="s">
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="G2" s="109" t="s">
         <v>98</v>
       </c>
-      <c r="H2" s="107"/>
+      <c r="H2" s="109"/>
       <c r="I2" s="28" t="s">
         <v>301</v>
       </c>
@@ -9454,17 +9592,17 @@
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="109" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="G2" s="107" t="s">
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="G2" s="109" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="107"/>
+      <c r="H2" s="109"/>
       <c r="I2" s="28" t="s">
         <v>230</v>
       </c>
@@ -9514,12 +9652,12 @@
       <c r="E4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="111" t="s">
+      <c r="G4" s="112" t="s">
         <v>322</v>
       </c>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
@@ -9537,12 +9675,12 @@
       <c r="E5" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="111" t="s">
+      <c r="G5" s="112" t="s">
         <v>321</v>
       </c>
-      <c r="H5" s="111"/>
-      <c r="I5" s="111"/>
-      <c r="J5" s="111"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
     </row>
     <row r="6" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
@@ -9603,12 +9741,12 @@
       <c r="E9" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="111" t="s">
+      <c r="G9" s="112" t="s">
         <v>328</v>
       </c>
-      <c r="H9" s="111"/>
-      <c r="I9" s="111"/>
-      <c r="J9" s="111"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
     </row>
     <row r="10" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
@@ -9626,12 +9764,12 @@
       <c r="E10" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="111" t="s">
+      <c r="G10" s="112" t="s">
         <v>327</v>
       </c>
-      <c r="H10" s="111"/>
-      <c r="I10" s="111"/>
-      <c r="J10" s="111"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="112"/>
+      <c r="J10" s="112"/>
     </row>
     <row r="11" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
@@ -9708,12 +9846,12 @@
       <c r="E15" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="111" t="s">
+      <c r="G15" s="112" t="s">
         <v>264</v>
       </c>
-      <c r="H15" s="111"/>
-      <c r="I15" s="111"/>
-      <c r="J15" s="111"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
@@ -9774,12 +9912,12 @@
       <c r="E19" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="111" t="s">
+      <c r="G19" s="112" t="s">
         <v>265</v>
       </c>
-      <c r="H19" s="111"/>
-      <c r="I19" s="111"/>
-      <c r="J19" s="111"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
     </row>
     <row r="20" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
@@ -9797,12 +9935,12 @@
       <c r="E20" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="111" t="s">
+      <c r="G20" s="112" t="s">
         <v>266</v>
       </c>
-      <c r="H20" s="111"/>
-      <c r="I20" s="111"/>
-      <c r="J20" s="111"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="112"/>
     </row>
     <row r="21" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
@@ -9820,12 +9958,12 @@
       <c r="E21" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="111" t="s">
+      <c r="G21" s="112" t="s">
         <v>267</v>
       </c>
-      <c r="H21" s="111"/>
-      <c r="I21" s="111"/>
-      <c r="J21" s="111"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="112"/>
+      <c r="J21" s="112"/>
     </row>
     <row r="22" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
@@ -9843,12 +9981,12 @@
       <c r="E22" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="111" t="s">
+      <c r="G22" s="112" t="s">
         <v>268</v>
       </c>
-      <c r="H22" s="111"/>
-      <c r="I22" s="111"/>
-      <c r="J22" s="111"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="112"/>
     </row>
     <row r="23" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
@@ -9925,12 +10063,12 @@
       <c r="E27" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="111" t="s">
+      <c r="G27" s="112" t="s">
         <v>269</v>
       </c>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
+      <c r="H27" s="112"/>
+      <c r="I27" s="112"/>
+      <c r="J27" s="112"/>
     </row>
     <row r="28" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
@@ -10010,12 +10148,12 @@
       <c r="E32" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G32" s="111" t="s">
+      <c r="G32" s="112" t="s">
         <v>318</v>
       </c>
-      <c r="H32" s="111"/>
-      <c r="I32" s="111"/>
-      <c r="J32" s="111"/>
+      <c r="H32" s="112"/>
+      <c r="I32" s="112"/>
+      <c r="J32" s="112"/>
     </row>
     <row r="33" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
@@ -10108,12 +10246,12 @@
       <c r="E38" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G38" s="111" t="s">
+      <c r="G38" s="112" t="s">
         <v>270</v>
       </c>
-      <c r="H38" s="111"/>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
+      <c r="H38" s="112"/>
+      <c r="I38" s="112"/>
+      <c r="J38" s="112"/>
     </row>
     <row r="39" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -10148,12 +10286,12 @@
       </c>
     </row>
     <row r="41" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="110" t="s">
+      <c r="B41" s="113" t="s">
         <v>248</v>
       </c>
-      <c r="C41" s="110"/>
-      <c r="D41" s="110"/>
-      <c r="E41" s="110"/>
+      <c r="C41" s="113"/>
+      <c r="D41" s="113"/>
+      <c r="E41" s="113"/>
       <c r="G41" s="15" t="s">
         <v>23</v>
       </c>
@@ -10241,12 +10379,12 @@
       <c r="E46" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G46" s="111" t="s">
+      <c r="G46" s="112" t="s">
         <v>271</v>
       </c>
-      <c r="H46" s="111"/>
-      <c r="I46" s="111"/>
-      <c r="J46" s="111"/>
+      <c r="H46" s="112"/>
+      <c r="I46" s="112"/>
+      <c r="J46" s="112"/>
     </row>
     <row r="47" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
@@ -10264,12 +10402,12 @@
       <c r="E47" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G47" s="111" t="s">
+      <c r="G47" s="112" t="s">
         <v>272</v>
       </c>
-      <c r="H47" s="111"/>
-      <c r="I47" s="111"/>
-      <c r="J47" s="111"/>
+      <c r="H47" s="112"/>
+      <c r="I47" s="112"/>
+      <c r="J47" s="112"/>
     </row>
     <row r="48" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
@@ -10287,12 +10425,12 @@
       <c r="E48" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="111" t="s">
+      <c r="G48" s="112" t="s">
         <v>273</v>
       </c>
-      <c r="H48" s="111"/>
-      <c r="I48" s="111"/>
-      <c r="J48" s="111"/>
+      <c r="H48" s="112"/>
+      <c r="I48" s="112"/>
+      <c r="J48" s="112"/>
     </row>
     <row r="49" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
@@ -10310,12 +10448,12 @@
       <c r="E49" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G49" s="111" t="s">
+      <c r="G49" s="112" t="s">
         <v>274</v>
       </c>
-      <c r="H49" s="111"/>
-      <c r="I49" s="111"/>
-      <c r="J49" s="111"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="112"/>
+      <c r="J49" s="112"/>
     </row>
     <row r="50" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
@@ -10333,12 +10471,12 @@
       <c r="E50" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G50" s="111" t="s">
+      <c r="G50" s="112" t="s">
         <v>275</v>
       </c>
-      <c r="H50" s="111"/>
-      <c r="I50" s="111"/>
-      <c r="J50" s="111"/>
+      <c r="H50" s="112"/>
+      <c r="I50" s="112"/>
+      <c r="J50" s="112"/>
     </row>
     <row r="51" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
@@ -10356,12 +10494,12 @@
       <c r="E51" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G51" s="111" t="s">
+      <c r="G51" s="112" t="s">
         <v>276</v>
       </c>
-      <c r="H51" s="111"/>
-      <c r="I51" s="111"/>
-      <c r="J51" s="111"/>
+      <c r="H51" s="112"/>
+      <c r="I51" s="112"/>
+      <c r="J51" s="112"/>
     </row>
     <row r="52" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
@@ -10379,12 +10517,12 @@
       <c r="E52" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G52" s="111" t="s">
+      <c r="G52" s="112" t="s">
         <v>277</v>
       </c>
-      <c r="H52" s="111"/>
-      <c r="I52" s="111"/>
-      <c r="J52" s="111"/>
+      <c r="H52" s="112"/>
+      <c r="I52" s="112"/>
+      <c r="J52" s="112"/>
     </row>
     <row r="53" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
@@ -10402,12 +10540,12 @@
       <c r="E53" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G53" s="111" t="s">
+      <c r="G53" s="112" t="s">
         <v>278</v>
       </c>
-      <c r="H53" s="111"/>
-      <c r="I53" s="111"/>
-      <c r="J53" s="111"/>
+      <c r="H53" s="112"/>
+      <c r="I53" s="112"/>
+      <c r="J53" s="112"/>
     </row>
     <row r="54" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
@@ -10425,12 +10563,12 @@
       <c r="E54" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G54" s="111" t="s">
+      <c r="G54" s="112" t="s">
         <v>279</v>
       </c>
-      <c r="H54" s="111"/>
-      <c r="I54" s="111"/>
-      <c r="J54" s="111"/>
+      <c r="H54" s="112"/>
+      <c r="I54" s="112"/>
+      <c r="J54" s="112"/>
     </row>
     <row r="55" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
@@ -10504,12 +10642,12 @@
       <c r="E59" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G59" s="111" t="s">
+      <c r="G59" s="112" t="s">
         <v>280</v>
       </c>
-      <c r="H59" s="111"/>
-      <c r="I59" s="111"/>
-      <c r="J59" s="111"/>
+      <c r="H59" s="112"/>
+      <c r="I59" s="112"/>
+      <c r="J59" s="112"/>
     </row>
     <row r="60" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
@@ -10570,12 +10708,12 @@
       <c r="E63" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G63" s="111" t="s">
+      <c r="G63" s="112" t="s">
         <v>281</v>
       </c>
-      <c r="H63" s="111"/>
-      <c r="I63" s="111"/>
-      <c r="J63" s="111"/>
+      <c r="H63" s="112"/>
+      <c r="I63" s="112"/>
+      <c r="J63" s="112"/>
     </row>
     <row r="64" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A64" s="31" t="s">
@@ -10593,12 +10731,12 @@
       <c r="E64" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G64" s="111" t="s">
+      <c r="G64" s="112" t="s">
         <v>282</v>
       </c>
-      <c r="H64" s="111"/>
-      <c r="I64" s="111"/>
-      <c r="J64" s="111"/>
+      <c r="H64" s="112"/>
+      <c r="I64" s="112"/>
+      <c r="J64" s="112"/>
     </row>
     <row r="65" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65" s="31" t="s">
@@ -10616,12 +10754,12 @@
       <c r="E65" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G65" s="111" t="s">
+      <c r="G65" s="112" t="s">
         <v>283</v>
       </c>
-      <c r="H65" s="111"/>
-      <c r="I65" s="111"/>
-      <c r="J65" s="111"/>
+      <c r="H65" s="112"/>
+      <c r="I65" s="112"/>
+      <c r="J65" s="112"/>
     </row>
     <row r="66" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A66" s="31" t="s">
@@ -10639,12 +10777,12 @@
       <c r="E66" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G66" s="111" t="s">
+      <c r="G66" s="112" t="s">
         <v>284</v>
       </c>
-      <c r="H66" s="111"/>
-      <c r="I66" s="111"/>
-      <c r="J66" s="111"/>
+      <c r="H66" s="112"/>
+      <c r="I66" s="112"/>
+      <c r="J66" s="112"/>
     </row>
     <row r="67" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="22"/>
@@ -10701,12 +10839,12 @@
       <c r="E70" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G70" s="111" t="s">
+      <c r="G70" s="112" t="s">
         <v>285</v>
       </c>
-      <c r="H70" s="111"/>
-      <c r="I70" s="111"/>
-      <c r="J70" s="111"/>
+      <c r="H70" s="112"/>
+      <c r="I70" s="112"/>
+      <c r="J70" s="112"/>
     </row>
     <row r="71" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22"/>
@@ -10780,12 +10918,12 @@
       <c r="E75" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G75" s="111" t="s">
+      <c r="G75" s="112" t="s">
         <v>320</v>
       </c>
-      <c r="H75" s="111"/>
-      <c r="I75" s="111"/>
-      <c r="J75" s="111"/>
+      <c r="H75" s="112"/>
+      <c r="I75" s="112"/>
+      <c r="J75" s="112"/>
     </row>
     <row r="76" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
@@ -10830,12 +10968,12 @@
       <c r="E78" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G78" s="111" t="s">
+      <c r="G78" s="112" t="s">
         <v>286</v>
       </c>
-      <c r="H78" s="111"/>
-      <c r="I78" s="111"/>
-      <c r="J78" s="111"/>
+      <c r="H78" s="112"/>
+      <c r="I78" s="112"/>
+      <c r="J78" s="112"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A79" s="30" t="s">
@@ -10853,12 +10991,12 @@
       <c r="E79" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G79" s="111" t="s">
+      <c r="G79" s="112" t="s">
         <v>287</v>
       </c>
-      <c r="H79" s="111"/>
-      <c r="I79" s="111"/>
-      <c r="J79" s="111"/>
+      <c r="H79" s="112"/>
+      <c r="I79" s="112"/>
+      <c r="J79" s="112"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
@@ -10874,12 +11012,12 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="110" t="s">
+      <c r="B81" s="113" t="s">
         <v>248</v>
       </c>
-      <c r="C81" s="110"/>
-      <c r="D81" s="110"/>
-      <c r="E81" s="110"/>
+      <c r="C81" s="113"/>
+      <c r="D81" s="113"/>
+      <c r="E81" s="113"/>
       <c r="G81" s="33" t="s">
         <v>23</v>
       </c>
@@ -10907,12 +11045,12 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="110" t="s">
+      <c r="B83" s="113" t="s">
         <v>248</v>
       </c>
-      <c r="C83" s="110"/>
-      <c r="D83" s="110"/>
-      <c r="E83" s="110"/>
+      <c r="C83" s="113"/>
+      <c r="D83" s="113"/>
+      <c r="E83" s="113"/>
       <c r="G83" s="33" t="s">
         <v>23</v>
       </c>
@@ -10955,12 +11093,12 @@
       <c r="E86" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G86" s="111" t="s">
+      <c r="G86" s="112" t="s">
         <v>288</v>
       </c>
-      <c r="H86" s="111"/>
-      <c r="I86" s="111"/>
-      <c r="J86" s="111"/>
+      <c r="H86" s="112"/>
+      <c r="I86" s="112"/>
+      <c r="J86" s="112"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
@@ -10990,12 +11128,12 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="37"/>
-      <c r="B89" s="110" t="s">
+      <c r="B89" s="113" t="s">
         <v>248</v>
       </c>
-      <c r="C89" s="110"/>
-      <c r="D89" s="110"/>
-      <c r="E89" s="110"/>
+      <c r="C89" s="113"/>
+      <c r="D89" s="113"/>
+      <c r="E89" s="113"/>
       <c r="F89" s="37"/>
       <c r="G89" s="33" t="s">
         <v>23</v>
@@ -11022,12 +11160,12 @@
       <c r="E91" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G91" s="111" t="s">
+      <c r="G91" s="112" t="s">
         <v>319</v>
       </c>
-      <c r="H91" s="111"/>
-      <c r="I91" s="111"/>
-      <c r="J91" s="111"/>
+      <c r="H91" s="112"/>
+      <c r="I91" s="112"/>
+      <c r="J91" s="112"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="22"/>
@@ -11084,12 +11222,12 @@
       <c r="E96" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G96" s="111" t="s">
+      <c r="G96" s="112" t="s">
         <v>289</v>
       </c>
-      <c r="H96" s="111"/>
-      <c r="I96" s="111"/>
-      <c r="J96" s="111"/>
+      <c r="H96" s="112"/>
+      <c r="I96" s="112"/>
+      <c r="J96" s="112"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="22"/>
@@ -11178,12 +11316,12 @@
       <c r="E103" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G103" s="111" t="s">
+      <c r="G103" s="112" t="s">
         <v>290</v>
       </c>
-      <c r="H103" s="111"/>
-      <c r="I103" s="111"/>
-      <c r="J103" s="111"/>
+      <c r="H103" s="112"/>
+      <c r="I103" s="112"/>
+      <c r="J103" s="112"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="22"/>
@@ -11253,12 +11391,12 @@
       <c r="E108" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G108" s="111" t="s">
+      <c r="G108" s="112" t="s">
         <v>291</v>
       </c>
-      <c r="H108" s="111"/>
-      <c r="I108" s="111"/>
-      <c r="J108" s="111"/>
+      <c r="H108" s="112"/>
+      <c r="I108" s="112"/>
+      <c r="J108" s="112"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="22"/>
@@ -11362,12 +11500,12 @@
       <c r="E116" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G116" s="111" t="s">
+      <c r="G116" s="112" t="s">
         <v>292</v>
       </c>
-      <c r="H116" s="111"/>
-      <c r="I116" s="111"/>
-      <c r="J116" s="111"/>
+      <c r="H116" s="112"/>
+      <c r="I116" s="112"/>
+      <c r="J116" s="112"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="22"/>
@@ -11580,12 +11718,12 @@
       <c r="E131" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G131" s="111" t="s">
+      <c r="G131" s="112" t="s">
         <v>336</v>
       </c>
-      <c r="H131" s="111"/>
-      <c r="I131" s="111"/>
-      <c r="J131" s="111"/>
+      <c r="H131" s="112"/>
+      <c r="I131" s="112"/>
+      <c r="J131" s="112"/>
     </row>
     <row r="132" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A132" s="30" t="s">
@@ -11603,12 +11741,12 @@
       <c r="E132" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G132" s="111" t="s">
+      <c r="G132" s="112" t="s">
         <v>376</v>
       </c>
-      <c r="H132" s="111"/>
-      <c r="I132" s="111"/>
-      <c r="J132" s="111"/>
+      <c r="H132" s="112"/>
+      <c r="I132" s="112"/>
+      <c r="J132" s="112"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="22"/>
@@ -11793,12 +11931,12 @@
       <c r="E146" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G146" s="111" t="s">
+      <c r="G146" s="112" t="s">
         <v>353</v>
       </c>
-      <c r="H146" s="111"/>
-      <c r="I146" s="111"/>
-      <c r="J146" s="111"/>
+      <c r="H146" s="112"/>
+      <c r="I146" s="112"/>
+      <c r="J146" s="112"/>
     </row>
     <row r="147" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A147" s="30" t="s">
@@ -11816,12 +11954,12 @@
       <c r="E147" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G147" s="111" t="s">
+      <c r="G147" s="112" t="s">
         <v>354</v>
       </c>
-      <c r="H147" s="111"/>
-      <c r="I147" s="111"/>
-      <c r="J147" s="111"/>
+      <c r="H147" s="112"/>
+      <c r="I147" s="112"/>
+      <c r="J147" s="112"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="22"/>
@@ -11868,12 +12006,12 @@
       <c r="E151" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G151" s="111" t="s">
+      <c r="G151" s="112" t="s">
         <v>339</v>
       </c>
-      <c r="H151" s="111"/>
-      <c r="I151" s="111"/>
-      <c r="J151" s="111"/>
+      <c r="H151" s="112"/>
+      <c r="I151" s="112"/>
+      <c r="J151" s="112"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="22"/>
@@ -11947,12 +12085,12 @@
       <c r="E156" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G156" s="111" t="s">
+      <c r="G156" s="112" t="s">
         <v>287</v>
       </c>
-      <c r="H156" s="111"/>
-      <c r="I156" s="111"/>
-      <c r="J156" s="111"/>
+      <c r="H156" s="112"/>
+      <c r="I156" s="112"/>
+      <c r="J156" s="112"/>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="22"/>
@@ -12034,12 +12172,12 @@
       <c r="E162" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G162" s="111" t="s">
+      <c r="G162" s="112" t="s">
         <v>333</v>
       </c>
-      <c r="H162" s="111"/>
-      <c r="I162" s="111"/>
-      <c r="J162" s="111"/>
+      <c r="H162" s="112"/>
+      <c r="I162" s="112"/>
+      <c r="J162" s="112"/>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="22"/>
@@ -12093,12 +12231,12 @@
       <c r="E166" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G166" s="111" t="s">
+      <c r="G166" s="112" t="s">
         <v>364</v>
       </c>
-      <c r="H166" s="111"/>
-      <c r="I166" s="111"/>
-      <c r="J166" s="111"/>
+      <c r="H166" s="112"/>
+      <c r="I166" s="112"/>
+      <c r="J166" s="112"/>
     </row>
     <row r="167" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A167" s="30" t="s">
@@ -12116,12 +12254,12 @@
       <c r="E167" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G167" s="111" t="s">
+      <c r="G167" s="112" t="s">
         <v>365</v>
       </c>
-      <c r="H167" s="111"/>
-      <c r="I167" s="111"/>
-      <c r="J167" s="111"/>
+      <c r="H167" s="112"/>
+      <c r="I167" s="112"/>
+      <c r="J167" s="112"/>
     </row>
     <row r="168" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A168" s="30" t="s">
@@ -12139,12 +12277,12 @@
       <c r="E168" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G168" s="111" t="s">
+      <c r="G168" s="112" t="s">
         <v>372</v>
       </c>
-      <c r="H168" s="111"/>
-      <c r="I168" s="111"/>
-      <c r="J168" s="111"/>
+      <c r="H168" s="112"/>
+      <c r="I168" s="112"/>
+      <c r="J168" s="112"/>
     </row>
     <row r="169" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A169" s="30" t="s">
@@ -12162,12 +12300,12 @@
       <c r="E169" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G169" s="111" t="s">
+      <c r="G169" s="112" t="s">
         <v>371</v>
       </c>
-      <c r="H169" s="111"/>
-      <c r="I169" s="111"/>
-      <c r="J169" s="111"/>
+      <c r="H169" s="112"/>
+      <c r="I169" s="112"/>
+      <c r="J169" s="112"/>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="22"/>
@@ -12214,12 +12352,12 @@
       <c r="E173" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G173" s="111" t="s">
+      <c r="G173" s="112" t="s">
         <v>293</v>
       </c>
-      <c r="H173" s="111"/>
-      <c r="I173" s="111"/>
-      <c r="J173" s="111"/>
+      <c r="H173" s="112"/>
+      <c r="I173" s="112"/>
+      <c r="J173" s="112"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="22"/>
@@ -12317,12 +12455,12 @@
       <c r="E180" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G180" s="111" t="s">
+      <c r="G180" s="112" t="s">
         <v>294</v>
       </c>
-      <c r="H180" s="111"/>
-      <c r="I180" s="111"/>
-      <c r="J180" s="111"/>
+      <c r="H180" s="112"/>
+      <c r="I180" s="112"/>
+      <c r="J180" s="112"/>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="22"/>
@@ -12431,12 +12569,12 @@
       <c r="E188" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G188" s="111" t="s">
+      <c r="G188" s="112" t="s">
         <v>585</v>
       </c>
-      <c r="H188" s="111"/>
-      <c r="I188" s="111"/>
-      <c r="J188" s="111"/>
+      <c r="H188" s="112"/>
+      <c r="I188" s="112"/>
+      <c r="J188" s="112"/>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="22"/>
@@ -12510,12 +12648,12 @@
       <c r="E193" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G193" s="111" t="s">
+      <c r="G193" s="112" t="s">
         <v>602</v>
       </c>
-      <c r="H193" s="111"/>
-      <c r="I193" s="111"/>
-      <c r="J193" s="111"/>
+      <c r="H193" s="112"/>
+      <c r="I193" s="112"/>
+      <c r="J193" s="112"/>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="22"/>
@@ -12573,12 +12711,12 @@
       <c r="E197" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G197" s="111" t="s">
+      <c r="G197" s="112" t="s">
         <v>295</v>
       </c>
-      <c r="H197" s="111"/>
-      <c r="I197" s="111"/>
-      <c r="J197" s="111"/>
+      <c r="H197" s="112"/>
+      <c r="I197" s="112"/>
+      <c r="J197" s="112"/>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="22"/>
@@ -12776,12 +12914,12 @@
       <c r="E210" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G210" s="111" t="s">
+      <c r="G210" s="112" t="s">
         <v>296</v>
       </c>
-      <c r="H210" s="111"/>
-      <c r="I210" s="111"/>
-      <c r="J210" s="111"/>
+      <c r="H210" s="112"/>
+      <c r="I210" s="112"/>
+      <c r="J210" s="112"/>
     </row>
     <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="22"/>
@@ -12858,29 +12996,26 @@
     </row>
   </sheetData>
   <mergeCells count="59">
-    <mergeCell ref="G210:J210"/>
-    <mergeCell ref="G156:J156"/>
-    <mergeCell ref="G169:J169"/>
-    <mergeCell ref="G173:J173"/>
-    <mergeCell ref="G180:J180"/>
-    <mergeCell ref="G197:J197"/>
-    <mergeCell ref="G193:J193"/>
-    <mergeCell ref="G188:J188"/>
-    <mergeCell ref="G116:J116"/>
-    <mergeCell ref="G131:J131"/>
-    <mergeCell ref="G166:J166"/>
-    <mergeCell ref="G167:J167"/>
-    <mergeCell ref="G168:J168"/>
-    <mergeCell ref="G162:J162"/>
-    <mergeCell ref="G151:J151"/>
-    <mergeCell ref="G146:J146"/>
-    <mergeCell ref="G147:J147"/>
-    <mergeCell ref="G132:J132"/>
-    <mergeCell ref="G86:J86"/>
-    <mergeCell ref="G91:J91"/>
-    <mergeCell ref="G96:J96"/>
-    <mergeCell ref="G103:J103"/>
-    <mergeCell ref="G108:J108"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="G63:J63"/>
+    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="G66:J66"/>
+    <mergeCell ref="G70:J70"/>
+    <mergeCell ref="G75:J75"/>
+    <mergeCell ref="G78:J78"/>
+    <mergeCell ref="G79:J79"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="A2:E2"/>
     <mergeCell ref="B89:E89"/>
     <mergeCell ref="G15:J15"/>
     <mergeCell ref="G19:J19"/>
@@ -12897,26 +13032,29 @@
     <mergeCell ref="G50:J50"/>
     <mergeCell ref="G51:J51"/>
     <mergeCell ref="G52:J52"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="G63:J63"/>
-    <mergeCell ref="G64:J64"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="G66:J66"/>
-    <mergeCell ref="G70:J70"/>
-    <mergeCell ref="G75:J75"/>
-    <mergeCell ref="G78:J78"/>
-    <mergeCell ref="G79:J79"/>
+    <mergeCell ref="G86:J86"/>
+    <mergeCell ref="G91:J91"/>
+    <mergeCell ref="G96:J96"/>
+    <mergeCell ref="G103:J103"/>
+    <mergeCell ref="G108:J108"/>
+    <mergeCell ref="G116:J116"/>
+    <mergeCell ref="G131:J131"/>
+    <mergeCell ref="G166:J166"/>
+    <mergeCell ref="G167:J167"/>
+    <mergeCell ref="G168:J168"/>
+    <mergeCell ref="G162:J162"/>
+    <mergeCell ref="G151:J151"/>
+    <mergeCell ref="G146:J146"/>
+    <mergeCell ref="G147:J147"/>
+    <mergeCell ref="G132:J132"/>
+    <mergeCell ref="G210:J210"/>
+    <mergeCell ref="G156:J156"/>
+    <mergeCell ref="G169:J169"/>
+    <mergeCell ref="G173:J173"/>
+    <mergeCell ref="G180:J180"/>
+    <mergeCell ref="G197:J197"/>
+    <mergeCell ref="G193:J193"/>
+    <mergeCell ref="G188:J188"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Baselines and Templates
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="-3540" windowWidth="10065" windowHeight="12525" activeTab="1"/>
+    <workbookView xWindow="12510" yWindow="-3540" windowWidth="10065" windowHeight="12525" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATION" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="649">
   <si>
     <t>SSP</t>
   </si>
@@ -1827,9 +1827,6 @@
     <t>OSCAL prop fields, part assmblies, and annotation  assemblies must have a name flag set.</t>
   </si>
   <si>
-    <t>The following have become part of the core OSCAL syntax. As a result, the FedRAMP extension has been depreciated.</t>
-  </si>
-  <si>
     <t>doc-id</t>
   </si>
   <si>
@@ -2134,9 +2131,6 @@
     <t>system-id</t>
   </si>
   <si>
-    <t>/*/back-matter/resource/prop[@name="baseline"][@ns="https://fedramp.gov/ns/oscal"]</t>
-  </si>
-  <si>
     <t>When no OSCAL-based SSP exists, this is used to identify the system's short name.</t>
   </si>
   <si>
@@ -2173,12 +2167,6 @@
     <t>Backup or Alternate Data Center</t>
   </si>
   <si>
-    <t>baseline-resource-id</t>
-  </si>
-  <si>
-    <t>Resource ID of the Applicable Baseline</t>
-  </si>
-  <si>
     <t>Sampling</t>
   </si>
   <si>
@@ -2197,21 +2185,6 @@
     <t>Sampling [will not be used  | was not used] in the assessment.</t>
   </si>
   <si>
-    <t>fedramp-high-baseline</t>
-  </si>
-  <si>
-    <t>fedramp-moderate-baseline</t>
-  </si>
-  <si>
-    <t>Use the FedRAMP High Baseline</t>
-  </si>
-  <si>
-    <t>Use the FedRAMP Moderate Baseline</t>
-  </si>
-  <si>
-    <t>Use the FedRAMP Low Baseline</t>
-  </si>
-  <si>
     <t xml:space="preserve">** NOTE: All other previously defined party IDs have been eliminated. Tool developers are free to use any party ID they see fit, provided the parties are linked to the appropriate roles as defined above. </t>
   </si>
   <si>
@@ -2333,6 +2306,24 @@
   </si>
   <si>
     <t>/*/back-matter/resource/prop[@name="purpose"][@ns="https://fedramp.gov/ns/oscal"]</t>
+  </si>
+  <si>
+    <t>/*/back-matter/resource/prop[@name="baseline-uri"][@ns="https://fedramp.gov/ns/oscal"]</t>
+  </si>
+  <si>
+    <t>URI</t>
+  </si>
+  <si>
+    <t>When no OSCAL-based SSP exists, this is used to identify the appropriate FedRAMP Baseline (profile).</t>
+  </si>
+  <si>
+    <t>Import Profile (URI to Baseline)</t>
+  </si>
+  <si>
+    <t>import-profile</t>
+  </si>
+  <si>
+    <t>The following have become part of the core OSCAL syntax. As a result they are no longer considered extensions, and the @ns flag is no longer necessary.</t>
   </si>
 </sst>
 </file>
@@ -3170,11 +3161,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3678,7 +3669,7 @@
         <v>43983</v>
       </c>
       <c r="B18" s="67" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C18" s="67" t="s">
         <v>429</v>
@@ -3760,10 +3751,10 @@
   <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="7" ySplit="3" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="3" topLeftCell="H55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J69" sqref="J69"/>
+      <selection pane="bottomRight" activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3790,7 +3781,7 @@
       <c r="H1" s="108"/>
       <c r="I1" s="108"/>
       <c r="J1" s="91" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3816,12 +3807,12 @@
         <v>316</v>
       </c>
       <c r="M2" s="107" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
@@ -3871,7 +3862,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="H4" s="78" t="s">
         <v>28</v>
@@ -3881,13 +3872,13 @@
         <v>conformity</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O4" s="6"/>
     </row>
@@ -3915,22 +3906,22 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="H6" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="78" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="J6" s="83" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="O6" s="6"/>
     </row>
@@ -3958,7 +3949,7 @@
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>612</v>
+        <v>603</v>
       </c>
       <c r="H8" s="78" t="s">
         <v>28</v>
@@ -3967,13 +3958,13 @@
         <v>434</v>
       </c>
       <c r="J8" s="93" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="O8" s="6"/>
     </row>
@@ -4001,22 +3992,22 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="H10" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I10" s="78" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
       <c r="J10" s="93" t="s">
-        <v>613</v>
+        <v>604</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="O10" s="6"/>
     </row>
@@ -4044,22 +4035,22 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="H12" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I12" s="78" t="s">
+        <v>568</v>
+      </c>
+      <c r="J12" s="87" t="s">
         <v>569</v>
-      </c>
-      <c r="J12" s="87" t="s">
-        <v>570</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="O12" s="6"/>
     </row>
@@ -5457,7 +5448,7 @@
         <v>437</v>
       </c>
       <c r="J61" s="65" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K61" s="6" t="s">
         <v>317</v>
@@ -5489,7 +5480,7 @@
         <v>436</v>
       </c>
       <c r="J62" s="65" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="K62" s="6" t="s">
         <v>388</v>
@@ -5522,22 +5513,22 @@
         <v>10</v>
       </c>
       <c r="G64" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H64" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I64" s="78" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="J64" s="89" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K64" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N64" s="4" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -5557,22 +5548,22 @@
         <v>10</v>
       </c>
       <c r="G65" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H65" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I65" s="78" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="J65" s="89" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="K65" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N65" s="4" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="66" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -5592,25 +5583,22 @@
         <v>10</v>
       </c>
       <c r="G66" t="s">
-        <v>599</v>
+        <v>646</v>
       </c>
       <c r="H66" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I66" s="78" t="s">
-        <v>598</v>
+        <v>647</v>
       </c>
       <c r="J66" s="90" t="s">
-        <v>585</v>
+        <v>643</v>
       </c>
       <c r="K66" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="M66" s="6" t="s">
-        <v>23</v>
+        <v>644</v>
       </c>
       <c r="N66" s="4" t="s">
-        <v>588</v>
+        <v>645</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -5626,26 +5614,26 @@
       <c r="D67" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E67" s="6" t="s">
-        <v>10</v>
+      <c r="E67" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G67" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
       <c r="H67" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I67" s="78" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="J67" s="97" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="K67" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N67" s="4" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="68" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -5661,26 +5649,26 @@
       <c r="D68" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E68" s="6" t="s">
-        <v>10</v>
+      <c r="E68" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G68" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="H68" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I68" s="78" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
       <c r="J68" s="97" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="K68" s="6" t="s">
         <v>388</v>
       </c>
       <c r="N68" s="4" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="69" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -5696,20 +5684,20 @@
       <c r="D69" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E69" s="6" t="s">
-        <v>10</v>
+      <c r="E69" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G69" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
       <c r="H69" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I69" s="78" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
       <c r="J69" s="97" t="s">
-        <v>649</v>
+        <v>640</v>
       </c>
       <c r="K69" s="6" t="s">
         <v>388</v>
@@ -5718,7 +5706,7 @@
         <v>23</v>
       </c>
       <c r="N69" s="4" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="70" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -5748,16 +5736,16 @@
         <v>7</v>
       </c>
       <c r="G71" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="H71" s="78" t="s">
         <v>28</v>
       </c>
       <c r="I71" s="78" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="J71" s="93" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="K71" s="6" t="s">
         <v>388</v>
@@ -5766,7 +5754,7 @@
         <v>23</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="72" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -5786,7 +5774,7 @@
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G74" s="82" t="s">
-        <v>502</v>
+        <v>648</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
@@ -5816,7 +5804,7 @@
         <v>73</v>
       </c>
       <c r="H77" s="78" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I77" s="3" t="s">
         <v>7</v>
@@ -5824,7 +5812,7 @@
     </row>
     <row r="83" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G83" s="82" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="84" spans="7:9" x14ac:dyDescent="0.25">
@@ -5941,7 +5929,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
@@ -7217,7 +7205,7 @@
         <v>All FedRAMP Compliance tags must use name='conformity', as well as ns='https://fedramp.gov/ns/oscal'</v>
       </c>
       <c r="P1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -7237,12 +7225,12 @@
         <v>468</v>
       </c>
       <c r="P2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
@@ -7260,13 +7248,13 @@
         <v>431</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I3" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="J3" s="20" t="s">
         <v>505</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>506</v>
       </c>
       <c r="K3" s="53" t="s">
         <v>8</v>
@@ -7297,13 +7285,13 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
+        <v>572</v>
+      </c>
+      <c r="H5" s="84" t="s">
         <v>573</v>
       </c>
-      <c r="H5" s="84" t="s">
+      <c r="I5" s="79" t="s">
         <v>574</v>
-      </c>
-      <c r="I5" s="79" t="s">
-        <v>575</v>
       </c>
       <c r="J5" s="88" t="str">
         <f>CONCATENATE(I5,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H5,"']/..")</f>
@@ -7339,20 +7327,20 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
+        <v>507</v>
+      </c>
+      <c r="H7" s="84" t="s">
         <v>508</v>
       </c>
-      <c r="H7" s="84" t="s">
+      <c r="I7" s="79" t="s">
         <v>509</v>
-      </c>
-      <c r="I7" s="79" t="s">
-        <v>510</v>
       </c>
       <c r="J7" s="83" t="str">
         <f>CONCATENATE(I7,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H7,"']/..")</f>
         <v>/*/metadata/location/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='primary-data-center']/..</v>
       </c>
       <c r="K7" s="111" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="L7" s="83" t="str">
         <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H7,"&lt;/prop&gt;")</f>
@@ -7376,13 +7364,13 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="H8" s="84" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="I8" s="79" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="J8" s="83" t="str">
         <f>CONCATENATE(I8,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H8,"']/..")</f>
@@ -7422,13 +7410,13 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="I10" s="79" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="J10" s="83" t="str">
         <f>CONCATENATE(I10,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H10,"']/..")</f>
@@ -7467,13 +7455,13 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="I12" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J12" s="83" t="str">
         <f t="shared" ref="J12:J29" si="0">CONCATENATE(I12,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H12,"']/..")</f>
@@ -7501,13 +7489,13 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="I13" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J13" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7535,13 +7523,13 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
+        <v>560</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>562</v>
-      </c>
       <c r="I14" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J14" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7569,13 +7557,13 @@
         <v>5</v>
       </c>
       <c r="G15" t="s">
+        <v>562</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>563</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>564</v>
-      </c>
       <c r="I15" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J15" s="85" t="str">
         <f t="shared" si="0"/>
@@ -7603,13 +7591,13 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
+        <v>528</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>529</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>530</v>
-      </c>
       <c r="I16" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J16" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7637,13 +7625,13 @@
         <v>7</v>
       </c>
       <c r="G17" s="54" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>119</v>
       </c>
       <c r="I17" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J17" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7671,13 +7659,13 @@
         <v>7</v>
       </c>
       <c r="G18" s="54" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="I18" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J18" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7705,13 +7693,13 @@
         <v>7</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="I19" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J19" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7739,13 +7727,13 @@
         <v>7</v>
       </c>
       <c r="G20" s="54" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="I20" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J20" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7773,13 +7761,13 @@
         <v>7</v>
       </c>
       <c r="G21" s="54" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="I21" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J21" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7807,13 +7795,13 @@
         <v>7</v>
       </c>
       <c r="G22" s="54" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="I22" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J22" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7841,13 +7829,13 @@
         <v>7</v>
       </c>
       <c r="G23" s="54" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I23" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J23" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7875,13 +7863,13 @@
         <v>7</v>
       </c>
       <c r="G24" s="54" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I24" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J24" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7909,13 +7897,13 @@
         <v>1</v>
       </c>
       <c r="G25" s="54" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="I25" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J25" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7943,13 +7931,13 @@
         <v>1</v>
       </c>
       <c r="G26" s="54" t="s">
+        <v>548</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="I26" s="79" t="s">
         <v>549</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="I26" s="79" t="s">
-        <v>550</v>
       </c>
       <c r="J26" s="83" t="str">
         <f t="shared" si="0"/>
@@ -7977,13 +7965,13 @@
         <v>10</v>
       </c>
       <c r="G27" s="54" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="I27" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J27" s="83" t="str">
         <f t="shared" si="0"/>
@@ -8011,13 +7999,13 @@
         <v>6</v>
       </c>
       <c r="G28" s="54" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="I28" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J28" s="83" t="str">
         <f t="shared" si="0"/>
@@ -8045,13 +8033,13 @@
         <v>10</v>
       </c>
       <c r="G29" s="54" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I29" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J29" s="89" t="str">
         <f t="shared" si="0"/>
@@ -8079,13 +8067,13 @@
         <v>7</v>
       </c>
       <c r="G30" s="54" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>637</v>
+        <v>628</v>
       </c>
       <c r="I30" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J30" s="96" t="str">
         <f t="shared" ref="J30" si="3">CONCATENATE(I30,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H30,"']/..")</f>
@@ -8113,13 +8101,13 @@
         <v>7</v>
       </c>
       <c r="G31" s="54" t="s">
-        <v>636</v>
+        <v>627</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="I31" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J31" s="96" t="str">
         <f t="shared" ref="J31" si="5">CONCATENATE(I31,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H31,"']/..")</f>
@@ -8147,13 +8135,13 @@
         <v>7</v>
       </c>
       <c r="G32" s="54" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="H32" s="98" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="I32" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J32" s="96" t="str">
         <f t="shared" ref="J32" si="7">CONCATENATE(I32,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H32,"']/..")</f>
@@ -8181,13 +8169,13 @@
         <v>7</v>
       </c>
       <c r="G33" s="54" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="H33" s="98" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
       <c r="I33" s="79" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J33" s="96" t="str">
         <f t="shared" ref="J33" si="9">CONCATENATE(I33,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H33,"']/..")</f>
@@ -8216,7 +8204,7 @@
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="H36" s="86" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -8241,13 +8229,13 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H40" s="84" t="s">
         <v>202</v>
       </c>
       <c r="I40" s="79" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J40" s="66" t="str">
         <f>CONCATENATE(I40,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H40,"']/..")</f>
@@ -8281,7 +8269,7 @@
         <v>203</v>
       </c>
       <c r="I41" s="79" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J41" s="83" t="str">
         <f>CONCATENATE(I41,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H41,"']/..")</f>
@@ -8309,13 +8297,13 @@
         <v>1</v>
       </c>
       <c r="G42" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H42" s="84" t="s">
         <v>9</v>
       </c>
       <c r="I42" s="79" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="J42" s="83" t="str">
         <f>CONCATENATE(I42,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H42,"']/..")</f>
@@ -8389,7 +8377,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
@@ -8454,7 +8442,7 @@
         <v>187</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="Q5" s="1"/>
     </row>
@@ -8481,7 +8469,7 @@
         <v>188</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="Q6" s="1"/>
     </row>
@@ -8508,7 +8496,7 @@
         <v>189</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="Q7" s="1"/>
     </row>
@@ -9110,7 +9098,7 @@
         <v>23</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>160</v>
@@ -9136,10 +9124,10 @@
         <v>23</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -9162,10 +9150,10 @@
         <v>23</v>
       </c>
       <c r="I31" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="J31" s="4" t="s">
         <v>514</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -9188,10 +9176,10 @@
         <v>23</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>614</v>
+        <v>605</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -9214,10 +9202,10 @@
         <v>23</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>615</v>
+        <v>606</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -9240,10 +9228,10 @@
         <v>23</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>616</v>
+        <v>607</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -9266,10 +9254,10 @@
         <v>23</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -9292,10 +9280,10 @@
         <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -9318,10 +9306,10 @@
         <v>23</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -9344,10 +9332,10 @@
         <v>23</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>630</v>
+        <v>621</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -9370,10 +9358,10 @@
         <v>23</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>631</v>
+        <v>622</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>633</v>
+        <v>624</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -9396,10 +9384,10 @@
         <v>23</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>632</v>
+        <v>623</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>634</v>
+        <v>625</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -9466,12 +9454,12 @@
         <v>9</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>611</v>
+        <v>602</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -9482,7 +9470,7 @@
       <c r="E47" s="94"/>
       <c r="F47" s="27"/>
       <c r="G47" s="94" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="H47" s="94"/>
       <c r="I47" s="94"/>
@@ -9561,11 +9549,11 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:J217"/>
+  <dimension ref="A1:J212"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J192" sqref="J192"/>
+      <pane ySplit="3" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F188" sqref="A188:XFD192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9609,7 +9597,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>0</v>
@@ -9652,12 +9640,12 @@
       <c r="E4" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="112" t="s">
+      <c r="G4" s="113" t="s">
         <v>322</v>
       </c>
-      <c r="H4" s="112"/>
-      <c r="I4" s="112"/>
-      <c r="J4" s="112"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
+      <c r="J4" s="113"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="30" t="s">
@@ -9675,12 +9663,12 @@
       <c r="E5" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="112" t="s">
+      <c r="G5" s="113" t="s">
         <v>321</v>
       </c>
-      <c r="H5" s="112"/>
-      <c r="I5" s="112"/>
-      <c r="J5" s="112"/>
+      <c r="H5" s="113"/>
+      <c r="I5" s="113"/>
+      <c r="J5" s="113"/>
     </row>
     <row r="6" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="51"/>
@@ -9741,12 +9729,12 @@
       <c r="E9" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="112" t="s">
+      <c r="G9" s="113" t="s">
         <v>328</v>
       </c>
-      <c r="H9" s="112"/>
-      <c r="I9" s="112"/>
-      <c r="J9" s="112"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
     </row>
     <row r="10" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
@@ -9764,12 +9752,12 @@
       <c r="E10" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="112" t="s">
+      <c r="G10" s="113" t="s">
         <v>327</v>
       </c>
-      <c r="H10" s="112"/>
-      <c r="I10" s="112"/>
-      <c r="J10" s="112"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="113"/>
+      <c r="J10" s="113"/>
     </row>
     <row r="11" spans="1:10" s="48" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="51"/>
@@ -9846,12 +9834,12 @@
       <c r="E15" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="112" t="s">
+      <c r="G15" s="113" t="s">
         <v>264</v>
       </c>
-      <c r="H15" s="112"/>
-      <c r="I15" s="112"/>
-      <c r="J15" s="112"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
@@ -9912,12 +9900,12 @@
       <c r="E19" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="112" t="s">
+      <c r="G19" s="113" t="s">
         <v>265</v>
       </c>
-      <c r="H19" s="112"/>
-      <c r="I19" s="112"/>
-      <c r="J19" s="112"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="113"/>
+      <c r="J19" s="113"/>
     </row>
     <row r="20" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="31" t="s">
@@ -9935,12 +9923,12 @@
       <c r="E20" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="112" t="s">
+      <c r="G20" s="113" t="s">
         <v>266</v>
       </c>
-      <c r="H20" s="112"/>
-      <c r="I20" s="112"/>
-      <c r="J20" s="112"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="113"/>
+      <c r="J20" s="113"/>
     </row>
     <row r="21" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="31" t="s">
@@ -9958,12 +9946,12 @@
       <c r="E21" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="112" t="s">
+      <c r="G21" s="113" t="s">
         <v>267</v>
       </c>
-      <c r="H21" s="112"/>
-      <c r="I21" s="112"/>
-      <c r="J21" s="112"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
     </row>
     <row r="22" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
@@ -9981,12 +9969,12 @@
       <c r="E22" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="112" t="s">
+      <c r="G22" s="113" t="s">
         <v>268</v>
       </c>
-      <c r="H22" s="112"/>
-      <c r="I22" s="112"/>
-      <c r="J22" s="112"/>
+      <c r="H22" s="113"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="113"/>
     </row>
     <row r="23" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
@@ -10063,12 +10051,12 @@
       <c r="E27" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G27" s="112" t="s">
+      <c r="G27" s="113" t="s">
         <v>269</v>
       </c>
-      <c r="H27" s="112"/>
-      <c r="I27" s="112"/>
-      <c r="J27" s="112"/>
+      <c r="H27" s="113"/>
+      <c r="I27" s="113"/>
+      <c r="J27" s="113"/>
     </row>
     <row r="28" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="22"/>
@@ -10148,12 +10136,12 @@
       <c r="E32" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G32" s="112" t="s">
+      <c r="G32" s="113" t="s">
         <v>318</v>
       </c>
-      <c r="H32" s="112"/>
-      <c r="I32" s="112"/>
-      <c r="J32" s="112"/>
+      <c r="H32" s="113"/>
+      <c r="I32" s="113"/>
+      <c r="J32" s="113"/>
     </row>
     <row r="33" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="22"/>
@@ -10246,12 +10234,12 @@
       <c r="E38" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="G38" s="112" t="s">
+      <c r="G38" s="113" t="s">
         <v>270</v>
       </c>
-      <c r="H38" s="112"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
+      <c r="H38" s="113"/>
+      <c r="I38" s="113"/>
+      <c r="J38" s="113"/>
     </row>
     <row r="39" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22"/>
@@ -10286,12 +10274,12 @@
       </c>
     </row>
     <row r="41" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="113" t="s">
+      <c r="B41" s="112" t="s">
         <v>248</v>
       </c>
-      <c r="C41" s="113"/>
-      <c r="D41" s="113"/>
-      <c r="E41" s="113"/>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
       <c r="G41" s="15" t="s">
         <v>23</v>
       </c>
@@ -10379,12 +10367,12 @@
       <c r="E46" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G46" s="112" t="s">
+      <c r="G46" s="113" t="s">
         <v>271</v>
       </c>
-      <c r="H46" s="112"/>
-      <c r="I46" s="112"/>
-      <c r="J46" s="112"/>
+      <c r="H46" s="113"/>
+      <c r="I46" s="113"/>
+      <c r="J46" s="113"/>
     </row>
     <row r="47" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="31" t="s">
@@ -10402,12 +10390,12 @@
       <c r="E47" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G47" s="112" t="s">
+      <c r="G47" s="113" t="s">
         <v>272</v>
       </c>
-      <c r="H47" s="112"/>
-      <c r="I47" s="112"/>
-      <c r="J47" s="112"/>
+      <c r="H47" s="113"/>
+      <c r="I47" s="113"/>
+      <c r="J47" s="113"/>
     </row>
     <row r="48" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="31" t="s">
@@ -10425,12 +10413,12 @@
       <c r="E48" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G48" s="112" t="s">
+      <c r="G48" s="113" t="s">
         <v>273</v>
       </c>
-      <c r="H48" s="112"/>
-      <c r="I48" s="112"/>
-      <c r="J48" s="112"/>
+      <c r="H48" s="113"/>
+      <c r="I48" s="113"/>
+      <c r="J48" s="113"/>
     </row>
     <row r="49" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="31" t="s">
@@ -10448,12 +10436,12 @@
       <c r="E49" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G49" s="112" t="s">
+      <c r="G49" s="113" t="s">
         <v>274</v>
       </c>
-      <c r="H49" s="112"/>
-      <c r="I49" s="112"/>
-      <c r="J49" s="112"/>
+      <c r="H49" s="113"/>
+      <c r="I49" s="113"/>
+      <c r="J49" s="113"/>
     </row>
     <row r="50" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="31" t="s">
@@ -10471,12 +10459,12 @@
       <c r="E50" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G50" s="112" t="s">
+      <c r="G50" s="113" t="s">
         <v>275</v>
       </c>
-      <c r="H50" s="112"/>
-      <c r="I50" s="112"/>
-      <c r="J50" s="112"/>
+      <c r="H50" s="113"/>
+      <c r="I50" s="113"/>
+      <c r="J50" s="113"/>
     </row>
     <row r="51" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="31" t="s">
@@ -10494,12 +10482,12 @@
       <c r="E51" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G51" s="112" t="s">
+      <c r="G51" s="113" t="s">
         <v>276</v>
       </c>
-      <c r="H51" s="112"/>
-      <c r="I51" s="112"/>
-      <c r="J51" s="112"/>
+      <c r="H51" s="113"/>
+      <c r="I51" s="113"/>
+      <c r="J51" s="113"/>
     </row>
     <row r="52" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="31" t="s">
@@ -10517,12 +10505,12 @@
       <c r="E52" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G52" s="112" t="s">
+      <c r="G52" s="113" t="s">
         <v>277</v>
       </c>
-      <c r="H52" s="112"/>
-      <c r="I52" s="112"/>
-      <c r="J52" s="112"/>
+      <c r="H52" s="113"/>
+      <c r="I52" s="113"/>
+      <c r="J52" s="113"/>
     </row>
     <row r="53" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" s="31" t="s">
@@ -10540,12 +10528,12 @@
       <c r="E53" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G53" s="112" t="s">
+      <c r="G53" s="113" t="s">
         <v>278</v>
       </c>
-      <c r="H53" s="112"/>
-      <c r="I53" s="112"/>
-      <c r="J53" s="112"/>
+      <c r="H53" s="113"/>
+      <c r="I53" s="113"/>
+      <c r="J53" s="113"/>
     </row>
     <row r="54" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A54" s="31" t="s">
@@ -10563,12 +10551,12 @@
       <c r="E54" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G54" s="112" t="s">
+      <c r="G54" s="113" t="s">
         <v>279</v>
       </c>
-      <c r="H54" s="112"/>
-      <c r="I54" s="112"/>
-      <c r="J54" s="112"/>
+      <c r="H54" s="113"/>
+      <c r="I54" s="113"/>
+      <c r="J54" s="113"/>
     </row>
     <row r="55" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="22"/>
@@ -10642,12 +10630,12 @@
       <c r="E59" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G59" s="112" t="s">
+      <c r="G59" s="113" t="s">
         <v>280</v>
       </c>
-      <c r="H59" s="112"/>
-      <c r="I59" s="112"/>
-      <c r="J59" s="112"/>
+      <c r="H59" s="113"/>
+      <c r="I59" s="113"/>
+      <c r="J59" s="113"/>
     </row>
     <row r="60" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22"/>
@@ -10708,12 +10696,12 @@
       <c r="E63" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G63" s="112" t="s">
+      <c r="G63" s="113" t="s">
         <v>281</v>
       </c>
-      <c r="H63" s="112"/>
-      <c r="I63" s="112"/>
-      <c r="J63" s="112"/>
+      <c r="H63" s="113"/>
+      <c r="I63" s="113"/>
+      <c r="J63" s="113"/>
     </row>
     <row r="64" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A64" s="31" t="s">
@@ -10731,12 +10719,12 @@
       <c r="E64" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G64" s="112" t="s">
+      <c r="G64" s="113" t="s">
         <v>282</v>
       </c>
-      <c r="H64" s="112"/>
-      <c r="I64" s="112"/>
-      <c r="J64" s="112"/>
+      <c r="H64" s="113"/>
+      <c r="I64" s="113"/>
+      <c r="J64" s="113"/>
     </row>
     <row r="65" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65" s="31" t="s">
@@ -10754,12 +10742,12 @@
       <c r="E65" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G65" s="112" t="s">
+      <c r="G65" s="113" t="s">
         <v>283</v>
       </c>
-      <c r="H65" s="112"/>
-      <c r="I65" s="112"/>
-      <c r="J65" s="112"/>
+      <c r="H65" s="113"/>
+      <c r="I65" s="113"/>
+      <c r="J65" s="113"/>
     </row>
     <row r="66" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A66" s="31" t="s">
@@ -10777,12 +10765,12 @@
       <c r="E66" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G66" s="112" t="s">
+      <c r="G66" s="113" t="s">
         <v>284</v>
       </c>
-      <c r="H66" s="112"/>
-      <c r="I66" s="112"/>
-      <c r="J66" s="112"/>
+      <c r="H66" s="113"/>
+      <c r="I66" s="113"/>
+      <c r="J66" s="113"/>
     </row>
     <row r="67" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="22"/>
@@ -10839,12 +10827,12 @@
       <c r="E70" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="G70" s="112" t="s">
+      <c r="G70" s="113" t="s">
         <v>285</v>
       </c>
-      <c r="H70" s="112"/>
-      <c r="I70" s="112"/>
-      <c r="J70" s="112"/>
+      <c r="H70" s="113"/>
+      <c r="I70" s="113"/>
+      <c r="J70" s="113"/>
     </row>
     <row r="71" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22"/>
@@ -10918,12 +10906,12 @@
       <c r="E75" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G75" s="112" t="s">
+      <c r="G75" s="113" t="s">
         <v>320</v>
       </c>
-      <c r="H75" s="112"/>
-      <c r="I75" s="112"/>
-      <c r="J75" s="112"/>
+      <c r="H75" s="113"/>
+      <c r="I75" s="113"/>
+      <c r="J75" s="113"/>
     </row>
     <row r="76" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="22"/>
@@ -10968,12 +10956,12 @@
       <c r="E78" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G78" s="112" t="s">
+      <c r="G78" s="113" t="s">
         <v>286</v>
       </c>
-      <c r="H78" s="112"/>
-      <c r="I78" s="112"/>
-      <c r="J78" s="112"/>
+      <c r="H78" s="113"/>
+      <c r="I78" s="113"/>
+      <c r="J78" s="113"/>
     </row>
     <row r="79" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A79" s="30" t="s">
@@ -10991,12 +10979,12 @@
       <c r="E79" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G79" s="112" t="s">
+      <c r="G79" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="H79" s="112"/>
-      <c r="I79" s="112"/>
-      <c r="J79" s="112"/>
+      <c r="H79" s="113"/>
+      <c r="I79" s="113"/>
+      <c r="J79" s="113"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="22"/>
@@ -11012,12 +11000,12 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="113" t="s">
+      <c r="B81" s="112" t="s">
         <v>248</v>
       </c>
-      <c r="C81" s="113"/>
-      <c r="D81" s="113"/>
-      <c r="E81" s="113"/>
+      <c r="C81" s="112"/>
+      <c r="D81" s="112"/>
+      <c r="E81" s="112"/>
       <c r="G81" s="33" t="s">
         <v>23</v>
       </c>
@@ -11045,12 +11033,12 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="113" t="s">
+      <c r="B83" s="112" t="s">
         <v>248</v>
       </c>
-      <c r="C83" s="113"/>
-      <c r="D83" s="113"/>
-      <c r="E83" s="113"/>
+      <c r="C83" s="112"/>
+      <c r="D83" s="112"/>
+      <c r="E83" s="112"/>
       <c r="G83" s="33" t="s">
         <v>23</v>
       </c>
@@ -11093,12 +11081,12 @@
       <c r="E86" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G86" s="112" t="s">
+      <c r="G86" s="113" t="s">
         <v>288</v>
       </c>
-      <c r="H86" s="112"/>
-      <c r="I86" s="112"/>
-      <c r="J86" s="112"/>
+      <c r="H86" s="113"/>
+      <c r="I86" s="113"/>
+      <c r="J86" s="113"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="22"/>
@@ -11128,12 +11116,12 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="37"/>
-      <c r="B89" s="113" t="s">
+      <c r="B89" s="112" t="s">
         <v>248</v>
       </c>
-      <c r="C89" s="113"/>
-      <c r="D89" s="113"/>
-      <c r="E89" s="113"/>
+      <c r="C89" s="112"/>
+      <c r="D89" s="112"/>
+      <c r="E89" s="112"/>
       <c r="F89" s="37"/>
       <c r="G89" s="33" t="s">
         <v>23</v>
@@ -11160,12 +11148,12 @@
       <c r="E91" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G91" s="112" t="s">
+      <c r="G91" s="113" t="s">
         <v>319</v>
       </c>
-      <c r="H91" s="112"/>
-      <c r="I91" s="112"/>
-      <c r="J91" s="112"/>
+      <c r="H91" s="113"/>
+      <c r="I91" s="113"/>
+      <c r="J91" s="113"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="22"/>
@@ -11222,12 +11210,12 @@
       <c r="E96" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G96" s="112" t="s">
+      <c r="G96" s="113" t="s">
         <v>289</v>
       </c>
-      <c r="H96" s="112"/>
-      <c r="I96" s="112"/>
-      <c r="J96" s="112"/>
+      <c r="H96" s="113"/>
+      <c r="I96" s="113"/>
+      <c r="J96" s="113"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="22"/>
@@ -11316,12 +11304,12 @@
       <c r="E103" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G103" s="112" t="s">
+      <c r="G103" s="113" t="s">
         <v>290</v>
       </c>
-      <c r="H103" s="112"/>
-      <c r="I103" s="112"/>
-      <c r="J103" s="112"/>
+      <c r="H103" s="113"/>
+      <c r="I103" s="113"/>
+      <c r="J103" s="113"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="22"/>
@@ -11391,12 +11379,12 @@
       <c r="E108" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G108" s="112" t="s">
+      <c r="G108" s="113" t="s">
         <v>291</v>
       </c>
-      <c r="H108" s="112"/>
-      <c r="I108" s="112"/>
-      <c r="J108" s="112"/>
+      <c r="H108" s="113"/>
+      <c r="I108" s="113"/>
+      <c r="J108" s="113"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="22"/>
@@ -11500,12 +11488,12 @@
       <c r="E116" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G116" s="112" t="s">
+      <c r="G116" s="113" t="s">
         <v>292</v>
       </c>
-      <c r="H116" s="112"/>
-      <c r="I116" s="112"/>
-      <c r="J116" s="112"/>
+      <c r="H116" s="113"/>
+      <c r="I116" s="113"/>
+      <c r="J116" s="113"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="22"/>
@@ -11718,12 +11706,12 @@
       <c r="E131" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G131" s="112" t="s">
+      <c r="G131" s="113" t="s">
         <v>336</v>
       </c>
-      <c r="H131" s="112"/>
-      <c r="I131" s="112"/>
-      <c r="J131" s="112"/>
+      <c r="H131" s="113"/>
+      <c r="I131" s="113"/>
+      <c r="J131" s="113"/>
     </row>
     <row r="132" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A132" s="30" t="s">
@@ -11741,12 +11729,12 @@
       <c r="E132" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G132" s="112" t="s">
+      <c r="G132" s="113" t="s">
         <v>376</v>
       </c>
-      <c r="H132" s="112"/>
-      <c r="I132" s="112"/>
-      <c r="J132" s="112"/>
+      <c r="H132" s="113"/>
+      <c r="I132" s="113"/>
+      <c r="J132" s="113"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="22"/>
@@ -11931,12 +11919,12 @@
       <c r="E146" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G146" s="112" t="s">
+      <c r="G146" s="113" t="s">
         <v>353</v>
       </c>
-      <c r="H146" s="112"/>
-      <c r="I146" s="112"/>
-      <c r="J146" s="112"/>
+      <c r="H146" s="113"/>
+      <c r="I146" s="113"/>
+      <c r="J146" s="113"/>
     </row>
     <row r="147" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A147" s="30" t="s">
@@ -11954,12 +11942,12 @@
       <c r="E147" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G147" s="112" t="s">
+      <c r="G147" s="113" t="s">
         <v>354</v>
       </c>
-      <c r="H147" s="112"/>
-      <c r="I147" s="112"/>
-      <c r="J147" s="112"/>
+      <c r="H147" s="113"/>
+      <c r="I147" s="113"/>
+      <c r="J147" s="113"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="22"/>
@@ -12006,12 +11994,12 @@
       <c r="E151" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G151" s="112" t="s">
+      <c r="G151" s="113" t="s">
         <v>339</v>
       </c>
-      <c r="H151" s="112"/>
-      <c r="I151" s="112"/>
-      <c r="J151" s="112"/>
+      <c r="H151" s="113"/>
+      <c r="I151" s="113"/>
+      <c r="J151" s="113"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="22"/>
@@ -12085,12 +12073,12 @@
       <c r="E156" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G156" s="112" t="s">
+      <c r="G156" s="113" t="s">
         <v>287</v>
       </c>
-      <c r="H156" s="112"/>
-      <c r="I156" s="112"/>
-      <c r="J156" s="112"/>
+      <c r="H156" s="113"/>
+      <c r="I156" s="113"/>
+      <c r="J156" s="113"/>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="22"/>
@@ -12172,12 +12160,12 @@
       <c r="E162" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G162" s="112" t="s">
+      <c r="G162" s="113" t="s">
         <v>333</v>
       </c>
-      <c r="H162" s="112"/>
-      <c r="I162" s="112"/>
-      <c r="J162" s="112"/>
+      <c r="H162" s="113"/>
+      <c r="I162" s="113"/>
+      <c r="J162" s="113"/>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="22"/>
@@ -12231,12 +12219,12 @@
       <c r="E166" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G166" s="112" t="s">
+      <c r="G166" s="113" t="s">
         <v>364</v>
       </c>
-      <c r="H166" s="112"/>
-      <c r="I166" s="112"/>
-      <c r="J166" s="112"/>
+      <c r="H166" s="113"/>
+      <c r="I166" s="113"/>
+      <c r="J166" s="113"/>
     </row>
     <row r="167" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A167" s="30" t="s">
@@ -12254,12 +12242,12 @@
       <c r="E167" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G167" s="112" t="s">
+      <c r="G167" s="113" t="s">
         <v>365</v>
       </c>
-      <c r="H167" s="112"/>
-      <c r="I167" s="112"/>
-      <c r="J167" s="112"/>
+      <c r="H167" s="113"/>
+      <c r="I167" s="113"/>
+      <c r="J167" s="113"/>
     </row>
     <row r="168" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A168" s="30" t="s">
@@ -12277,12 +12265,12 @@
       <c r="E168" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G168" s="112" t="s">
+      <c r="G168" s="113" t="s">
         <v>372</v>
       </c>
-      <c r="H168" s="112"/>
-      <c r="I168" s="112"/>
-      <c r="J168" s="112"/>
+      <c r="H168" s="113"/>
+      <c r="I168" s="113"/>
+      <c r="J168" s="113"/>
     </row>
     <row r="169" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A169" s="30" t="s">
@@ -12300,12 +12288,12 @@
       <c r="E169" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G169" s="112" t="s">
+      <c r="G169" s="113" t="s">
         <v>371</v>
       </c>
-      <c r="H169" s="112"/>
-      <c r="I169" s="112"/>
-      <c r="J169" s="112"/>
+      <c r="H169" s="113"/>
+      <c r="I169" s="113"/>
+      <c r="J169" s="113"/>
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="22"/>
@@ -12352,12 +12340,12 @@
       <c r="E173" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G173" s="112" t="s">
+      <c r="G173" s="113" t="s">
         <v>293</v>
       </c>
-      <c r="H173" s="112"/>
-      <c r="I173" s="112"/>
-      <c r="J173" s="112"/>
+      <c r="H173" s="113"/>
+      <c r="I173" s="113"/>
+      <c r="J173" s="113"/>
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="22"/>
@@ -12455,12 +12443,12 @@
       <c r="E180" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="G180" s="112" t="s">
+      <c r="G180" s="113" t="s">
         <v>294</v>
       </c>
-      <c r="H180" s="112"/>
-      <c r="I180" s="112"/>
-      <c r="J180" s="112"/>
+      <c r="H180" s="113"/>
+      <c r="I180" s="113"/>
+      <c r="J180" s="113"/>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="22"/>
@@ -12563,18 +12551,18 @@
       <c r="C188" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D188" s="32" t="s">
-        <v>7</v>
+      <c r="D188" s="30" t="s">
+        <v>53</v>
       </c>
       <c r="E188" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="G188" s="112" t="s">
-        <v>585</v>
-      </c>
-      <c r="H188" s="112"/>
-      <c r="I188" s="112"/>
-      <c r="J188" s="112"/>
+      <c r="G188" s="113" t="s">
+        <v>598</v>
+      </c>
+      <c r="H188" s="113"/>
+      <c r="I188" s="113"/>
+      <c r="J188" s="113"/>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="22"/>
@@ -12586,10 +12574,10 @@
         <v>23</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>606</v>
+        <v>138</v>
       </c>
       <c r="J189" s="4" t="s">
-        <v>608</v>
+        <v>600</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
@@ -12602,10 +12590,10 @@
         <v>23</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>607</v>
+        <v>139</v>
       </c>
       <c r="J190" s="4" t="s">
-        <v>609</v>
+        <v>601</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.25">
@@ -12614,109 +12602,112 @@
       <c r="C191" s="92"/>
       <c r="D191" s="92"/>
       <c r="E191" s="92"/>
-      <c r="H191" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I191" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="J191" s="4" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A192" s="22"/>
-      <c r="B192" s="22"/>
-      <c r="C192" s="92"/>
-      <c r="D192" s="92"/>
-      <c r="E192" s="92"/>
-      <c r="H192" s="13"/>
-    </row>
-    <row r="193" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A193" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B193" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C193" s="30" t="s">
+      <c r="H191" s="13"/>
+    </row>
+    <row r="192" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A192" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D193" s="30" t="s">
+      <c r="B192" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="E193" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="G193" s="112" t="s">
-        <v>602</v>
-      </c>
-      <c r="H193" s="112"/>
-      <c r="I193" s="112"/>
-      <c r="J193" s="112"/>
+      <c r="C192" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D192" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E192" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G192" s="113" t="s">
+        <v>295</v>
+      </c>
+      <c r="H192" s="113"/>
+      <c r="I192" s="113"/>
+      <c r="J192" s="113"/>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A193" s="22"/>
+      <c r="B193" s="22"/>
+      <c r="C193" s="15"/>
+      <c r="D193" s="15"/>
+      <c r="E193" s="25"/>
+      <c r="G193" s="13"/>
+      <c r="H193" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I193" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J193" s="4" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="22"/>
       <c r="B194" s="22"/>
-      <c r="C194" s="92"/>
-      <c r="D194" s="92"/>
-      <c r="E194" s="92"/>
-      <c r="H194" s="6" t="s">
+      <c r="C194" s="15"/>
+      <c r="D194" s="15"/>
+      <c r="E194" s="25"/>
+      <c r="G194" s="13"/>
+      <c r="H194" s="13" t="s">
         <v>23</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>138</v>
+        <v>76</v>
       </c>
       <c r="J194" s="4" t="s">
-        <v>604</v>
+        <v>129</v>
       </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="22"/>
       <c r="B195" s="22"/>
-      <c r="C195" s="92"/>
-      <c r="D195" s="92"/>
-      <c r="E195" s="92"/>
-      <c r="H195" s="6" t="s">
+      <c r="C195" s="15"/>
+      <c r="D195" s="15"/>
+      <c r="E195" s="25"/>
+      <c r="H195" s="13" t="s">
         <v>23</v>
       </c>
       <c r="I195" s="1" t="s">
-        <v>139</v>
+        <v>77</v>
       </c>
       <c r="J195" s="4" t="s">
-        <v>605</v>
+        <v>130</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="22"/>
       <c r="B196" s="22"/>
-      <c r="C196" s="92"/>
-      <c r="D196" s="92"/>
-      <c r="E196" s="92"/>
-      <c r="H196" s="13"/>
-    </row>
-    <row r="197" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A197" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B197" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C197" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D197" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E197" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G197" s="112" t="s">
-        <v>295</v>
-      </c>
-      <c r="H197" s="112"/>
-      <c r="I197" s="112"/>
-      <c r="J197" s="112"/>
+      <c r="C196" s="15"/>
+      <c r="D196" s="15"/>
+      <c r="E196" s="25"/>
+      <c r="H196" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I196" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="J196" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A197" s="22"/>
+      <c r="B197" s="22"/>
+      <c r="C197" s="15"/>
+      <c r="D197" s="15"/>
+      <c r="E197" s="25"/>
+      <c r="H197" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I197" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="J197" s="4" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="22"/>
@@ -12729,10 +12720,10 @@
         <v>23</v>
       </c>
       <c r="I198" s="18" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="J198" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
@@ -12746,10 +12737,10 @@
         <v>23</v>
       </c>
       <c r="I199" s="1" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="J199" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
@@ -12762,10 +12753,10 @@
         <v>23</v>
       </c>
       <c r="I200" s="1" t="s">
-        <v>77</v>
+        <v>119</v>
       </c>
       <c r="J200" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
@@ -12778,10 +12769,10 @@
         <v>23</v>
       </c>
       <c r="I201" s="18" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="J201" s="4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.25">
@@ -12794,10 +12785,10 @@
         <v>23</v>
       </c>
       <c r="I202" s="18" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="J202" s="4" t="s">
-        <v>410</v>
+        <v>127</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
@@ -12806,216 +12797,136 @@
       <c r="C203" s="15"/>
       <c r="D203" s="15"/>
       <c r="E203" s="25"/>
-      <c r="G203" s="13"/>
       <c r="H203" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I203" s="18" t="s">
-        <v>108</v>
+      <c r="I203" s="1" t="s">
+        <v>111</v>
       </c>
       <c r="J203" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A204" s="22"/>
-      <c r="B204" s="22"/>
-      <c r="C204" s="15"/>
-      <c r="D204" s="15"/>
-      <c r="E204" s="25"/>
-      <c r="G204" s="13"/>
-      <c r="H204" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I204" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J204" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A205" s="22"/>
-      <c r="B205" s="22"/>
-      <c r="C205" s="15"/>
-      <c r="D205" s="15"/>
-      <c r="E205" s="25"/>
-      <c r="H205" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I205" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J205" s="4" t="s">
-        <v>125</v>
-      </c>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A205" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B205" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C205" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D205" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E205" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G205" s="113" t="s">
+        <v>296</v>
+      </c>
+      <c r="H205" s="113"/>
+      <c r="I205" s="113"/>
+      <c r="J205" s="113"/>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="22"/>
       <c r="B206" s="22"/>
-      <c r="C206" s="15"/>
-      <c r="D206" s="15"/>
-      <c r="E206" s="25"/>
+      <c r="C206" s="22"/>
+      <c r="D206" s="22"/>
+      <c r="E206" s="22"/>
+      <c r="G206" s="13"/>
       <c r="H206" s="13" t="s">
         <v>23</v>
       </c>
       <c r="I206" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="J206" s="4" t="s">
-        <v>126</v>
+        <v>214</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="22"/>
       <c r="B207" s="22"/>
-      <c r="C207" s="15"/>
-      <c r="D207" s="15"/>
-      <c r="E207" s="25"/>
+      <c r="C207" s="22"/>
+      <c r="D207" s="22"/>
+      <c r="E207" s="22"/>
+      <c r="G207" s="13"/>
       <c r="H207" s="13" t="s">
         <v>23</v>
       </c>
       <c r="I207" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="J207" s="4" t="s">
-        <v>127</v>
+        <v>215</v>
       </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="22"/>
       <c r="B208" s="22"/>
-      <c r="C208" s="15"/>
-      <c r="D208" s="15"/>
-      <c r="E208" s="25"/>
+      <c r="C208" s="22"/>
+      <c r="D208" s="22"/>
+      <c r="E208" s="22"/>
       <c r="H208" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="I208" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="J208" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="210" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A210" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="B210" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="C210" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D210" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E210" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G210" s="112" t="s">
-        <v>296</v>
-      </c>
-      <c r="H210" s="112"/>
-      <c r="I210" s="112"/>
-      <c r="J210" s="112"/>
-    </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A211" s="22"/>
-      <c r="B211" s="22"/>
-      <c r="C211" s="22"/>
-      <c r="D211" s="22"/>
-      <c r="E211" s="22"/>
-      <c r="G211" s="13"/>
-      <c r="H211" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I211" s="18" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A212" s="22"/>
-      <c r="B212" s="22"/>
-      <c r="C212" s="22"/>
-      <c r="D212" s="22"/>
-      <c r="E212" s="22"/>
-      <c r="G212" s="13"/>
-      <c r="H212" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I212" s="18" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A213" s="22"/>
-      <c r="B213" s="22"/>
-      <c r="C213" s="22"/>
-      <c r="D213" s="22"/>
-      <c r="E213" s="22"/>
-      <c r="H213" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I213" s="18" t="s">
+      <c r="I208" s="18" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A214" s="22"/>
-      <c r="B214" s="22"/>
-      <c r="C214" s="22"/>
-      <c r="D214" s="22"/>
-      <c r="E214" s="22"/>
-      <c r="H214" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I214" s="18" t="s">
+    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A209" s="22"/>
+      <c r="B209" s="22"/>
+      <c r="C209" s="22"/>
+      <c r="D209" s="22"/>
+      <c r="E209" s="22"/>
+      <c r="H209" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I209" s="18" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A215" s="22"/>
-      <c r="B215" s="22"/>
-      <c r="C215" s="22"/>
-      <c r="D215" s="22"/>
-      <c r="E215" s="22"/>
-      <c r="H215" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I215" s="18" t="s">
+    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A210" s="22"/>
+      <c r="B210" s="22"/>
+      <c r="C210" s="22"/>
+      <c r="D210" s="22"/>
+      <c r="E210" s="22"/>
+      <c r="H210" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I210" s="18" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I216" s="18"/>
-    </row>
-    <row r="217" spans="1:10" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A217" s="90"/>
+    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I211" s="18"/>
+    </row>
+    <row r="212" spans="1:9" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+      <c r="A212" s="90"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="G63:J63"/>
-    <mergeCell ref="G64:J64"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="G66:J66"/>
-    <mergeCell ref="G70:J70"/>
-    <mergeCell ref="G75:J75"/>
-    <mergeCell ref="G78:J78"/>
-    <mergeCell ref="G79:J79"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="A2:E2"/>
+  <mergeCells count="58">
+    <mergeCell ref="G205:J205"/>
+    <mergeCell ref="G156:J156"/>
+    <mergeCell ref="G169:J169"/>
+    <mergeCell ref="G173:J173"/>
+    <mergeCell ref="G180:J180"/>
+    <mergeCell ref="G192:J192"/>
+    <mergeCell ref="G188:J188"/>
+    <mergeCell ref="G116:J116"/>
+    <mergeCell ref="G131:J131"/>
+    <mergeCell ref="G166:J166"/>
+    <mergeCell ref="G167:J167"/>
+    <mergeCell ref="G168:J168"/>
+    <mergeCell ref="G162:J162"/>
+    <mergeCell ref="G151:J151"/>
+    <mergeCell ref="G146:J146"/>
+    <mergeCell ref="G147:J147"/>
+    <mergeCell ref="G132:J132"/>
+    <mergeCell ref="G86:J86"/>
+    <mergeCell ref="G91:J91"/>
+    <mergeCell ref="G96:J96"/>
+    <mergeCell ref="G103:J103"/>
+    <mergeCell ref="G108:J108"/>
     <mergeCell ref="B89:E89"/>
     <mergeCell ref="G15:J15"/>
     <mergeCell ref="G19:J19"/>
@@ -13032,29 +12943,26 @@
     <mergeCell ref="G50:J50"/>
     <mergeCell ref="G51:J51"/>
     <mergeCell ref="G52:J52"/>
-    <mergeCell ref="G86:J86"/>
-    <mergeCell ref="G91:J91"/>
-    <mergeCell ref="G96:J96"/>
-    <mergeCell ref="G103:J103"/>
-    <mergeCell ref="G108:J108"/>
-    <mergeCell ref="G116:J116"/>
-    <mergeCell ref="G131:J131"/>
-    <mergeCell ref="G166:J166"/>
-    <mergeCell ref="G167:J167"/>
-    <mergeCell ref="G168:J168"/>
-    <mergeCell ref="G162:J162"/>
-    <mergeCell ref="G151:J151"/>
-    <mergeCell ref="G146:J146"/>
-    <mergeCell ref="G147:J147"/>
-    <mergeCell ref="G132:J132"/>
-    <mergeCell ref="G210:J210"/>
-    <mergeCell ref="G156:J156"/>
-    <mergeCell ref="G169:J169"/>
-    <mergeCell ref="G173:J173"/>
-    <mergeCell ref="G180:J180"/>
-    <mergeCell ref="G197:J197"/>
-    <mergeCell ref="G193:J193"/>
-    <mergeCell ref="G188:J188"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="G63:J63"/>
+    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="G66:J66"/>
+    <mergeCell ref="G70:J70"/>
+    <mergeCell ref="G75:J75"/>
+    <mergeCell ref="G78:J78"/>
+    <mergeCell ref="G79:J79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated SSP Template and Registry
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-3540" windowWidth="7380" windowHeight="5505" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="-3540" windowWidth="7380" windowHeight="5505"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATION" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3769" uniqueCount="944">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3770" uniqueCount="951">
   <si>
     <t>SSP</t>
   </si>
@@ -2582,9 +2582,6 @@
     <t>3.0 -&gt; 3.1 Diff: OF -&gt; O, TF -&gt; T</t>
   </si>
   <si>
-    <t>Data Type</t>
-  </si>
-  <si>
     <t>evidence</t>
   </si>
   <si>
@@ -3326,9 +3323,6 @@
     <t>interconnection</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>An interconnection to another system, typically governed by an interconnection security agreement (ISA).</t>
   </si>
   <si>
@@ -3377,12 +3371,39 @@
   <si>
     <t>** NOTE: NIST has switched from ID to UUID for most SSP, SAP, SAR and POA&amp;M identifiers. FedRAMP tools now identify parties based on their role affiliation</t>
   </si>
+  <si>
+    <t>Interconnection: Transmitted Information</t>
+  </si>
+  <si>
+    <t>information</t>
+  </si>
+  <si>
+    <t>ipv4-address</t>
+  </si>
+  <si>
+    <t>ipv6-address</t>
+  </si>
+  <si>
+    <t>Interconnection: IPv4 Address (see notes)</t>
+  </si>
+  <si>
+    <t>Interconnection: IPv6 Address (see notes)</t>
+  </si>
+  <si>
+    <t>Use @class="local" or @class="remote" for Local and Remote addresses</t>
+  </si>
+  <si>
+    <t>ip-v6-address</t>
+  </si>
+  <si>
+    <t>OSCAL Data Type</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3671,6 +3692,14 @@
       <color theme="0" tint="-0.249977111117893"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -4017,7 +4046,7 @@
     <xf numFmtId="0" fontId="25" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -4326,26 +4355,26 @@
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="9" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4358,6 +4387,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4711,7 +4743,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -4865,7 +4897,7 @@
     </row>
     <row r="18" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="64">
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="B18" s="57" t="s">
         <v>525</v>
@@ -4977,35 +5009,35 @@
       <c r="C1" s="6"/>
       <c r="D1"/>
       <c r="E1" s="6"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
       <c r="J1" s="80" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="G2" s="54" t="s">
         <v>405</v>
       </c>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
       <c r="J2" t="s">
         <v>443</v>
       </c>
-      <c r="K2" s="129" t="s">
-        <v>738</v>
-      </c>
-      <c r="L2" s="129" t="s">
+      <c r="K2" s="140" t="s">
+        <v>950</v>
+      </c>
+      <c r="L2" s="128" t="s">
         <v>303</v>
       </c>
-      <c r="M2" s="129" t="s">
+      <c r="M2" s="128" t="s">
         <v>554</v>
       </c>
     </row>
@@ -5037,9 +5069,9 @@
       <c r="J3" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
-      <c r="M3" s="129"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="128"/>
+      <c r="M3" s="128"/>
       <c r="N3" s="43" t="s">
         <v>8</v>
       </c>
@@ -5112,7 +5144,7 @@
         <v>28</v>
       </c>
       <c r="I6" s="68" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="J6" s="73" t="s">
         <v>524</v>
@@ -5198,7 +5230,7 @@
         <v>28</v>
       </c>
       <c r="I10" s="68" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="J10" s="76" t="s">
         <v>536</v>
@@ -5752,7 +5784,7 @@
         <v>430</v>
       </c>
       <c r="J29" s="55" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K29" s="6" t="s">
         <v>365</v>
@@ -5794,7 +5826,7 @@
         <v>431</v>
       </c>
       <c r="J31" s="55" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="K31" s="6" t="s">
         <v>365</v>
@@ -5817,20 +5849,23 @@
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>53</v>
+        <v>946</v>
       </c>
       <c r="H32" s="68" t="s">
         <v>28</v>
       </c>
       <c r="I32" s="68" t="s">
-        <v>432</v>
+        <v>944</v>
       </c>
       <c r="J32" s="55" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="K32" s="6" t="s">
         <v>366</v>
       </c>
+      <c r="N32" s="4" t="s">
+        <v>948</v>
+      </c>
     </row>
     <row r="33" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
@@ -5849,19 +5884,22 @@
         <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>54</v>
+        <v>947</v>
       </c>
       <c r="H33" s="68" t="s">
         <v>28</v>
       </c>
       <c r="I33" s="68" t="s">
-        <v>433</v>
+        <v>945</v>
       </c>
       <c r="J33" s="55" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>366</v>
+        <v>949</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>948</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -5890,7 +5928,7 @@
         <v>434</v>
       </c>
       <c r="J34" s="55" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="K34" s="6" t="s">
         <v>364</v>
@@ -5916,16 +5954,16 @@
         <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>57</v>
+        <v>942</v>
       </c>
       <c r="H35" s="68" t="s">
         <v>28</v>
       </c>
       <c r="I35" s="68" t="s">
-        <v>438</v>
+        <v>943</v>
       </c>
       <c r="J35" s="55" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="K35" s="6" t="s">
         <v>365</v>
@@ -5960,7 +5998,7 @@
         <v>435</v>
       </c>
       <c r="J36" s="55" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="K36" s="6" t="s">
         <v>365</v>
@@ -5995,7 +6033,7 @@
         <v>436</v>
       </c>
       <c r="J37" s="55" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="K37" s="6" t="s">
         <v>365</v>
@@ -6030,7 +6068,7 @@
         <v>437</v>
       </c>
       <c r="J38" s="55" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="K38" s="6" t="s">
         <v>365</v>
@@ -6520,16 +6558,16 @@
         <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="H55" s="68" t="s">
         <v>28</v>
       </c>
       <c r="I55" s="68" t="s">
+        <v>862</v>
+      </c>
+      <c r="J55" s="101" t="s">
         <v>863</v>
-      </c>
-      <c r="J55" s="101" t="s">
-        <v>864</v>
       </c>
       <c r="K55" s="6" t="s">
         <v>365</v>
@@ -6586,7 +6624,7 @@
         <v>23</v>
       </c>
       <c r="N57" s="4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -6621,7 +6659,7 @@
         <v>304</v>
       </c>
       <c r="N58" s="4" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="59" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -6656,7 +6694,7 @@
         <v>365</v>
       </c>
       <c r="N59" s="4" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="60" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -6957,22 +6995,22 @@
         <v>1</v>
       </c>
       <c r="G70" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="H70" s="68" t="s">
         <v>28</v>
       </c>
       <c r="I70" s="68" t="s">
+        <v>824</v>
+      </c>
+      <c r="J70" s="99" t="s">
         <v>825</v>
-      </c>
-      <c r="J70" s="99" t="s">
-        <v>826</v>
       </c>
       <c r="K70" s="6" t="s">
         <v>365</v>
       </c>
       <c r="N70" s="4" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
@@ -6991,12 +7029,12 @@
       <c r="L72" s="79"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G73" s="130" t="s">
+      <c r="G73" s="131" t="s">
         <v>606</v>
       </c>
-      <c r="H73" s="130"/>
-      <c r="I73" s="130"/>
-      <c r="J73" s="130"/>
+      <c r="H73" s="131"/>
+      <c r="I73" s="131"/>
+      <c r="J73" s="131"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
@@ -7032,12 +7070,12 @@
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G78" s="130" t="s">
+      <c r="G78" s="131" t="s">
         <v>535</v>
       </c>
-      <c r="H78" s="130"/>
-      <c r="I78" s="130"/>
-      <c r="J78" s="130"/>
+      <c r="H78" s="131"/>
+      <c r="I78" s="131"/>
+      <c r="J78" s="131"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
@@ -7078,16 +7116,19 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="G78:J78"/>
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="M2:M3"/>
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="G73:J73"/>
-    <mergeCell ref="G78:J78"/>
-    <mergeCell ref="K2:K3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="K2:K3" r:id="rId1" display="OSCAL Data Type"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="3" orientation="landscape" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7124,7 +7165,7 @@
       <c r="D1"/>
       <c r="E1" s="6"/>
       <c r="H1" s="70"/>
-      <c r="I1" s="131" t="str">
+      <c r="I1" s="129" t="str">
         <f>CONCATENATE("All FedRAMP Compliance tags must use name='", tagname, "', as well as ns='https://fedramp.gov/ns/oscal'")</f>
         <v>All FedRAMP Compliance tags must use name='conformity', as well as ns='https://fedramp.gov/ns/oscal'</v>
       </c>
@@ -7133,18 +7174,18 @@
       </c>
     </row>
     <row r="2" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="G2" s="54" t="s">
         <v>405</v>
       </c>
       <c r="H2" s="70"/>
-      <c r="I2" s="131"/>
+      <c r="I2" s="129"/>
       <c r="J2" t="s">
         <v>443</v>
       </c>
@@ -7184,7 +7225,7 @@
         <v>8</v>
       </c>
       <c r="L3" s="43" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
@@ -7242,7 +7283,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -7254,10 +7295,10 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
+        <v>915</v>
+      </c>
+      <c r="H7" s="74" t="s">
         <v>916</v>
-      </c>
-      <c r="H7" s="74" t="s">
-        <v>917</v>
       </c>
       <c r="I7" s="69" t="s">
         <v>483</v>
@@ -7267,7 +7308,7 @@
         <v>/*/metadata/location/prop[@name='conformity'][@ns='https://fedramp.gov/ns/oscal'][string(.)='data-center']/..</v>
       </c>
       <c r="K7" s="132" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="L7" s="115" t="str">
         <f>CONCATENATE("&lt;prop name='", tagname,"' ns='https://fedramp.gov/ns/oscal'&gt;",H7,"&lt;/prop&gt;")</f>
@@ -7326,7 +7367,7 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="H9" s="74" t="s">
         <v>560</v>
@@ -7417,13 +7458,13 @@
         <v>10</v>
       </c>
       <c r="G13" t="s">
+        <v>829</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>830</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="69" t="s">
         <v>831</v>
-      </c>
-      <c r="I13" s="69" t="s">
-        <v>832</v>
       </c>
       <c r="J13" s="101" t="str">
         <f t="shared" ref="J13:J18" si="0">CONCATENATE(I13,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H13,"']/..")</f>
@@ -7451,13 +7492,13 @@
         <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="I14" s="69" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="J14" s="101" t="str">
         <f t="shared" si="0"/>
@@ -7485,13 +7526,13 @@
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="I15" s="69" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="J15" s="101" t="str">
         <f t="shared" si="0"/>
@@ -7519,13 +7560,13 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="I16" s="69" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="J16" s="101" t="str">
         <f t="shared" si="0"/>
@@ -7553,13 +7594,13 @@
         <v>10</v>
       </c>
       <c r="G17" t="s">
+        <v>888</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="H17" s="1" t="s">
-        <v>890</v>
-      </c>
       <c r="I17" s="69" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="J17" s="111" t="str">
         <f t="shared" si="0"/>
@@ -7587,13 +7628,13 @@
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="I18" s="69" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="J18" s="101" t="str">
         <f t="shared" si="0"/>
@@ -7632,13 +7673,13 @@
         <v>10</v>
       </c>
       <c r="G20" t="s">
+        <v>903</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>904</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="I20" s="69" t="s">
         <v>905</v>
-      </c>
-      <c r="I20" s="69" t="s">
-        <v>906</v>
       </c>
       <c r="J20" s="111" t="str">
         <f>CONCATENATE(I20,"/prop[@name='", tagname, "'][@ns='https://fedramp.gov/ns/oscal'][string(.)='",H20,"']/..")</f>
@@ -8224,7 +8265,7 @@
         <v>533</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="I38" s="69" t="s">
         <v>521</v>
@@ -8289,10 +8330,10 @@
         <v>7</v>
       </c>
       <c r="G40" s="44" t="s">
+        <v>805</v>
+      </c>
+      <c r="H40" s="1" t="s">
         <v>806</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>807</v>
       </c>
       <c r="I40" s="69" t="s">
         <v>521</v>
@@ -8404,9 +8445,9 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Q64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8431,17 +8472,17 @@
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="G2" s="128" t="s">
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="G2" s="130" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="128"/>
+      <c r="H2" s="130"/>
       <c r="I2" s="24" t="s">
         <v>288</v>
       </c>
@@ -9205,7 +9246,7 @@
         <v>190</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -9231,7 +9272,7 @@
         <v>9</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -9257,7 +9298,7 @@
         <v>489</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -9537,7 +9578,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
     </row>
     <row r="47" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -9688,7 +9729,7 @@
       <c r="E55" s="83"/>
       <c r="F55" s="23"/>
       <c r="G55" s="83" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="H55" s="83"/>
       <c r="I55" s="83"/>
@@ -9718,7 +9759,7 @@
         <v>613</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -9741,10 +9782,10 @@
         <v>23</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -9770,7 +9811,7 @@
         <v>630</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -9796,7 +9837,7 @@
         <v>682</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -9822,7 +9863,7 @@
         <v>734</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -9845,7 +9886,7 @@
         <v>23</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
@@ -9868,8 +9909,8 @@
   <dimension ref="A1:J299"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I87" sqref="I87"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9896,17 +9937,17 @@
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="G2" s="128" t="s">
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="G2" s="130" t="s">
         <v>88</v>
       </c>
-      <c r="H2" s="128"/>
+      <c r="H2" s="130"/>
       <c r="I2" s="24" t="s">
         <v>217</v>
       </c>
@@ -9956,12 +9997,12 @@
       <c r="E4" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="133" t="s">
+      <c r="G4" s="134" t="s">
         <v>309</v>
       </c>
-      <c r="H4" s="133"/>
-      <c r="I4" s="133"/>
-      <c r="J4" s="133"/>
+      <c r="H4" s="134"/>
+      <c r="I4" s="134"/>
+      <c r="J4" s="134"/>
     </row>
     <row r="5" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
@@ -9979,12 +10020,12 @@
       <c r="E5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="133" t="s">
+      <c r="G5" s="134" t="s">
         <v>308</v>
       </c>
-      <c r="H5" s="133"/>
-      <c r="I5" s="133"/>
-      <c r="J5" s="133"/>
+      <c r="H5" s="134"/>
+      <c r="I5" s="134"/>
+      <c r="J5" s="134"/>
     </row>
     <row r="6" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="97" t="s">
@@ -10065,12 +10106,12 @@
       <c r="E9" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="133" t="s">
+      <c r="G9" s="134" t="s">
         <v>315</v>
       </c>
-      <c r="H9" s="133"/>
-      <c r="I9" s="133"/>
-      <c r="J9" s="133"/>
+      <c r="H9" s="134"/>
+      <c r="I9" s="134"/>
+      <c r="J9" s="134"/>
     </row>
     <row r="10" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
@@ -10088,12 +10129,12 @@
       <c r="E10" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="133" t="s">
+      <c r="G10" s="134" t="s">
         <v>314</v>
       </c>
-      <c r="H10" s="133"/>
-      <c r="I10" s="133"/>
-      <c r="J10" s="133"/>
+      <c r="H10" s="134"/>
+      <c r="I10" s="134"/>
+      <c r="J10" s="134"/>
     </row>
     <row r="11" spans="1:10" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="97" t="s">
@@ -10200,12 +10241,12 @@
       <c r="E15" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="133" t="s">
+      <c r="G15" s="134" t="s">
         <v>251</v>
       </c>
-      <c r="H15" s="133"/>
-      <c r="I15" s="133"/>
-      <c r="J15" s="133"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="134"/>
+      <c r="J15" s="134"/>
     </row>
     <row r="16" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="96" t="s">
@@ -10286,12 +10327,12 @@
       <c r="E19" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G19" s="133" t="s">
+      <c r="G19" s="134" t="s">
         <v>252</v>
       </c>
-      <c r="H19" s="133"/>
-      <c r="I19" s="133"/>
-      <c r="J19" s="133"/>
+      <c r="H19" s="134"/>
+      <c r="I19" s="134"/>
+      <c r="J19" s="134"/>
     </row>
     <row r="20" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
@@ -10309,12 +10350,12 @@
       <c r="E20" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="133" t="s">
+      <c r="G20" s="134" t="s">
         <v>253</v>
       </c>
-      <c r="H20" s="133"/>
-      <c r="I20" s="133"/>
-      <c r="J20" s="133"/>
+      <c r="H20" s="134"/>
+      <c r="I20" s="134"/>
+      <c r="J20" s="134"/>
     </row>
     <row r="21" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
@@ -10332,12 +10373,12 @@
       <c r="E21" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="133" t="s">
+      <c r="G21" s="134" t="s">
         <v>254</v>
       </c>
-      <c r="H21" s="133"/>
-      <c r="I21" s="133"/>
-      <c r="J21" s="133"/>
+      <c r="H21" s="134"/>
+      <c r="I21" s="134"/>
+      <c r="J21" s="134"/>
     </row>
     <row r="22" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
@@ -10355,12 +10396,12 @@
       <c r="E22" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G22" s="133" t="s">
+      <c r="G22" s="134" t="s">
         <v>255</v>
       </c>
-      <c r="H22" s="133"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="133"/>
+      <c r="H22" s="134"/>
+      <c r="I22" s="134"/>
+      <c r="J22" s="134"/>
     </row>
     <row r="23" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="96" t="s">
@@ -10467,12 +10508,12 @@
       <c r="E27" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G27" s="133" t="s">
+      <c r="G27" s="134" t="s">
         <v>256</v>
       </c>
-      <c r="H27" s="133"/>
-      <c r="I27" s="133"/>
-      <c r="J27" s="133"/>
+      <c r="H27" s="134"/>
+      <c r="I27" s="134"/>
+      <c r="J27" s="134"/>
     </row>
     <row r="28" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="96" t="s">
@@ -10582,12 +10623,12 @@
       <c r="E32" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="133" t="s">
+      <c r="G32" s="134" t="s">
         <v>305</v>
       </c>
-      <c r="H32" s="133"/>
-      <c r="I32" s="133"/>
-      <c r="J32" s="133"/>
+      <c r="H32" s="134"/>
+      <c r="I32" s="134"/>
+      <c r="J32" s="134"/>
     </row>
     <row r="33" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="96" t="s">
@@ -10720,12 +10761,12 @@
       <c r="E38" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="133" t="s">
+      <c r="G38" s="134" t="s">
         <v>257</v>
       </c>
-      <c r="H38" s="133"/>
-      <c r="I38" s="133"/>
-      <c r="J38" s="133"/>
+      <c r="H38" s="134"/>
+      <c r="I38" s="134"/>
+      <c r="J38" s="134"/>
     </row>
     <row r="39" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="96" t="s">
@@ -10780,12 +10821,12 @@
       </c>
     </row>
     <row r="41" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="134" t="s">
+      <c r="B41" s="133" t="s">
         <v>235</v>
       </c>
-      <c r="C41" s="134"/>
-      <c r="D41" s="134"/>
-      <c r="E41" s="134"/>
+      <c r="C41" s="133"/>
+      <c r="D41" s="133"/>
+      <c r="E41" s="133"/>
       <c r="G41" s="15" t="s">
         <v>23</v>
       </c>
@@ -10903,12 +10944,12 @@
       <c r="E46" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G46" s="133" t="s">
+      <c r="G46" s="134" t="s">
         <v>258</v>
       </c>
-      <c r="H46" s="133"/>
-      <c r="I46" s="133"/>
-      <c r="J46" s="133"/>
+      <c r="H46" s="134"/>
+      <c r="I46" s="134"/>
+      <c r="J46" s="134"/>
     </row>
     <row r="47" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
@@ -10926,12 +10967,12 @@
       <c r="E47" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G47" s="133" t="s">
+      <c r="G47" s="134" t="s">
         <v>259</v>
       </c>
-      <c r="H47" s="133"/>
-      <c r="I47" s="133"/>
-      <c r="J47" s="133"/>
+      <c r="H47" s="134"/>
+      <c r="I47" s="134"/>
+      <c r="J47" s="134"/>
     </row>
     <row r="48" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A48" s="27" t="s">
@@ -10949,12 +10990,12 @@
       <c r="E48" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G48" s="133" t="s">
+      <c r="G48" s="134" t="s">
         <v>260</v>
       </c>
-      <c r="H48" s="133"/>
-      <c r="I48" s="133"/>
-      <c r="J48" s="133"/>
+      <c r="H48" s="134"/>
+      <c r="I48" s="134"/>
+      <c r="J48" s="134"/>
     </row>
     <row r="49" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A49" s="27" t="s">
@@ -10972,12 +11013,12 @@
       <c r="E49" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G49" s="133" t="s">
+      <c r="G49" s="134" t="s">
         <v>261</v>
       </c>
-      <c r="H49" s="133"/>
-      <c r="I49" s="133"/>
-      <c r="J49" s="133"/>
+      <c r="H49" s="134"/>
+      <c r="I49" s="134"/>
+      <c r="J49" s="134"/>
     </row>
     <row r="50" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
@@ -10995,12 +11036,12 @@
       <c r="E50" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G50" s="133" t="s">
+      <c r="G50" s="134" t="s">
         <v>262</v>
       </c>
-      <c r="H50" s="133"/>
-      <c r="I50" s="133"/>
-      <c r="J50" s="133"/>
+      <c r="H50" s="134"/>
+      <c r="I50" s="134"/>
+      <c r="J50" s="134"/>
     </row>
     <row r="51" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A51" s="27" t="s">
@@ -11018,12 +11059,12 @@
       <c r="E51" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G51" s="133" t="s">
+      <c r="G51" s="134" t="s">
         <v>263</v>
       </c>
-      <c r="H51" s="133"/>
-      <c r="I51" s="133"/>
-      <c r="J51" s="133"/>
+      <c r="H51" s="134"/>
+      <c r="I51" s="134"/>
+      <c r="J51" s="134"/>
     </row>
     <row r="52" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
@@ -11041,12 +11082,12 @@
       <c r="E52" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G52" s="133" t="s">
+      <c r="G52" s="134" t="s">
         <v>264</v>
       </c>
-      <c r="H52" s="133"/>
-      <c r="I52" s="133"/>
-      <c r="J52" s="133"/>
+      <c r="H52" s="134"/>
+      <c r="I52" s="134"/>
+      <c r="J52" s="134"/>
     </row>
     <row r="53" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
@@ -11064,12 +11105,12 @@
       <c r="E53" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G53" s="133" t="s">
+      <c r="G53" s="134" t="s">
         <v>265</v>
       </c>
-      <c r="H53" s="133"/>
-      <c r="I53" s="133"/>
-      <c r="J53" s="133"/>
+      <c r="H53" s="134"/>
+      <c r="I53" s="134"/>
+      <c r="J53" s="134"/>
     </row>
     <row r="54" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A54" s="27" t="s">
@@ -11087,12 +11128,12 @@
       <c r="E54" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G54" s="133" t="s">
+      <c r="G54" s="134" t="s">
         <v>266</v>
       </c>
-      <c r="H54" s="133"/>
-      <c r="I54" s="133"/>
-      <c r="J54" s="133"/>
+      <c r="H54" s="134"/>
+      <c r="I54" s="134"/>
+      <c r="J54" s="134"/>
     </row>
     <row r="55" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="96" t="s">
@@ -11196,12 +11237,12 @@
       <c r="E59" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G59" s="133" t="s">
+      <c r="G59" s="134" t="s">
         <v>267</v>
       </c>
-      <c r="H59" s="133"/>
-      <c r="I59" s="133"/>
-      <c r="J59" s="133"/>
+      <c r="H59" s="134"/>
+      <c r="I59" s="134"/>
+      <c r="J59" s="134"/>
     </row>
     <row r="60" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="96" t="s">
@@ -11282,12 +11323,12 @@
       <c r="E63" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G63" s="133" t="s">
+      <c r="G63" s="134" t="s">
         <v>268</v>
       </c>
-      <c r="H63" s="133"/>
-      <c r="I63" s="133"/>
-      <c r="J63" s="133"/>
+      <c r="H63" s="134"/>
+      <c r="I63" s="134"/>
+      <c r="J63" s="134"/>
     </row>
     <row r="64" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A64" s="27" t="s">
@@ -11305,12 +11346,12 @@
       <c r="E64" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G64" s="133" t="s">
+      <c r="G64" s="134" t="s">
         <v>269</v>
       </c>
-      <c r="H64" s="133"/>
-      <c r="I64" s="133"/>
-      <c r="J64" s="133"/>
+      <c r="H64" s="134"/>
+      <c r="I64" s="134"/>
+      <c r="J64" s="134"/>
     </row>
     <row r="65" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
@@ -11328,12 +11369,12 @@
       <c r="E65" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G65" s="133" t="s">
+      <c r="G65" s="134" t="s">
         <v>270</v>
       </c>
-      <c r="H65" s="133"/>
-      <c r="I65" s="133"/>
-      <c r="J65" s="133"/>
+      <c r="H65" s="134"/>
+      <c r="I65" s="134"/>
+      <c r="J65" s="134"/>
     </row>
     <row r="66" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A66" s="27" t="s">
@@ -11351,12 +11392,12 @@
       <c r="E66" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G66" s="133" t="s">
+      <c r="G66" s="134" t="s">
         <v>271</v>
       </c>
-      <c r="H66" s="133"/>
-      <c r="I66" s="133"/>
-      <c r="J66" s="133"/>
+      <c r="H66" s="134"/>
+      <c r="I66" s="134"/>
+      <c r="J66" s="134"/>
     </row>
     <row r="67" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="96" t="s">
@@ -11433,12 +11474,12 @@
       <c r="E70" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G70" s="133" t="s">
+      <c r="G70" s="134" t="s">
         <v>272</v>
       </c>
-      <c r="H70" s="133"/>
-      <c r="I70" s="133"/>
-      <c r="J70" s="133"/>
+      <c r="H70" s="134"/>
+      <c r="I70" s="134"/>
+      <c r="J70" s="134"/>
     </row>
     <row r="71" spans="1:10" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A71" s="27" t="s">
@@ -11457,7 +11498,7 @@
         <v>50</v>
       </c>
       <c r="G71" s="111" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="H71" s="89"/>
       <c r="I71" s="114"/>
@@ -11480,7 +11521,7 @@
         <v>50</v>
       </c>
       <c r="G72" s="89" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="H72" s="89"/>
       <c r="I72" s="114"/>
@@ -11589,7 +11630,7 @@
         <v>50</v>
       </c>
       <c r="G77" s="111" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H77" s="111"/>
       <c r="I77" s="114"/>
@@ -11612,7 +11653,7 @@
         <v>50</v>
       </c>
       <c r="G78" s="111" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="H78" s="111"/>
       <c r="I78" s="114"/>
@@ -11635,7 +11676,7 @@
         <v>50</v>
       </c>
       <c r="G79" s="111" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="H79" s="111"/>
       <c r="I79" s="114"/>
@@ -11662,10 +11703,10 @@
       </c>
       <c r="H80" s="13"/>
       <c r="I80" s="12" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="J80" s="16" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -11689,10 +11730,10 @@
       </c>
       <c r="H81" s="13"/>
       <c r="I81" s="12" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J81" s="16" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="82" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -11716,10 +11757,10 @@
       </c>
       <c r="H82" s="13"/>
       <c r="I82" s="12" t="s">
+        <v>899</v>
+      </c>
+      <c r="J82" s="16" t="s">
         <v>900</v>
-      </c>
-      <c r="J82" s="16" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="83" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
@@ -11749,12 +11790,12 @@
       <c r="E84" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G84" s="133" t="s">
-        <v>899</v>
-      </c>
-      <c r="H84" s="133"/>
-      <c r="I84" s="133"/>
-      <c r="J84" s="133"/>
+      <c r="G84" s="134" t="s">
+        <v>898</v>
+      </c>
+      <c r="H84" s="134"/>
+      <c r="I84" s="134"/>
+      <c r="J84" s="134"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="96" t="s">
@@ -11776,10 +11817,10 @@
         <v>23</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -11802,10 +11843,10 @@
         <v>23</v>
       </c>
       <c r="I86" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>821</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -11825,10 +11866,10 @@
         <v>50</v>
       </c>
       <c r="I87" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>756</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -11855,12 +11896,12 @@
       <c r="E89" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G89" s="133" t="s">
+      <c r="G89" s="134" t="s">
         <v>307</v>
       </c>
-      <c r="H89" s="133"/>
-      <c r="I89" s="133"/>
-      <c r="J89" s="133"/>
+      <c r="H89" s="134"/>
+      <c r="I89" s="134"/>
+      <c r="J89" s="134"/>
     </row>
     <row r="90" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="96" t="s">
@@ -11915,12 +11956,12 @@
       <c r="E92" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G92" s="133" t="s">
+      <c r="G92" s="134" t="s">
         <v>273</v>
       </c>
-      <c r="H92" s="133"/>
-      <c r="I92" s="133"/>
-      <c r="J92" s="133"/>
+      <c r="H92" s="134"/>
+      <c r="I92" s="134"/>
+      <c r="J92" s="134"/>
     </row>
     <row r="93" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A93" s="27" t="s">
@@ -11938,12 +11979,12 @@
       <c r="E93" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G93" s="133" t="s">
+      <c r="G93" s="134" t="s">
         <v>274</v>
       </c>
-      <c r="H93" s="133"/>
-      <c r="I93" s="133"/>
-      <c r="J93" s="133"/>
+      <c r="H93" s="134"/>
+      <c r="I93" s="134"/>
+      <c r="J93" s="134"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="96" t="s">
@@ -11965,17 +12006,17 @@
         <v>23</v>
       </c>
       <c r="I94" s="117" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="95" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="134" t="s">
+      <c r="A95" s="133" t="s">
         <v>235</v>
       </c>
-      <c r="B95" s="134"/>
-      <c r="C95" s="134"/>
-      <c r="D95" s="134"/>
-      <c r="E95" s="134"/>
+      <c r="B95" s="133"/>
+      <c r="C95" s="133"/>
+      <c r="D95" s="133"/>
+      <c r="E95" s="133"/>
       <c r="G95" s="28" t="s">
         <v>23</v>
       </c>
@@ -12006,20 +12047,20 @@
         <v>23</v>
       </c>
       <c r="I96" s="117" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="J96" s="4" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="97" spans="1:10" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="134" t="s">
+      <c r="A97" s="133" t="s">
         <v>235</v>
       </c>
-      <c r="B97" s="134"/>
-      <c r="C97" s="134"/>
-      <c r="D97" s="134"/>
-      <c r="E97" s="134"/>
+      <c r="B97" s="133"/>
+      <c r="C97" s="133"/>
+      <c r="D97" s="133"/>
+      <c r="E97" s="133"/>
       <c r="G97" s="28" t="s">
         <v>23</v>
       </c>
@@ -12072,12 +12113,12 @@
       <c r="E100" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G100" s="133" t="s">
+      <c r="G100" s="134" t="s">
         <v>275</v>
       </c>
-      <c r="H100" s="133"/>
-      <c r="I100" s="133"/>
-      <c r="J100" s="133"/>
+      <c r="H100" s="134"/>
+      <c r="I100" s="134"/>
+      <c r="J100" s="134"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="96" t="s">
@@ -12126,13 +12167,13 @@
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A103" s="134" t="s">
+      <c r="A103" s="133" t="s">
         <v>235</v>
       </c>
-      <c r="B103" s="134"/>
-      <c r="C103" s="134"/>
-      <c r="D103" s="134"/>
-      <c r="E103" s="134"/>
+      <c r="B103" s="133"/>
+      <c r="C103" s="133"/>
+      <c r="D103" s="133"/>
+      <c r="E103" s="133"/>
       <c r="F103" s="31"/>
       <c r="G103" s="28" t="s">
         <v>23</v>
@@ -12159,12 +12200,12 @@
       <c r="E105" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G105" s="133" t="s">
+      <c r="G105" s="134" t="s">
         <v>306</v>
       </c>
-      <c r="H105" s="133"/>
-      <c r="I105" s="133"/>
-      <c r="J105" s="133"/>
+      <c r="H105" s="134"/>
+      <c r="I105" s="134"/>
+      <c r="J105" s="134"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="96" t="s">
@@ -12251,12 +12292,12 @@
       <c r="E110" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G110" s="133" t="s">
+      <c r="G110" s="134" t="s">
         <v>276</v>
       </c>
-      <c r="H110" s="133"/>
-      <c r="I110" s="133"/>
-      <c r="J110" s="133"/>
+      <c r="H110" s="134"/>
+      <c r="I110" s="134"/>
+      <c r="J110" s="134"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="96" t="s">
@@ -12395,12 +12436,12 @@
       <c r="E117" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G117" s="133" t="s">
+      <c r="G117" s="134" t="s">
         <v>277</v>
       </c>
-      <c r="H117" s="133"/>
-      <c r="I117" s="133"/>
-      <c r="J117" s="133"/>
+      <c r="H117" s="134"/>
+      <c r="I117" s="134"/>
+      <c r="J117" s="134"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="96" t="s">
@@ -12500,12 +12541,12 @@
       <c r="E122" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G122" s="133" t="s">
+      <c r="G122" s="134" t="s">
         <v>278</v>
       </c>
-      <c r="H122" s="133"/>
-      <c r="I122" s="133"/>
-      <c r="J122" s="133"/>
+      <c r="H122" s="134"/>
+      <c r="I122" s="134"/>
+      <c r="J122" s="134"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="96" t="s">
@@ -12669,12 +12710,12 @@
       <c r="E130" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G130" s="133" t="s">
+      <c r="G130" s="134" t="s">
         <v>279</v>
       </c>
-      <c r="H130" s="133"/>
-      <c r="I130" s="133"/>
-      <c r="J130" s="133"/>
+      <c r="H130" s="134"/>
+      <c r="I130" s="134"/>
+      <c r="J130" s="134"/>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="96" t="s">
@@ -12696,7 +12737,7 @@
         <v>23</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="J131" s="4" t="s">
         <v>137</v>
@@ -12770,17 +12811,14 @@
       <c r="E134" s="97" t="s">
         <v>50</v>
       </c>
-      <c r="G134" s="6" t="s">
-        <v>934</v>
-      </c>
-      <c r="H134" s="13" t="s">
-        <v>934</v>
+      <c r="G134" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>933</v>
+        <v>97</v>
       </c>
       <c r="J134" s="4" t="s">
-        <v>935</v>
+        <v>931</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
@@ -12803,10 +12841,10 @@
         <v>23</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>97</v>
+        <v>932</v>
       </c>
       <c r="J135" s="4" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
@@ -13049,12 +13087,12 @@
       <c r="E146" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G146" s="133" t="s">
+      <c r="G146" s="134" t="s">
         <v>323</v>
       </c>
-      <c r="H146" s="133"/>
-      <c r="I146" s="133"/>
-      <c r="J146" s="133"/>
+      <c r="H146" s="134"/>
+      <c r="I146" s="134"/>
+      <c r="J146" s="134"/>
     </row>
     <row r="147" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A147" s="27" t="s">
@@ -13072,12 +13110,12 @@
       <c r="E147" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G147" s="133" t="s">
+      <c r="G147" s="134" t="s">
         <v>353</v>
       </c>
-      <c r="H147" s="133"/>
-      <c r="I147" s="133"/>
-      <c r="J147" s="133"/>
+      <c r="H147" s="134"/>
+      <c r="I147" s="134"/>
+      <c r="J147" s="134"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="96" t="s">
@@ -13099,7 +13137,7 @@
         <v>23</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="J148" s="4" t="s">
         <v>324</v>
@@ -13382,12 +13420,12 @@
       <c r="E161" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G161" s="133" t="s">
+      <c r="G161" s="134" t="s">
         <v>339</v>
       </c>
-      <c r="H161" s="133"/>
-      <c r="I161" s="133"/>
-      <c r="J161" s="133"/>
+      <c r="H161" s="134"/>
+      <c r="I161" s="134"/>
+      <c r="J161" s="134"/>
     </row>
     <row r="162" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A162" s="27" t="s">
@@ -13405,12 +13443,12 @@
       <c r="E162" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G162" s="133" t="s">
+      <c r="G162" s="134" t="s">
         <v>340</v>
       </c>
-      <c r="H162" s="133"/>
-      <c r="I162" s="133"/>
-      <c r="J162" s="133"/>
+      <c r="H162" s="134"/>
+      <c r="I162" s="134"/>
+      <c r="J162" s="134"/>
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="96" t="s">
@@ -13477,12 +13515,12 @@
       <c r="E166" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G166" s="133" t="s">
+      <c r="G166" s="134" t="s">
         <v>326</v>
       </c>
-      <c r="H166" s="133"/>
-      <c r="I166" s="133"/>
-      <c r="J166" s="133"/>
+      <c r="H166" s="134"/>
+      <c r="I166" s="134"/>
+      <c r="J166" s="134"/>
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="96" t="s">
@@ -13585,7 +13623,7 @@
         <v>21</v>
       </c>
       <c r="J170" s="4" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.25">
@@ -13612,12 +13650,12 @@
       <c r="E172" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G172" s="133" t="s">
+      <c r="G172" s="134" t="s">
         <v>274</v>
       </c>
-      <c r="H172" s="133"/>
-      <c r="I172" s="133"/>
-      <c r="J172" s="133"/>
+      <c r="H172" s="134"/>
+      <c r="I172" s="134"/>
+      <c r="J172" s="134"/>
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="96" t="s">
@@ -13739,12 +13777,12 @@
       <c r="E178" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G178" s="133" t="s">
+      <c r="G178" s="134" t="s">
         <v>320</v>
       </c>
-      <c r="H178" s="133"/>
-      <c r="I178" s="133"/>
-      <c r="J178" s="133"/>
+      <c r="H178" s="134"/>
+      <c r="I178" s="134"/>
+      <c r="J178" s="134"/>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="96" t="s">
@@ -13818,12 +13856,12 @@
       <c r="E182" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G182" s="133" t="s">
+      <c r="G182" s="134" t="s">
         <v>341</v>
       </c>
-      <c r="H182" s="133"/>
-      <c r="I182" s="133"/>
-      <c r="J182" s="133"/>
+      <c r="H182" s="134"/>
+      <c r="I182" s="134"/>
+      <c r="J182" s="134"/>
     </row>
     <row r="183" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A183" s="27" t="s">
@@ -13841,12 +13879,12 @@
       <c r="E183" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G183" s="133" t="s">
+      <c r="G183" s="134" t="s">
         <v>342</v>
       </c>
-      <c r="H183" s="133"/>
-      <c r="I183" s="133"/>
-      <c r="J183" s="133"/>
+      <c r="H183" s="134"/>
+      <c r="I183" s="134"/>
+      <c r="J183" s="134"/>
     </row>
     <row r="184" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A184" s="27" t="s">
@@ -13864,12 +13902,12 @@
       <c r="E184" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G184" s="133" t="s">
+      <c r="G184" s="134" t="s">
         <v>349</v>
       </c>
-      <c r="H184" s="133"/>
-      <c r="I184" s="133"/>
-      <c r="J184" s="133"/>
+      <c r="H184" s="134"/>
+      <c r="I184" s="134"/>
+      <c r="J184" s="134"/>
     </row>
     <row r="185" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A185" s="27" t="s">
@@ -13887,12 +13925,12 @@
       <c r="E185" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G185" s="133" t="s">
+      <c r="G185" s="134" t="s">
         <v>348</v>
       </c>
-      <c r="H185" s="133"/>
-      <c r="I185" s="133"/>
-      <c r="J185" s="133"/>
+      <c r="H185" s="134"/>
+      <c r="I185" s="134"/>
+      <c r="J185" s="134"/>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="96" t="s">
@@ -13959,12 +13997,12 @@
       <c r="E189" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G189" s="133" t="s">
+      <c r="G189" s="134" t="s">
         <v>280</v>
       </c>
-      <c r="H189" s="133"/>
-      <c r="I189" s="133"/>
-      <c r="J189" s="133"/>
+      <c r="H189" s="134"/>
+      <c r="I189" s="134"/>
+      <c r="J189" s="134"/>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="96" t="s">
@@ -14112,12 +14150,12 @@
       <c r="E196" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G196" s="133" t="s">
+      <c r="G196" s="134" t="s">
         <v>281</v>
       </c>
-      <c r="H196" s="133"/>
-      <c r="I196" s="133"/>
-      <c r="J196" s="133"/>
+      <c r="H196" s="134"/>
+      <c r="I196" s="134"/>
+      <c r="J196" s="134"/>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="96" t="s">
@@ -14142,7 +14180,7 @@
         <v>83</v>
       </c>
       <c r="J197" s="4" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.25">
@@ -14168,7 +14206,7 @@
         <v>84</v>
       </c>
       <c r="J198" s="4" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.25">
@@ -14194,7 +14232,7 @@
         <v>85</v>
       </c>
       <c r="J199" s="4" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.25">
@@ -14220,7 +14258,7 @@
         <v>86</v>
       </c>
       <c r="J200" s="4" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.25">
@@ -14246,15 +14284,15 @@
         <v>87</v>
       </c>
       <c r="J201" s="4" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="202" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
       <c r="I202" s="119" t="s">
+        <v>913</v>
+      </c>
+      <c r="J202" s="4" t="s">
         <v>914</v>
-      </c>
-      <c r="J202" s="4" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.25">
@@ -14276,12 +14314,12 @@
       <c r="E204" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G204" s="133" t="s">
+      <c r="G204" s="134" t="s">
         <v>563</v>
       </c>
-      <c r="H204" s="133"/>
-      <c r="I204" s="133"/>
-      <c r="J204" s="133"/>
+      <c r="H204" s="134"/>
+      <c r="I204" s="134"/>
+      <c r="J204" s="134"/>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="96" t="s">
@@ -14359,12 +14397,12 @@
       <c r="E208" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G208" s="133" t="s">
+      <c r="G208" s="134" t="s">
         <v>563</v>
       </c>
-      <c r="H208" s="133"/>
-      <c r="I208" s="133"/>
-      <c r="J208" s="133"/>
+      <c r="H208" s="134"/>
+      <c r="I208" s="134"/>
+      <c r="J208" s="134"/>
     </row>
     <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="96" t="s">
@@ -14442,12 +14480,12 @@
       <c r="E212" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G212" s="133" t="s">
+      <c r="G212" s="134" t="s">
         <v>607</v>
       </c>
-      <c r="H212" s="133"/>
-      <c r="I212" s="133"/>
-      <c r="J212" s="133"/>
+      <c r="H212" s="134"/>
+      <c r="I212" s="134"/>
+      <c r="J212" s="134"/>
     </row>
     <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="96" t="s">
@@ -14525,12 +14563,12 @@
       <c r="E216" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G216" s="133" t="s">
-        <v>754</v>
-      </c>
-      <c r="H216" s="133"/>
-      <c r="I216" s="133"/>
-      <c r="J216" s="133"/>
+      <c r="G216" s="134" t="s">
+        <v>753</v>
+      </c>
+      <c r="H216" s="134"/>
+      <c r="I216" s="134"/>
+      <c r="J216" s="134"/>
     </row>
     <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="96" t="s">
@@ -14608,12 +14646,12 @@
       <c r="E220" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G220" s="133" t="s">
-        <v>754</v>
-      </c>
-      <c r="H220" s="133"/>
-      <c r="I220" s="133"/>
-      <c r="J220" s="133"/>
+      <c r="G220" s="134" t="s">
+        <v>753</v>
+      </c>
+      <c r="H220" s="134"/>
+      <c r="I220" s="134"/>
+      <c r="J220" s="134"/>
     </row>
     <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="96" t="s">
@@ -14761,12 +14799,12 @@
       <c r="E227" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G227" s="133" t="s">
-        <v>759</v>
-      </c>
-      <c r="H227" s="133"/>
-      <c r="I227" s="133"/>
-      <c r="J227" s="133"/>
+      <c r="G227" s="134" t="s">
+        <v>758</v>
+      </c>
+      <c r="H227" s="134"/>
+      <c r="I227" s="134"/>
+      <c r="J227" s="134"/>
     </row>
     <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="96" t="s">
@@ -14788,10 +14826,10 @@
         <v>23</v>
       </c>
       <c r="I228" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="J228" s="4" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="229" spans="1:10" x14ac:dyDescent="0.25">
@@ -14814,10 +14852,10 @@
         <v>23</v>
       </c>
       <c r="I229" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="J229" s="4" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="230" spans="1:10" x14ac:dyDescent="0.25">
@@ -14843,7 +14881,7 @@
         <v>621</v>
       </c>
       <c r="J230" s="4" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="231" spans="1:10" x14ac:dyDescent="0.25">
@@ -14866,10 +14904,10 @@
         <v>23</v>
       </c>
       <c r="I231" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="J231" s="4" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="232" spans="1:10" x14ac:dyDescent="0.25">
@@ -14892,10 +14930,10 @@
         <v>23</v>
       </c>
       <c r="I232" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="J232" s="4" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="233" spans="1:10" x14ac:dyDescent="0.25">
@@ -14905,10 +14943,10 @@
       <c r="D233" s="97"/>
       <c r="E233" s="97"/>
       <c r="I233" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="J233" s="4" t="s">
         <v>756</v>
-      </c>
-      <c r="J233" s="4" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="234" spans="1:10" x14ac:dyDescent="0.25">
@@ -14935,12 +14973,12 @@
       <c r="E235" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G235" s="133" t="s">
-        <v>760</v>
-      </c>
-      <c r="H235" s="133"/>
-      <c r="I235" s="133"/>
-      <c r="J235" s="133"/>
+      <c r="G235" s="134" t="s">
+        <v>759</v>
+      </c>
+      <c r="H235" s="134"/>
+      <c r="I235" s="134"/>
+      <c r="J235" s="134"/>
     </row>
     <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="96" t="s">
@@ -14962,10 +15000,10 @@
         <v>23</v>
       </c>
       <c r="I236" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="J236" s="4" t="s">
         <v>772</v>
-      </c>
-      <c r="J236" s="4" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="237" spans="1:10" x14ac:dyDescent="0.25">
@@ -14988,10 +15026,10 @@
         <v>23</v>
       </c>
       <c r="I237" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="J237" s="4" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="238" spans="1:10" x14ac:dyDescent="0.25">
@@ -15014,10 +15052,10 @@
         <v>23</v>
       </c>
       <c r="I238" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="J238" s="4" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="239" spans="1:10" x14ac:dyDescent="0.25">
@@ -15040,10 +15078,10 @@
         <v>23</v>
       </c>
       <c r="I239" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="J239" s="4" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="240" spans="1:10" x14ac:dyDescent="0.25">
@@ -15066,10 +15104,10 @@
         <v>23</v>
       </c>
       <c r="I240" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="J240" s="4" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.25">
@@ -15092,10 +15130,10 @@
         <v>23</v>
       </c>
       <c r="I241" s="1" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="J241" s="4" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.25">
@@ -15105,10 +15143,10 @@
       <c r="D242" s="97"/>
       <c r="E242" s="97"/>
       <c r="I242" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="J242" s="4" t="s">
         <v>756</v>
-      </c>
-      <c r="J242" s="4" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.25">
@@ -15135,12 +15173,12 @@
       <c r="E244" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G244" s="133" t="s">
-        <v>788</v>
-      </c>
-      <c r="H244" s="133"/>
-      <c r="I244" s="133"/>
-      <c r="J244" s="133"/>
+      <c r="G244" s="134" t="s">
+        <v>787</v>
+      </c>
+      <c r="H244" s="134"/>
+      <c r="I244" s="134"/>
+      <c r="J244" s="134"/>
     </row>
     <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="96" t="s">
@@ -15162,10 +15200,10 @@
         <v>23</v>
       </c>
       <c r="I245" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="J245" s="4" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.25">
@@ -15188,10 +15226,10 @@
         <v>23</v>
       </c>
       <c r="I246" s="1" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="J246" s="4" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="247" spans="1:10" x14ac:dyDescent="0.25">
@@ -15214,10 +15252,10 @@
         <v>23</v>
       </c>
       <c r="I247" s="1" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="J247" s="4" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.25">
@@ -15243,7 +15281,7 @@
         <v>619</v>
       </c>
       <c r="J248" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="249" spans="1:10" x14ac:dyDescent="0.25">
@@ -15266,10 +15304,10 @@
         <v>23</v>
       </c>
       <c r="I249" s="1" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="J249" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="250" spans="1:10" x14ac:dyDescent="0.25">
@@ -15292,10 +15330,10 @@
         <v>23</v>
       </c>
       <c r="I250" s="1" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="J250" s="4" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="251" spans="1:10" x14ac:dyDescent="0.25">
@@ -15322,12 +15360,12 @@
       <c r="E252" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G252" s="133" t="s">
-        <v>787</v>
-      </c>
-      <c r="H252" s="133"/>
-      <c r="I252" s="133"/>
-      <c r="J252" s="133"/>
+      <c r="G252" s="134" t="s">
+        <v>786</v>
+      </c>
+      <c r="H252" s="134"/>
+      <c r="I252" s="134"/>
+      <c r="J252" s="134"/>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="96" t="s">
@@ -15352,7 +15390,7 @@
         <v>618</v>
       </c>
       <c r="J253" s="4" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.25">
@@ -15378,7 +15416,7 @@
         <v>620</v>
       </c>
       <c r="J254" s="4" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.25">
@@ -15401,10 +15439,10 @@
         <v>23</v>
       </c>
       <c r="I255" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="J255" s="4" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
@@ -15427,10 +15465,10 @@
         <v>23</v>
       </c>
       <c r="I256" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="J256" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
@@ -15457,12 +15495,12 @@
       <c r="E258" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G258" s="133" t="s">
-        <v>813</v>
-      </c>
-      <c r="H258" s="133"/>
-      <c r="I258" s="133"/>
-      <c r="J258" s="133"/>
+      <c r="G258" s="134" t="s">
+        <v>812</v>
+      </c>
+      <c r="H258" s="134"/>
+      <c r="I258" s="134"/>
+      <c r="J258" s="134"/>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="96" t="s">
@@ -15484,10 +15522,10 @@
         <v>23</v>
       </c>
       <c r="I259" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="J259" s="4" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
@@ -15513,7 +15551,7 @@
         <v>77</v>
       </c>
       <c r="J260" s="4" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
@@ -15533,10 +15571,10 @@
         <v>50</v>
       </c>
       <c r="I261" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="J261" s="4" t="s">
         <v>756</v>
-      </c>
-      <c r="J261" s="4" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
@@ -15563,12 +15601,12 @@
       <c r="E263" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G263" s="133" t="s">
-        <v>816</v>
-      </c>
-      <c r="H263" s="133"/>
-      <c r="I263" s="133"/>
-      <c r="J263" s="133"/>
+      <c r="G263" s="134" t="s">
+        <v>815</v>
+      </c>
+      <c r="H263" s="134"/>
+      <c r="I263" s="134"/>
+      <c r="J263" s="134"/>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="96" t="s">
@@ -15593,7 +15631,7 @@
         <v>618</v>
       </c>
       <c r="J264" s="4" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="265" spans="1:10" x14ac:dyDescent="0.25">
@@ -15619,7 +15657,7 @@
         <v>619</v>
       </c>
       <c r="J265" s="4" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.25">
@@ -15639,10 +15677,10 @@
         <v>50</v>
       </c>
       <c r="I266" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="J266" s="4" t="s">
         <v>756</v>
-      </c>
-      <c r="J266" s="4" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
@@ -15669,12 +15707,12 @@
       <c r="E268" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G268" s="133" t="s">
+      <c r="G268" s="134" t="s">
         <v>282</v>
       </c>
-      <c r="H268" s="133"/>
-      <c r="I268" s="133"/>
-      <c r="J268" s="133"/>
+      <c r="H268" s="134"/>
+      <c r="I268" s="134"/>
+      <c r="J268" s="134"/>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="97" t="s">
@@ -15986,10 +16024,10 @@
         <v>23</v>
       </c>
       <c r="I280" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="J280" s="4" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="281" spans="1:10" x14ac:dyDescent="0.25">
@@ -16012,10 +16050,10 @@
         <v>23</v>
       </c>
       <c r="I281" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="J281" s="4" t="s">
         <v>770</v>
-      </c>
-      <c r="J281" s="4" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.25">
@@ -16038,10 +16076,10 @@
         <v>23</v>
       </c>
       <c r="I282" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="J282" s="4" t="s">
         <v>739</v>
-      </c>
-      <c r="J282" s="4" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
@@ -16064,10 +16102,10 @@
         <v>23</v>
       </c>
       <c r="I283" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="J283" s="4" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="284" spans="1:10" x14ac:dyDescent="0.25">
@@ -16090,10 +16128,10 @@
         <v>23</v>
       </c>
       <c r="I284" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="J284" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="285" spans="1:10" x14ac:dyDescent="0.25">
@@ -16116,10 +16154,10 @@
         <v>23</v>
       </c>
       <c r="I285" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="J285" s="4" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="286" spans="1:10" x14ac:dyDescent="0.25">
@@ -16142,10 +16180,10 @@
         <v>23</v>
       </c>
       <c r="I286" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="J286" s="4" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="287" spans="1:10" x14ac:dyDescent="0.25">
@@ -16168,10 +16206,10 @@
         <v>23</v>
       </c>
       <c r="I287" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="J287" s="4" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="288" spans="1:10" x14ac:dyDescent="0.25">
@@ -16194,10 +16232,10 @@
         <v>23</v>
       </c>
       <c r="I288" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="J288" s="4" t="s">
         <v>751</v>
-      </c>
-      <c r="J288" s="4" t="s">
-        <v>752</v>
       </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
@@ -16220,10 +16258,10 @@
         <v>23</v>
       </c>
       <c r="I289" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="J289" s="4" t="s">
         <v>828</v>
-      </c>
-      <c r="J289" s="4" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="291" spans="1:10" ht="15.75" x14ac:dyDescent="0.3">
@@ -16242,12 +16280,12 @@
       <c r="E291" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="G291" s="133" t="s">
+      <c r="G291" s="134" t="s">
         <v>283</v>
       </c>
-      <c r="H291" s="133"/>
-      <c r="I291" s="133"/>
-      <c r="J291" s="133"/>
+      <c r="H291" s="134"/>
+      <c r="I291" s="134"/>
+      <c r="J291" s="134"/>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="97" t="s">
@@ -16269,7 +16307,7 @@
         <v>23</v>
       </c>
       <c r="I292" s="117" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
@@ -16396,6 +16434,59 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="G166:J166"/>
+    <mergeCell ref="G161:J161"/>
+    <mergeCell ref="G162:J162"/>
+    <mergeCell ref="G208:J208"/>
+    <mergeCell ref="G147:J147"/>
+    <mergeCell ref="G291:J291"/>
+    <mergeCell ref="G172:J172"/>
+    <mergeCell ref="G185:J185"/>
+    <mergeCell ref="G189:J189"/>
+    <mergeCell ref="G196:J196"/>
+    <mergeCell ref="G268:J268"/>
+    <mergeCell ref="G204:J204"/>
+    <mergeCell ref="G212:J212"/>
+    <mergeCell ref="G252:J252"/>
+    <mergeCell ref="G227:J227"/>
+    <mergeCell ref="G235:J235"/>
+    <mergeCell ref="G244:J244"/>
+    <mergeCell ref="G258:J258"/>
+    <mergeCell ref="G263:J263"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="G49:J49"/>
+    <mergeCell ref="G50:J50"/>
+    <mergeCell ref="G70:J70"/>
+    <mergeCell ref="G89:J89"/>
+    <mergeCell ref="G92:J92"/>
+    <mergeCell ref="G93:J93"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="G63:J63"/>
+    <mergeCell ref="G64:J64"/>
+    <mergeCell ref="G65:J65"/>
+    <mergeCell ref="G66:J66"/>
+    <mergeCell ref="G84:J84"/>
     <mergeCell ref="A103:E103"/>
     <mergeCell ref="A97:E97"/>
     <mergeCell ref="A95:E95"/>
@@ -16412,59 +16503,6 @@
     <mergeCell ref="G183:J183"/>
     <mergeCell ref="G184:J184"/>
     <mergeCell ref="G178:J178"/>
-    <mergeCell ref="G70:J70"/>
-    <mergeCell ref="G89:J89"/>
-    <mergeCell ref="G92:J92"/>
-    <mergeCell ref="G93:J93"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="G63:J63"/>
-    <mergeCell ref="G64:J64"/>
-    <mergeCell ref="G65:J65"/>
-    <mergeCell ref="G66:J66"/>
-    <mergeCell ref="G84:J84"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="G46:J46"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="G48:J48"/>
-    <mergeCell ref="G49:J49"/>
-    <mergeCell ref="G50:J50"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="G291:J291"/>
-    <mergeCell ref="G172:J172"/>
-    <mergeCell ref="G185:J185"/>
-    <mergeCell ref="G189:J189"/>
-    <mergeCell ref="G196:J196"/>
-    <mergeCell ref="G268:J268"/>
-    <mergeCell ref="G204:J204"/>
-    <mergeCell ref="G212:J212"/>
-    <mergeCell ref="G252:J252"/>
-    <mergeCell ref="G227:J227"/>
-    <mergeCell ref="G235:J235"/>
-    <mergeCell ref="G244:J244"/>
-    <mergeCell ref="G258:J258"/>
-    <mergeCell ref="G263:J263"/>
-    <mergeCell ref="G166:J166"/>
-    <mergeCell ref="G161:J161"/>
-    <mergeCell ref="G162:J162"/>
-    <mergeCell ref="G208:J208"/>
-    <mergeCell ref="G147:J147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" r:id="rId1"/>
@@ -16506,7 +16544,7 @@
         <v>381</v>
       </c>
       <c r="B1" s="137" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C1" s="137"/>
       <c r="D1" s="137"/>
@@ -16519,16 +16557,16 @@
         <v>622</v>
       </c>
       <c r="B2" s="91" t="s">
+        <v>839</v>
+      </c>
+      <c r="C2" s="91" t="s">
         <v>840</v>
       </c>
-      <c r="C2" s="91" t="s">
-        <v>841</v>
-      </c>
       <c r="D2" s="91" t="s">
+        <v>886</v>
+      </c>
+      <c r="E2" s="91" t="s">
         <v>887</v>
-      </c>
-      <c r="E2" s="91" t="s">
-        <v>888</v>
       </c>
       <c r="F2" s="91" t="s">
         <v>363</v>
@@ -16551,25 +16589,25 @@
       <c r="F3" s="105"/>
       <c r="G3" s="105"/>
       <c r="I3" s="105" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="92" t="s">
+        <v>842</v>
+      </c>
+      <c r="B4" s="92" t="s">
         <v>843</v>
-      </c>
-      <c r="B4" s="92" t="s">
-        <v>844</v>
       </c>
       <c r="C4" s="92"/>
       <c r="D4" s="92" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E4" s="92" t="s">
         <v>613</v>
       </c>
       <c r="F4" s="92" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G4" s="92"/>
       <c r="I4" s="106" t="str">
@@ -16583,20 +16621,20 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="92" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="B5" s="92" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C5" s="92"/>
       <c r="D5" s="92" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E5" s="92" t="s">
         <v>613</v>
       </c>
       <c r="F5" s="92" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G5" s="92"/>
       <c r="I5" s="106" t="str">
@@ -16610,20 +16648,20 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="92" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B6" s="92" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C6" s="92"/>
       <c r="D6" s="92" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E6" s="92" t="s">
         <v>613</v>
       </c>
       <c r="F6" s="92" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G6" s="92"/>
       <c r="I6" s="106" t="str">
@@ -16637,20 +16675,20 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="92" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B7" s="92" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C7" s="92"/>
       <c r="D7" s="92" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E7" s="92" t="s">
         <v>613</v>
       </c>
       <c r="F7" s="92" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G7" s="92"/>
       <c r="I7" s="106" t="str">
@@ -16664,10 +16702,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="92" t="s">
+        <v>848</v>
+      </c>
+      <c r="B8" s="92" t="s">
         <v>849</v>
-      </c>
-      <c r="B8" s="92" t="s">
-        <v>850</v>
       </c>
       <c r="C8" s="92"/>
       <c r="D8" s="92"/>
@@ -16675,7 +16713,7 @@
         <v>613</v>
       </c>
       <c r="F8" s="92" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G8" s="92"/>
       <c r="I8" s="106" t="str">
@@ -16689,10 +16727,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="92" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B9" s="92" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C9" s="92"/>
       <c r="D9" s="92"/>
@@ -16700,7 +16738,7 @@
         <v>613</v>
       </c>
       <c r="G9" s="92" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="I9" s="106" t="str">
         <f t="shared" si="0"/>
@@ -16713,10 +16751,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="92" t="s">
+        <v>850</v>
+      </c>
+      <c r="B10" s="92" t="s">
         <v>851</v>
-      </c>
-      <c r="B10" s="92" t="s">
-        <v>852</v>
       </c>
       <c r="C10" s="92"/>
       <c r="D10" s="92"/>
@@ -16724,7 +16762,7 @@
         <v>613</v>
       </c>
       <c r="G10" s="92" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="I10" s="106" t="str">
         <f t="shared" si="0"/>
@@ -16737,10 +16775,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="92" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C11" s="92"/>
       <c r="D11" s="92"/>
@@ -16748,7 +16786,7 @@
         <v>613</v>
       </c>
       <c r="G11" s="92" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="I11" s="106" t="str">
         <f t="shared" si="0"/>
@@ -16761,10 +16799,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="92" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C12" s="92"/>
       <c r="D12" s="92"/>
@@ -16772,7 +16810,7 @@
         <v>613</v>
       </c>
       <c r="G12" s="92" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="I12" s="106" t="str">
         <f>IF(ISBLANK(B12), "", CONCATENATE("&lt;risk-metric name='", B12,"'",IF(ISBLANK(D12), "", CONCATENATE(" class='", D12, "'")), " system='", E12, IF(ISBLANK(F12), " /&gt;", "'&gt;value&lt;/risk-metric&gt;")))</f>
@@ -16785,10 +16823,10 @@
     </row>
     <row r="13" spans="1:13" s="110" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="92" t="s">
+        <v>878</v>
+      </c>
+      <c r="B13" s="92" t="s">
         <v>879</v>
-      </c>
-      <c r="B13" s="92" t="s">
-        <v>880</v>
       </c>
       <c r="C13" s="92"/>
       <c r="D13" s="92"/>
@@ -16796,10 +16834,10 @@
         <v>613</v>
       </c>
       <c r="F13" s="110" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G13" s="92" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="I13" s="106" t="str">
         <f>IF(ISBLANK(B13), "", CONCATENATE("&lt;risk-metric name='", B13,"'",IF(ISBLANK(D13), "", CONCATENATE(" class='", D13, "'")), " system='", E13, IF(ISBLANK(F13), " /&gt;", "'&gt;value&lt;/risk-metric&gt;")))</f>
@@ -16822,7 +16860,7 @@
     </row>
     <row r="15" spans="1:13" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="105" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B15" s="105"/>
       <c r="C15" s="105"/>
@@ -16831,26 +16869,26 @@
       <c r="F15" s="105"/>
       <c r="G15" s="105"/>
       <c r="I15" s="105" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="92" t="s">
+        <v>870</v>
+      </c>
+      <c r="B16" s="92" t="s">
         <v>871</v>
-      </c>
-      <c r="B16" s="92" t="s">
-        <v>872</v>
       </c>
       <c r="C16" s="92"/>
       <c r="D16" s="92"/>
       <c r="E16" s="92" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F16" s="92" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="G16" s="138" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I16" s="106" t="str">
         <f t="shared" ref="I16:I21" si="1">IF(ISBLANK(B16), "", CONCATENATE("&lt;risk-metric name='", B16,"'",IF(ISBLANK(D16), "", CONCATENATE(" class='", D16, "'")), " system='", E16, IF(ISBLANK(F16), " /&gt;", "'&gt;value&lt;/risk-metric&gt;")))</f>
@@ -16863,18 +16901,18 @@
     </row>
     <row r="17" spans="1:13" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="92" t="s">
+        <v>864</v>
+      </c>
+      <c r="B17" s="92" t="s">
         <v>865</v>
-      </c>
-      <c r="B17" s="92" t="s">
-        <v>866</v>
       </c>
       <c r="C17" s="92"/>
       <c r="D17" s="92"/>
       <c r="E17" s="92" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="F17" s="92" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="G17" s="138"/>
       <c r="I17" s="106" t="str">
@@ -16888,18 +16926,18 @@
     </row>
     <row r="18" spans="1:13" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="B18" s="92" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C18" s="92"/>
       <c r="D18" s="92"/>
       <c r="E18" s="92" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F18" s="92" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="G18" s="138"/>
       <c r="I18" s="106" t="str">
@@ -16913,18 +16951,18 @@
     </row>
     <row r="19" spans="1:13" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="92" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B19" s="92" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C19" s="92"/>
       <c r="D19" s="92"/>
       <c r="E19" s="92" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F19" s="92" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G19" s="138"/>
       <c r="I19" s="106" t="str">
@@ -16938,18 +16976,18 @@
     </row>
     <row r="20" spans="1:13" s="108" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="92" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B20" s="92" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
       <c r="E20" s="92" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F20" s="92" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G20" s="138"/>
       <c r="I20" s="106" t="str">
@@ -16991,7 +17029,7 @@
       <c r="F22" s="136"/>
       <c r="G22" s="136"/>
       <c r="I22" s="105" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -17379,7 +17417,7 @@
       <c r="F41" s="136"/>
       <c r="G41" s="136"/>
       <c r="I41" s="105" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -17953,7 +17991,7 @@
       <c r="F68" s="136"/>
       <c r="G68" s="136"/>
       <c r="I68" s="105" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -18562,13 +18600,13 @@
       <c r="I1" s="84"/>
     </row>
     <row r="2" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="128" t="s">
+      <c r="A2" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="128"/>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
+      <c r="B2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
       <c r="G2" s="54" t="s">
         <v>406</v>
       </c>
@@ -18579,10 +18617,10 @@
       <c r="J2" t="s">
         <v>443</v>
       </c>
-      <c r="K2" s="129" t="s">
+      <c r="K2" s="128" t="s">
         <v>363</v>
       </c>
-      <c r="L2" s="129" t="s">
+      <c r="L2" s="128" t="s">
         <v>303</v>
       </c>
     </row>
@@ -18614,8 +18652,8 @@
       <c r="J3" s="19" t="s">
         <v>290</v>
       </c>
-      <c r="K3" s="129"/>
-      <c r="L3" s="129"/>
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
       <c r="M3" s="43" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
SAP and POAM templates updated. SAR template and all three guides still WIP
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\fedramp-automation-new\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D2610A-0DCD-473E-9A2B-C9D095DE79E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF89DD49-0D6E-4AB0-AAB5-2D58184AE673}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24540" yWindow="2025" windowWidth="21135" windowHeight="17670" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22980" yWindow="3825" windowWidth="21090" windowHeight="12135" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATION" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="137">
   <si>
     <t>SSP</t>
   </si>
@@ -517,14 +517,20 @@
     <t>See the FedRAMP Extensions file here:</t>
   </si>
   <si>
-    <t>https://github.com/GSA/fedramp-automation/tree/master/src/resources/xml</t>
+    <t>HTML Version (Human Readable)</t>
+  </si>
+  <si>
+    <t>XML Version (Machine Readable)</t>
+  </si>
+  <si>
+    <t>JSON Version (Machine Readable)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,6 +655,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -759,7 +772,7 @@
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -823,6 +836,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -832,16 +848,17 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="AUTHOR-NOTE" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1191,10 +1208,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,10 +1225,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="25"/>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
       <c r="H1" s="12" t="s">
         <v>64</v>
       </c>
@@ -1225,22 +1242,35 @@
       <c r="B3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="26"/>
+      <c r="B4" s="27"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
     </row>
     <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="25" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="32" t="s">
         <v>134</v>
       </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1248,11 +1278,13 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{F6DF431D-1A7B-4AE2-B18D-075140E00CDA}"/>
+    <hyperlink ref="A6" r:id="rId1" display="https://github.com/GSA/fedramp-automation/raw/master/resources/xml/FedRAMP_extensions.xml" xr:uid="{C11280DE-CD0B-4C2C-BFDE-718C5627D230}"/>
+    <hyperlink ref="A7" r:id="rId2" display="https://github.com/GSA/fedramp-automation/raw/master/resources/json/FedRAMP_extensions.json" xr:uid="{BDCC9178-CB00-47B5-A553-2F5BCE8CAD8A}"/>
+    <hyperlink ref="A8" r:id="rId3" display="https://github.com/GSA/fedramp-automation/raw/master/documents/FedRAMP_extensions.html" xr:uid="{3B6B626F-6AA8-49C6-8622-C5E437C785C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1294,13 +1326,13 @@
       <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
       <c r="G2" s="18" t="s">
         <v>71</v>
       </c>
@@ -1311,10 +1343,10 @@
       <c r="J2" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="28" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1346,8 +1378,8 @@
       <c r="J3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="10" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Updated guides and templates to align with OSCAL RC-2
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\fedramp-automation-new\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF89DD49-0D6E-4AB0-AAB5-2D58184AE673}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1193B436-BF2A-4D20-BB4A-7BD8D5CF185B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22980" yWindow="3825" windowWidth="21090" windowHeight="12135" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="138">
   <si>
     <t>SSP</t>
   </si>
@@ -524,6 +524,9 @@
   </si>
   <si>
     <t>JSON Version (Machine Readable)</t>
+  </si>
+  <si>
+    <t>PDF Version (Human Readable)</t>
   </si>
 </sst>
 </file>
@@ -839,6 +842,10 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -854,11 +861,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="AUTHOR-NOTE" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1211,7 +1214,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1225,10 +1228,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="26"/>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="H1" s="12" t="s">
         <v>64</v>
       </c>
@@ -1242,10 +1245,10 @@
       <c r="B3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
     </row>
@@ -1255,22 +1258,24 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="26" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="27" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="27" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="33"/>
+      <c r="A9" s="33" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1281,10 +1286,11 @@
     <hyperlink ref="A6" r:id="rId1" display="https://github.com/GSA/fedramp-automation/raw/master/resources/xml/FedRAMP_extensions.xml" xr:uid="{C11280DE-CD0B-4C2C-BFDE-718C5627D230}"/>
     <hyperlink ref="A7" r:id="rId2" display="https://github.com/GSA/fedramp-automation/raw/master/resources/json/FedRAMP_extensions.json" xr:uid="{BDCC9178-CB00-47B5-A553-2F5BCE8CAD8A}"/>
     <hyperlink ref="A8" r:id="rId3" display="https://github.com/GSA/fedramp-automation/raw/master/documents/FedRAMP_extensions.html" xr:uid="{3B6B626F-6AA8-49C6-8622-C5E437C785C4}"/>
+    <hyperlink ref="A9" r:id="rId4" xr:uid="{AA444CB8-FAC5-435F-9776-A0F9777419BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -1326,27 +1332,27 @@
       <c r="I1" s="24"/>
     </row>
     <row r="2" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
       <c r="G2" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="I2" s="29"/>
+      <c r="I2" s="31"/>
       <c r="J2" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="30" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1378,8 +1384,8 @@
       <c r="J3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
       <c r="M3" s="10" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Update outdated Excel registry links.
</commit_message>
<xml_diff>
--- a/documents/FedRAMP_OSCAL_Registry.xlsx
+++ b/documents/FedRAMP_OSCAL_Registry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitRepos\fedramp-automation-new\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astein/Code/fedramp-automation/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1193B436-BF2A-4D20-BB4A-7BD8D5CF185B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E433CEF-9029-0D43-B4DE-FD821ED3CECD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22980" yWindow="3825" windowWidth="21090" windowHeight="12135" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12500" yWindow="3820" windowWidth="21100" windowHeight="12140" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORMATION" sheetId="6" r:id="rId1"/>
@@ -536,6 +536,13 @@
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -658,13 +665,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -764,23 +764,23 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -789,79 +789,78 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="3">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="3">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="AUTHOR-NOTE" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1217,63 +1216,63 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="104" style="12" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" style="12" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="62.83203125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="12" customWidth="1"/>
+    <col min="4" max="4" width="22.83203125" style="12" customWidth="1"/>
     <col min="5" max="5" width="19" style="12" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="12"/>
+    <col min="6" max="16384" width="8.6640625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
       <c r="H1" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="14"/>
     </row>
-    <row r="3" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="28"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="26" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="26" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="26" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1283,9 +1282,9 @@
     <mergeCell ref="A4:B4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" display="https://github.com/GSA/fedramp-automation/raw/master/resources/xml/FedRAMP_extensions.xml" xr:uid="{C11280DE-CD0B-4C2C-BFDE-718C5627D230}"/>
-    <hyperlink ref="A7" r:id="rId2" display="https://github.com/GSA/fedramp-automation/raw/master/resources/json/FedRAMP_extensions.json" xr:uid="{BDCC9178-CB00-47B5-A553-2F5BCE8CAD8A}"/>
-    <hyperlink ref="A8" r:id="rId3" display="https://github.com/GSA/fedramp-automation/raw/master/documents/FedRAMP_extensions.html" xr:uid="{3B6B626F-6AA8-49C6-8622-C5E437C785C4}"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{C11280DE-CD0B-4C2C-BFDE-718C5627D230}"/>
+    <hyperlink ref="A7" r:id="rId2" xr:uid="{BDCC9178-CB00-47B5-A553-2F5BCE8CAD8A}"/>
+    <hyperlink ref="A8" r:id="rId3" xr:uid="{3B6B626F-6AA8-49C6-8622-C5E437C785C4}"/>
     <hyperlink ref="A9" r:id="rId4" xr:uid="{AA444CB8-FAC5-435F-9776-A0F9777419BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1306,20 +1305,20 @@
       <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="1.140625" customWidth="1"/>
-    <col min="7" max="7" width="37.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="184.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="86.140625" style="3" customWidth="1"/>
+    <col min="1" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="1.1640625" customWidth="1"/>
+    <col min="7" max="7" width="37.5" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="31.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="184.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="4" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="86.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>65</v>
       </c>
@@ -1331,32 +1330,32 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
       <c r="G2" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="I2" s="31"/>
+      <c r="I2" s="30"/>
       <c r="J2" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="30" t="s">
+      <c r="K2" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="30" t="s">
+      <c r="L2" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>131</v>
       </c>
@@ -1384,13 +1383,13 @@
       <c r="J3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
       <c r="M3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
@@ -1467,7 +1466,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="2"/>
@@ -1478,7 +1477,7 @@
       <c r="J6" s="20"/>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="2"/>
@@ -1489,7 +1488,7 @@
       <c r="J7" s="20"/>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="2"/>
@@ -1500,7 +1499,7 @@
       <c r="J8" s="20"/>
       <c r="N8" s="4"/>
     </row>
-    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="2"/>
@@ -1511,7 +1510,7 @@
       <c r="J9" s="20"/>
       <c r="N9" s="4"/>
     </row>
-    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="2"/>
@@ -1522,7 +1521,7 @@
       <c r="J10" s="20"/>
       <c r="N10" s="4"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="2"/>
@@ -1533,7 +1532,7 @@
       <c r="J11" s="20"/>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="2"/>
@@ -1544,7 +1543,7 @@
       <c r="J12" s="20"/>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="2"/>
@@ -1555,18 +1554,18 @@
       <c r="J13" s="20"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
       <c r="J14" s="20"/>
     </row>
-    <row r="15" spans="1:14" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
       <c r="F15" s="23"/>
     </row>
-    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -1616,7 +1615,7 @@
       <c r="I17" s="21"/>
       <c r="J17" s="20"/>
     </row>
-    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>3</v>
       </c>
@@ -1648,7 +1647,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
@@ -1660,7 +1659,7 @@
       <c r="I19" s="21"/>
       <c r="J19" s="20"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>3</v>
       </c>
@@ -1692,7 +1691,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>3</v>
       </c>
@@ -1724,7 +1723,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>3</v>
       </c>
@@ -1736,7 +1735,7 @@
       <c r="I22" s="21"/>
       <c r="J22" s="20"/>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>3</v>
       </c>
@@ -1768,7 +1767,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
@@ -1800,7 +1799,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>3</v>
       </c>
@@ -1832,7 +1831,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
@@ -1867,7 +1866,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -1902,7 +1901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>3</v>
       </c>
@@ -1937,7 +1936,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -1972,7 +1971,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
@@ -2004,7 +2003,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
@@ -2013,7 +2012,7 @@
       <c r="I31" s="21"/>
       <c r="J31" s="20"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -2048,7 +2047,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>3</v>
       </c>
@@ -2083,7 +2082,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>3</v>
       </c>
@@ -2153,7 +2152,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>3</v>
       </c>
@@ -2188,7 +2187,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>3</v>
       </c>
@@ -2198,7 +2197,7 @@
       <c r="I37" s="21"/>
       <c r="J37" s="20"/>
     </row>
-    <row r="38" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>3</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>3</v>
       </c>
@@ -2268,7 +2267,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>3</v>
       </c>
@@ -2303,7 +2302,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
@@ -2312,7 +2311,7 @@
       <c r="I41" s="21"/>
       <c r="J41" s="20"/>
     </row>
-    <row r="42" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>3</v>
       </c>
@@ -2347,7 +2346,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>3</v>
       </c>
@@ -2382,7 +2381,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>3</v>
       </c>
@@ -2417,7 +2416,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>3</v>
       </c>
@@ -2452,7 +2451,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="2"/>
@@ -2462,7 +2461,7 @@
       <c r="I46" s="21"/>
       <c r="J46" s="20"/>
     </row>
-    <row r="47" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>2</v>
       </c>
@@ -2500,7 +2499,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>5</v>
       </c>
@@ -2538,7 +2537,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>5</v>
       </c>
@@ -2576,12 +2575,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H50" s="21"/>
       <c r="I50" s="21"/>
       <c r="J50" s="19"/>
     </row>
-    <row r="51" spans="1:13" s="19" customFormat="1" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22"/>
       <c r="F51" s="23"/>
     </row>

</xml_diff>